<commit_message>
Preparing the GUI to display the values read from the LPS25HB sensor
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="51">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -141,13 +141,41 @@
   </si>
   <si>
     <t xml:space="preserve">Small</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a-z,A-Z,0-9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperatura: &lt;value&gt; *C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cisnienie: &lt;value&gt; hpa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -419,127 +447,127 @@
     </border>
   </borders>
   <cellStyleXfs count="82">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyAlignment="0"/>
   </cellStyleXfs>
   <cellXfs count="26">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="81" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="81" applyFont="1" applyAlignment="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="81" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -547,91 +575,91 @@
   <cellStyles count="82">
     <cellStyle name="Accent1" xfId="81" builtinId="29"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="1"/>
-    <cellStyle name="Normal 10 2" xfId="2"/>
-    <cellStyle name="Normal 11" xfId="3"/>
-    <cellStyle name="Normal 12" xfId="4"/>
-    <cellStyle name="Normal 13" xfId="5"/>
-    <cellStyle name="Normal 14" xfId="6"/>
-    <cellStyle name="Normal 14 2" xfId="7"/>
-    <cellStyle name="Normal 15" xfId="8"/>
-    <cellStyle name="Normal 16" xfId="9"/>
-    <cellStyle name="Normal 16 2" xfId="10"/>
-    <cellStyle name="Normal 16 3" xfId="11"/>
-    <cellStyle name="Normal 17 2" xfId="12"/>
-    <cellStyle name="Normal 17 3" xfId="13"/>
-    <cellStyle name="Normal 2" xfId="14"/>
-    <cellStyle name="Normal 2 2" xfId="15"/>
-    <cellStyle name="Normal 2 3" xfId="16"/>
-    <cellStyle name="Normal 2 4" xfId="17"/>
-    <cellStyle name="Normal 2 5" xfId="18"/>
-    <cellStyle name="Normal 2 6" xfId="19"/>
-    <cellStyle name="Normal 2 7" xfId="20"/>
-    <cellStyle name="Normal 2 8" xfId="21"/>
-    <cellStyle name="Normal 2 9" xfId="22"/>
-    <cellStyle name="Normal 22" xfId="23"/>
-    <cellStyle name="Normal 22 10" xfId="24"/>
-    <cellStyle name="Normal 22 11" xfId="25"/>
-    <cellStyle name="Normal 22 12" xfId="26"/>
-    <cellStyle name="Normal 22 13" xfId="27"/>
-    <cellStyle name="Normal 22 14" xfId="28"/>
-    <cellStyle name="Normal 22 15" xfId="29"/>
-    <cellStyle name="Normal 22 16" xfId="30"/>
-    <cellStyle name="Normal 22 17" xfId="31"/>
-    <cellStyle name="Normal 22 18" xfId="32"/>
-    <cellStyle name="Normal 22 2" xfId="33"/>
-    <cellStyle name="Normal 22 3" xfId="34"/>
-    <cellStyle name="Normal 22 4" xfId="35"/>
-    <cellStyle name="Normal 22 5" xfId="36"/>
-    <cellStyle name="Normal 22 6" xfId="37"/>
-    <cellStyle name="Normal 22 7" xfId="38"/>
-    <cellStyle name="Normal 22 8" xfId="39"/>
-    <cellStyle name="Normal 22 9" xfId="40"/>
-    <cellStyle name="Normal 23 10" xfId="41"/>
-    <cellStyle name="Normal 23 11" xfId="42"/>
-    <cellStyle name="Normal 23 12" xfId="43"/>
-    <cellStyle name="Normal 23 13" xfId="44"/>
-    <cellStyle name="Normal 23 14" xfId="45"/>
-    <cellStyle name="Normal 23 15" xfId="46"/>
-    <cellStyle name="Normal 23 16" xfId="47"/>
-    <cellStyle name="Normal 23 17" xfId="48"/>
-    <cellStyle name="Normal 23 18" xfId="49"/>
-    <cellStyle name="Normal 23 2" xfId="50"/>
-    <cellStyle name="Normal 23 3" xfId="51"/>
-    <cellStyle name="Normal 23 4" xfId="52"/>
-    <cellStyle name="Normal 23 5" xfId="53"/>
-    <cellStyle name="Normal 23 6" xfId="54"/>
-    <cellStyle name="Normal 23 7" xfId="55"/>
-    <cellStyle name="Normal 23 8" xfId="56"/>
-    <cellStyle name="Normal 23 9" xfId="57"/>
-    <cellStyle name="Normal 25 10" xfId="58"/>
-    <cellStyle name="Normal 25 11" xfId="59"/>
-    <cellStyle name="Normal 25 12" xfId="60"/>
-    <cellStyle name="Normal 25 13" xfId="61"/>
-    <cellStyle name="Normal 25 14" xfId="62"/>
-    <cellStyle name="Normal 25 15" xfId="63"/>
-    <cellStyle name="Normal 25 16" xfId="64"/>
-    <cellStyle name="Normal 25 17" xfId="65"/>
-    <cellStyle name="Normal 25 2" xfId="66"/>
-    <cellStyle name="Normal 25 3" xfId="67"/>
-    <cellStyle name="Normal 25 4" xfId="68"/>
-    <cellStyle name="Normal 25 5" xfId="69"/>
-    <cellStyle name="Normal 25 6" xfId="70"/>
-    <cellStyle name="Normal 25 7" xfId="71"/>
-    <cellStyle name="Normal 25 8" xfId="72"/>
-    <cellStyle name="Normal 25 9" xfId="73"/>
-    <cellStyle name="Normal 3" xfId="74"/>
-    <cellStyle name="Normal 4" xfId="75"/>
-    <cellStyle name="Normal 5" xfId="76"/>
-    <cellStyle name="Normal 6" xfId="77"/>
-    <cellStyle name="Normal 7" xfId="78"/>
-    <cellStyle name="Normal 8" xfId="79"/>
-    <cellStyle name="Normal 9" xfId="80"/>
+    <cellStyle name="Normal 10" xfId="1" builtinId="0"/>
+    <cellStyle name="Normal 10 2" xfId="2" builtinId="0"/>
+    <cellStyle name="Normal 11" xfId="3" builtinId="0"/>
+    <cellStyle name="Normal 12" xfId="4" builtinId="0"/>
+    <cellStyle name="Normal 13" xfId="5" builtinId="0"/>
+    <cellStyle name="Normal 14" xfId="6" builtinId="0"/>
+    <cellStyle name="Normal 14 2" xfId="7" builtinId="0"/>
+    <cellStyle name="Normal 15" xfId="8" builtinId="0"/>
+    <cellStyle name="Normal 16" xfId="9" builtinId="0"/>
+    <cellStyle name="Normal 16 2" xfId="10" builtinId="0"/>
+    <cellStyle name="Normal 16 3" xfId="11" builtinId="0"/>
+    <cellStyle name="Normal 17 2" xfId="12" builtinId="0"/>
+    <cellStyle name="Normal 17 3" xfId="13" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="14" builtinId="0"/>
+    <cellStyle name="Normal 2 2" xfId="15" builtinId="0"/>
+    <cellStyle name="Normal 2 3" xfId="16" builtinId="0"/>
+    <cellStyle name="Normal 2 4" xfId="17" builtinId="0"/>
+    <cellStyle name="Normal 2 5" xfId="18" builtinId="0"/>
+    <cellStyle name="Normal 2 6" xfId="19" builtinId="0"/>
+    <cellStyle name="Normal 2 7" xfId="20" builtinId="0"/>
+    <cellStyle name="Normal 2 8" xfId="21" builtinId="0"/>
+    <cellStyle name="Normal 2 9" xfId="22" builtinId="0"/>
+    <cellStyle name="Normal 22" xfId="23" builtinId="0"/>
+    <cellStyle name="Normal 22 10" xfId="24" builtinId="0"/>
+    <cellStyle name="Normal 22 11" xfId="25" builtinId="0"/>
+    <cellStyle name="Normal 22 12" xfId="26" builtinId="0"/>
+    <cellStyle name="Normal 22 13" xfId="27" builtinId="0"/>
+    <cellStyle name="Normal 22 14" xfId="28" builtinId="0"/>
+    <cellStyle name="Normal 22 15" xfId="29" builtinId="0"/>
+    <cellStyle name="Normal 22 16" xfId="30" builtinId="0"/>
+    <cellStyle name="Normal 22 17" xfId="31" builtinId="0"/>
+    <cellStyle name="Normal 22 18" xfId="32" builtinId="0"/>
+    <cellStyle name="Normal 22 2" xfId="33" builtinId="0"/>
+    <cellStyle name="Normal 22 3" xfId="34" builtinId="0"/>
+    <cellStyle name="Normal 22 4" xfId="35" builtinId="0"/>
+    <cellStyle name="Normal 22 5" xfId="36" builtinId="0"/>
+    <cellStyle name="Normal 22 6" xfId="37" builtinId="0"/>
+    <cellStyle name="Normal 22 7" xfId="38" builtinId="0"/>
+    <cellStyle name="Normal 22 8" xfId="39" builtinId="0"/>
+    <cellStyle name="Normal 22 9" xfId="40" builtinId="0"/>
+    <cellStyle name="Normal 23 10" xfId="41" builtinId="0"/>
+    <cellStyle name="Normal 23 11" xfId="42" builtinId="0"/>
+    <cellStyle name="Normal 23 12" xfId="43" builtinId="0"/>
+    <cellStyle name="Normal 23 13" xfId="44" builtinId="0"/>
+    <cellStyle name="Normal 23 14" xfId="45" builtinId="0"/>
+    <cellStyle name="Normal 23 15" xfId="46" builtinId="0"/>
+    <cellStyle name="Normal 23 16" xfId="47" builtinId="0"/>
+    <cellStyle name="Normal 23 17" xfId="48" builtinId="0"/>
+    <cellStyle name="Normal 23 18" xfId="49" builtinId="0"/>
+    <cellStyle name="Normal 23 2" xfId="50" builtinId="0"/>
+    <cellStyle name="Normal 23 3" xfId="51" builtinId="0"/>
+    <cellStyle name="Normal 23 4" xfId="52" builtinId="0"/>
+    <cellStyle name="Normal 23 5" xfId="53" builtinId="0"/>
+    <cellStyle name="Normal 23 6" xfId="54" builtinId="0"/>
+    <cellStyle name="Normal 23 7" xfId="55" builtinId="0"/>
+    <cellStyle name="Normal 23 8" xfId="56" builtinId="0"/>
+    <cellStyle name="Normal 23 9" xfId="57" builtinId="0"/>
+    <cellStyle name="Normal 25 10" xfId="58" builtinId="0"/>
+    <cellStyle name="Normal 25 11" xfId="59" builtinId="0"/>
+    <cellStyle name="Normal 25 12" xfId="60" builtinId="0"/>
+    <cellStyle name="Normal 25 13" xfId="61" builtinId="0"/>
+    <cellStyle name="Normal 25 14" xfId="62" builtinId="0"/>
+    <cellStyle name="Normal 25 15" xfId="63" builtinId="0"/>
+    <cellStyle name="Normal 25 16" xfId="64" builtinId="0"/>
+    <cellStyle name="Normal 25 17" xfId="65" builtinId="0"/>
+    <cellStyle name="Normal 25 2" xfId="66" builtinId="0"/>
+    <cellStyle name="Normal 25 3" xfId="67" builtinId="0"/>
+    <cellStyle name="Normal 25 4" xfId="68" builtinId="0"/>
+    <cellStyle name="Normal 25 5" xfId="69" builtinId="0"/>
+    <cellStyle name="Normal 25 6" xfId="70" builtinId="0"/>
+    <cellStyle name="Normal 25 7" xfId="71" builtinId="0"/>
+    <cellStyle name="Normal 25 8" xfId="72" builtinId="0"/>
+    <cellStyle name="Normal 25 9" xfId="73" builtinId="0"/>
+    <cellStyle name="Normal 3" xfId="74" builtinId="0"/>
+    <cellStyle name="Normal 4" xfId="75" builtinId="0"/>
+    <cellStyle name="Normal 5" xfId="76" builtinId="0"/>
+    <cellStyle name="Normal 6" xfId="77" builtinId="0"/>
+    <cellStyle name="Normal 7" xfId="78" builtinId="0"/>
+    <cellStyle name="Normal 8" xfId="79" builtinId="0"/>
+    <cellStyle name="Normal 9" xfId="80" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="left"/>
+      <border>
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -651,8 +679,8 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="left"/>
+      <border>
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -674,8 +702,8 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="left"/>
+      <border>
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -697,7 +725,7 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <border>
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -722,7 +750,7 @@
       <font>
         <b/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
+      <border>
         <left/>
         <right style="thin">
           <color indexed="64"/>
@@ -749,7 +777,7 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <border>
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -772,7 +800,7 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <border>
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -790,7 +818,7 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <border>
         <left style="medium">
           <color indexed="64"/>
         </left>
@@ -866,7 +894,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="TableStyleLight9 2" pivot="0" count="7">
+    <tableStyle name="TableStyleLight9 2" pivot="0" table="0" count="7">
       <tableStyleElement type="wholeTable" dxfId="16"/>
       <tableStyleElement type="firstColumn" dxfId="15"/>
       <tableStyleElement type="lastColumn" dxfId="14"/>
@@ -877,44 +905,44 @@
     </tableStyle>
   </tableStyles>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="B3:J100" totalsRowShown="0" tableBorderDxfId="9">
-  <sortState ref="B4:E6">
-    <sortCondition descending="1" ref="B3:B65536"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="B3:J100" tableType="worksheet" headerRowCount="1" insertRow="0" insertRowShift="0" totalsRowShown="0" published="0" tableBorderDxfId="9">
+  <sortState columnSort="0" caseSensitive="0" sortMethod="none" ref="B4:E6">
+    <sortCondition descending="1" sortBy="value" ref="B3:B65536" iconSet="3Arrows"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" name="Typography Name"/>
-    <tableColumn id="2" name="Font"/>
-    <tableColumn id="3" name="Size"/>
-    <tableColumn id="4" name="Bpp"/>
-    <tableColumn id="5" name="Fallback Character"/>
-    <tableColumn id="6" name="Wildcard Characters"/>
-    <tableColumn id="9" name="Widget Wildcard Characters"/>
-    <tableColumn id="7" name="Wildcard Ranges"/>
-    <tableColumn id="8" name="Ellipsis Character"/>
+    <tableColumn id="1" name="Typography Name" totalsRowFunction="none"/>
+    <tableColumn id="2" name="Font" totalsRowFunction="none"/>
+    <tableColumn id="3" name="Size" totalsRowFunction="none"/>
+    <tableColumn id="4" name="Bpp" totalsRowFunction="none"/>
+    <tableColumn id="5" name="Fallback Character" totalsRowFunction="none"/>
+    <tableColumn id="6" name="Wildcard Characters" totalsRowFunction="none"/>
+    <tableColumn id="9" name="Widget Wildcard Characters" totalsRowFunction="none"/>
+    <tableColumn id="7" name="Wildcard Ranges" totalsRowFunction="none"/>
+    <tableColumn id="8" name="Ellipsis Character" totalsRowFunction="none"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table3" displayName="Table3" ref="L4:P10" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table3" displayName="Table3" ref="L4:P10" tableType="worksheet" headerRowCount="1" insertRow="0" insertRowShift="0" totalsRowShown="0" published="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
   <tableColumns count="5">
-    <tableColumn id="1" name="Column" dataDxfId="4"/>
-    <tableColumn id="2" name="Description" dataDxfId="3"/>
-    <tableColumn id="3" name="Example 1" dataDxfId="2"/>
-    <tableColumn id="4" name="Example 2" dataDxfId="1"/>
-    <tableColumn id="5" name="Example 3" dataDxfId="0"/>
+    <tableColumn id="1" name="Column" totalsRowFunction="none" dataDxfId="4"/>
+    <tableColumn id="2" name="Description" totalsRowFunction="none" dataDxfId="3"/>
+    <tableColumn id="3" name="Example 1" totalsRowFunction="none" dataDxfId="2"/>
+    <tableColumn id="4" name="Example 2" totalsRowFunction="none" dataDxfId="1"/>
+    <tableColumn id="5" name="Example 3" totalsRowFunction="none"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -964,8 +992,8 @@
     <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
+        <a:ea/>
+        <a:cs/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
@@ -999,8 +1027,8 @@
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
+        <a:ea/>
+        <a:cs/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
@@ -1035,169 +1063,108 @@
     </a:fontScheme>
     <a:fmtScheme name="Office">
       <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill flip="none" rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <gs>
               <a:schemeClr val="phClr">
                 <a:tint val="50000"/>
                 <a:satMod val="300000"/>
               </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
+            </gs>
+            <gs pos="35000">
               <a:schemeClr val="phClr">
                 <a:tint val="37000"/>
                 <a:satMod val="300000"/>
               </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
+            </gs>
+            <gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
-            </a:gs>
+            </gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill flip="none" rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <gs>
               <a:schemeClr val="phClr">
                 <a:shade val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
+            </gs>
+            <gs pos="80000">
               <a:schemeClr val="phClr">
                 <a:shade val="93000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
+            </gs>
+            <gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
-            </a:gs>
+            </gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+      </a:fillStyleLst>
+      <a:bgFillStyleLst>
+        <a:gradFill flip="none" rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <gs>
               <a:schemeClr val="phClr">
                 <a:tint val="40000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
+            </gs>
+            <gs pos="40000">
               <a:schemeClr val="phClr">
                 <a:tint val="45000"/>
                 <a:shade val="99000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
+            </gs>
+            <gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
-            </a:gs>
+            </gs>
           </a:gsLst>
           <a:path path="circle">
             <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill flip="none" rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <gs>
               <a:schemeClr val="phClr">
                 <a:tint val="80000"/>
                 <a:satMod val="300000"/>
               </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
+            </gs>
+            <gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
-            </a:gs>
+            </gs>
           </a:gsLst>
           <a:path path="circle">
             <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
       </a:bgFillStyleLst>
+      <a:lnStyleLst/>
+      <a:effectStyleLst/>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults>
@@ -1208,24 +1175,23 @@
           <a:ext cx="1" cy="1"/>
         </a:xfrm>
         <a:custGeom>
+          <a:rect l="0" t="0" r="0" b="0"/>
           <a:avLst/>
           <a:gdLst/>
-          <a:ahLst/>
           <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst/>
         </a:custGeom>
         <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="090000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+          <a:srgbClr val="090000"/>
         </a:solidFill>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="400000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+            <a:srgbClr val="400000"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:round/>
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="none" w="med" len="med"/>
+          <a:headEnd w="med" len="med"/>
+          <a:tailEnd w="med" len="med"/>
         </a:ln>
         <a:effectLst/>
         <a:extLst>
@@ -1240,7 +1206,7 @@
           </a:ext>
         </a:extLst>
       </a:spPr>
-      <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" upright="1"/>
+      <a:bodyPr rot="0" vertOverflow="clip" vert="horz" wrap="square" lIns="18288" rtlCol="0" anchor="t" upright="1"/>
       <a:lstStyle/>
     </a:spDef>
     <a:lnDef>
@@ -1250,24 +1216,23 @@
           <a:ext cx="1" cy="1"/>
         </a:xfrm>
         <a:custGeom>
+          <a:rect l="0" t="0" r="0" b="0"/>
           <a:avLst/>
           <a:gdLst/>
-          <a:ahLst/>
           <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst/>
         </a:custGeom>
         <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="090000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+          <a:srgbClr val="090000"/>
         </a:solidFill>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="400000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+            <a:srgbClr val="400000"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:round/>
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="none" w="med" len="med"/>
+          <a:headEnd w="med" len="med"/>
+          <a:tailEnd w="med" len="med"/>
         </a:ln>
         <a:effectLst/>
         <a:extLst>
@@ -1282,7 +1247,7 @@
           </a:ext>
         </a:extLst>
       </a:spPr>
-      <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" upright="1"/>
+      <a:bodyPr rot="0" vertOverflow="clip" vert="horz" wrap="square" lIns="18288" rtlCol="0" anchor="t" upright="1"/>
       <a:lstStyle/>
     </a:lnDef>
   </a:objectDefaults>
@@ -1374,7 +1339,7 @@
         <v>39</v>
       </c>
       <c r="D4">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -1382,10 +1347,18 @@
       <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="G4"/>
-      <c r="H4"/>
-      <c r="I4"/>
-      <c r="J4"/>
+      <c r="G4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" t="s">
+        <v>44</v>
+      </c>
       <c r="L4" s="4" t="s">
         <v>9</v>
       </c>
@@ -1418,10 +1391,18 @@
       <c r="F5" t="s">
         <v>17</v>
       </c>
-      <c r="G5"/>
-      <c r="H5"/>
-      <c r="I5"/>
-      <c r="J5"/>
+      <c r="G5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" t="s">
+        <v>44</v>
+      </c>
       <c r="L5" s="7" t="s">
         <v>1</v>
       </c>
@@ -1452,10 +1433,18 @@
       <c r="F6" t="s">
         <v>17</v>
       </c>
-      <c r="G6"/>
-      <c r="H6"/>
-      <c r="I6"/>
-      <c r="J6"/>
+      <c r="G6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" t="s">
+        <v>44</v>
+      </c>
       <c r="L6" s="7" t="s">
         <v>2</v>
       </c>
@@ -1601,6 +1590,40 @@
         <v>36</v>
       </c>
     </row>
+    <row r="4">
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Improved pressure display and changes to the gitignore file
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="52">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t xml:space="preserve">Cisnienie: &lt;value&gt; hpa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cisnienie: &lt;value&gt; hPa</t>
   </si>
 </sst>
 </file>
@@ -1621,7 +1624,7 @@
         <v>47</v>
       </c>
       <c r="F5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removal of the use of the LPS25 sensor
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -141,44 +141,13 @@
   </si>
   <si>
     <t xml:space="preserve">Small</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a-z,A-Z,0-9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"/>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Left</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LTR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Temperatura: &lt;value&gt; *C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cisnienie: &lt;value&gt; hpa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cisnienie: &lt;value&gt; hPa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -450,127 +419,127 @@
     </border>
   </borders>
   <cellStyleXfs count="82">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="26">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="81" applyFont="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="81" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="81" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -578,91 +547,91 @@
   <cellStyles count="82">
     <cellStyle name="Accent1" xfId="81" builtinId="29"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="1" builtinId="0"/>
-    <cellStyle name="Normal 10 2" xfId="2" builtinId="0"/>
-    <cellStyle name="Normal 11" xfId="3" builtinId="0"/>
-    <cellStyle name="Normal 12" xfId="4" builtinId="0"/>
-    <cellStyle name="Normal 13" xfId="5" builtinId="0"/>
-    <cellStyle name="Normal 14" xfId="6" builtinId="0"/>
-    <cellStyle name="Normal 14 2" xfId="7" builtinId="0"/>
-    <cellStyle name="Normal 15" xfId="8" builtinId="0"/>
-    <cellStyle name="Normal 16" xfId="9" builtinId="0"/>
-    <cellStyle name="Normal 16 2" xfId="10" builtinId="0"/>
-    <cellStyle name="Normal 16 3" xfId="11" builtinId="0"/>
-    <cellStyle name="Normal 17 2" xfId="12" builtinId="0"/>
-    <cellStyle name="Normal 17 3" xfId="13" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="14" builtinId="0"/>
-    <cellStyle name="Normal 2 2" xfId="15" builtinId="0"/>
-    <cellStyle name="Normal 2 3" xfId="16" builtinId="0"/>
-    <cellStyle name="Normal 2 4" xfId="17" builtinId="0"/>
-    <cellStyle name="Normal 2 5" xfId="18" builtinId="0"/>
-    <cellStyle name="Normal 2 6" xfId="19" builtinId="0"/>
-    <cellStyle name="Normal 2 7" xfId="20" builtinId="0"/>
-    <cellStyle name="Normal 2 8" xfId="21" builtinId="0"/>
-    <cellStyle name="Normal 2 9" xfId="22" builtinId="0"/>
-    <cellStyle name="Normal 22" xfId="23" builtinId="0"/>
-    <cellStyle name="Normal 22 10" xfId="24" builtinId="0"/>
-    <cellStyle name="Normal 22 11" xfId="25" builtinId="0"/>
-    <cellStyle name="Normal 22 12" xfId="26" builtinId="0"/>
-    <cellStyle name="Normal 22 13" xfId="27" builtinId="0"/>
-    <cellStyle name="Normal 22 14" xfId="28" builtinId="0"/>
-    <cellStyle name="Normal 22 15" xfId="29" builtinId="0"/>
-    <cellStyle name="Normal 22 16" xfId="30" builtinId="0"/>
-    <cellStyle name="Normal 22 17" xfId="31" builtinId="0"/>
-    <cellStyle name="Normal 22 18" xfId="32" builtinId="0"/>
-    <cellStyle name="Normal 22 2" xfId="33" builtinId="0"/>
-    <cellStyle name="Normal 22 3" xfId="34" builtinId="0"/>
-    <cellStyle name="Normal 22 4" xfId="35" builtinId="0"/>
-    <cellStyle name="Normal 22 5" xfId="36" builtinId="0"/>
-    <cellStyle name="Normal 22 6" xfId="37" builtinId="0"/>
-    <cellStyle name="Normal 22 7" xfId="38" builtinId="0"/>
-    <cellStyle name="Normal 22 8" xfId="39" builtinId="0"/>
-    <cellStyle name="Normal 22 9" xfId="40" builtinId="0"/>
-    <cellStyle name="Normal 23 10" xfId="41" builtinId="0"/>
-    <cellStyle name="Normal 23 11" xfId="42" builtinId="0"/>
-    <cellStyle name="Normal 23 12" xfId="43" builtinId="0"/>
-    <cellStyle name="Normal 23 13" xfId="44" builtinId="0"/>
-    <cellStyle name="Normal 23 14" xfId="45" builtinId="0"/>
-    <cellStyle name="Normal 23 15" xfId="46" builtinId="0"/>
-    <cellStyle name="Normal 23 16" xfId="47" builtinId="0"/>
-    <cellStyle name="Normal 23 17" xfId="48" builtinId="0"/>
-    <cellStyle name="Normal 23 18" xfId="49" builtinId="0"/>
-    <cellStyle name="Normal 23 2" xfId="50" builtinId="0"/>
-    <cellStyle name="Normal 23 3" xfId="51" builtinId="0"/>
-    <cellStyle name="Normal 23 4" xfId="52" builtinId="0"/>
-    <cellStyle name="Normal 23 5" xfId="53" builtinId="0"/>
-    <cellStyle name="Normal 23 6" xfId="54" builtinId="0"/>
-    <cellStyle name="Normal 23 7" xfId="55" builtinId="0"/>
-    <cellStyle name="Normal 23 8" xfId="56" builtinId="0"/>
-    <cellStyle name="Normal 23 9" xfId="57" builtinId="0"/>
-    <cellStyle name="Normal 25 10" xfId="58" builtinId="0"/>
-    <cellStyle name="Normal 25 11" xfId="59" builtinId="0"/>
-    <cellStyle name="Normal 25 12" xfId="60" builtinId="0"/>
-    <cellStyle name="Normal 25 13" xfId="61" builtinId="0"/>
-    <cellStyle name="Normal 25 14" xfId="62" builtinId="0"/>
-    <cellStyle name="Normal 25 15" xfId="63" builtinId="0"/>
-    <cellStyle name="Normal 25 16" xfId="64" builtinId="0"/>
-    <cellStyle name="Normal 25 17" xfId="65" builtinId="0"/>
-    <cellStyle name="Normal 25 2" xfId="66" builtinId="0"/>
-    <cellStyle name="Normal 25 3" xfId="67" builtinId="0"/>
-    <cellStyle name="Normal 25 4" xfId="68" builtinId="0"/>
-    <cellStyle name="Normal 25 5" xfId="69" builtinId="0"/>
-    <cellStyle name="Normal 25 6" xfId="70" builtinId="0"/>
-    <cellStyle name="Normal 25 7" xfId="71" builtinId="0"/>
-    <cellStyle name="Normal 25 8" xfId="72" builtinId="0"/>
-    <cellStyle name="Normal 25 9" xfId="73" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="74" builtinId="0"/>
-    <cellStyle name="Normal 4" xfId="75" builtinId="0"/>
-    <cellStyle name="Normal 5" xfId="76" builtinId="0"/>
-    <cellStyle name="Normal 6" xfId="77" builtinId="0"/>
-    <cellStyle name="Normal 7" xfId="78" builtinId="0"/>
-    <cellStyle name="Normal 8" xfId="79" builtinId="0"/>
-    <cellStyle name="Normal 9" xfId="80" builtinId="0"/>
+    <cellStyle name="Normal 10" xfId="1"/>
+    <cellStyle name="Normal 10 2" xfId="2"/>
+    <cellStyle name="Normal 11" xfId="3"/>
+    <cellStyle name="Normal 12" xfId="4"/>
+    <cellStyle name="Normal 13" xfId="5"/>
+    <cellStyle name="Normal 14" xfId="6"/>
+    <cellStyle name="Normal 14 2" xfId="7"/>
+    <cellStyle name="Normal 15" xfId="8"/>
+    <cellStyle name="Normal 16" xfId="9"/>
+    <cellStyle name="Normal 16 2" xfId="10"/>
+    <cellStyle name="Normal 16 3" xfId="11"/>
+    <cellStyle name="Normal 17 2" xfId="12"/>
+    <cellStyle name="Normal 17 3" xfId="13"/>
+    <cellStyle name="Normal 2" xfId="14"/>
+    <cellStyle name="Normal 2 2" xfId="15"/>
+    <cellStyle name="Normal 2 3" xfId="16"/>
+    <cellStyle name="Normal 2 4" xfId="17"/>
+    <cellStyle name="Normal 2 5" xfId="18"/>
+    <cellStyle name="Normal 2 6" xfId="19"/>
+    <cellStyle name="Normal 2 7" xfId="20"/>
+    <cellStyle name="Normal 2 8" xfId="21"/>
+    <cellStyle name="Normal 2 9" xfId="22"/>
+    <cellStyle name="Normal 22" xfId="23"/>
+    <cellStyle name="Normal 22 10" xfId="24"/>
+    <cellStyle name="Normal 22 11" xfId="25"/>
+    <cellStyle name="Normal 22 12" xfId="26"/>
+    <cellStyle name="Normal 22 13" xfId="27"/>
+    <cellStyle name="Normal 22 14" xfId="28"/>
+    <cellStyle name="Normal 22 15" xfId="29"/>
+    <cellStyle name="Normal 22 16" xfId="30"/>
+    <cellStyle name="Normal 22 17" xfId="31"/>
+    <cellStyle name="Normal 22 18" xfId="32"/>
+    <cellStyle name="Normal 22 2" xfId="33"/>
+    <cellStyle name="Normal 22 3" xfId="34"/>
+    <cellStyle name="Normal 22 4" xfId="35"/>
+    <cellStyle name="Normal 22 5" xfId="36"/>
+    <cellStyle name="Normal 22 6" xfId="37"/>
+    <cellStyle name="Normal 22 7" xfId="38"/>
+    <cellStyle name="Normal 22 8" xfId="39"/>
+    <cellStyle name="Normal 22 9" xfId="40"/>
+    <cellStyle name="Normal 23 10" xfId="41"/>
+    <cellStyle name="Normal 23 11" xfId="42"/>
+    <cellStyle name="Normal 23 12" xfId="43"/>
+    <cellStyle name="Normal 23 13" xfId="44"/>
+    <cellStyle name="Normal 23 14" xfId="45"/>
+    <cellStyle name="Normal 23 15" xfId="46"/>
+    <cellStyle name="Normal 23 16" xfId="47"/>
+    <cellStyle name="Normal 23 17" xfId="48"/>
+    <cellStyle name="Normal 23 18" xfId="49"/>
+    <cellStyle name="Normal 23 2" xfId="50"/>
+    <cellStyle name="Normal 23 3" xfId="51"/>
+    <cellStyle name="Normal 23 4" xfId="52"/>
+    <cellStyle name="Normal 23 5" xfId="53"/>
+    <cellStyle name="Normal 23 6" xfId="54"/>
+    <cellStyle name="Normal 23 7" xfId="55"/>
+    <cellStyle name="Normal 23 8" xfId="56"/>
+    <cellStyle name="Normal 23 9" xfId="57"/>
+    <cellStyle name="Normal 25 10" xfId="58"/>
+    <cellStyle name="Normal 25 11" xfId="59"/>
+    <cellStyle name="Normal 25 12" xfId="60"/>
+    <cellStyle name="Normal 25 13" xfId="61"/>
+    <cellStyle name="Normal 25 14" xfId="62"/>
+    <cellStyle name="Normal 25 15" xfId="63"/>
+    <cellStyle name="Normal 25 16" xfId="64"/>
+    <cellStyle name="Normal 25 17" xfId="65"/>
+    <cellStyle name="Normal 25 2" xfId="66"/>
+    <cellStyle name="Normal 25 3" xfId="67"/>
+    <cellStyle name="Normal 25 4" xfId="68"/>
+    <cellStyle name="Normal 25 5" xfId="69"/>
+    <cellStyle name="Normal 25 6" xfId="70"/>
+    <cellStyle name="Normal 25 7" xfId="71"/>
+    <cellStyle name="Normal 25 8" xfId="72"/>
+    <cellStyle name="Normal 25 9" xfId="73"/>
+    <cellStyle name="Normal 3" xfId="74"/>
+    <cellStyle name="Normal 4" xfId="75"/>
+    <cellStyle name="Normal 5" xfId="76"/>
+    <cellStyle name="Normal 6" xfId="77"/>
+    <cellStyle name="Normal 7" xfId="78"/>
+    <cellStyle name="Normal 8" xfId="79"/>
+    <cellStyle name="Normal 9" xfId="80"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
-      <alignment horizontal="left"/>
-      <border>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -682,8 +651,8 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="left"/>
-      <border>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -705,8 +674,8 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="left"/>
-      <border>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -728,7 +697,7 @@
       </border>
     </dxf>
     <dxf>
-      <border>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -753,7 +722,7 @@
       <font>
         <b/>
       </font>
-      <border>
+      <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
           <color indexed="64"/>
@@ -780,7 +749,7 @@
       </border>
     </dxf>
     <dxf>
-      <border>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -803,7 +772,7 @@
       </border>
     </dxf>
     <dxf>
-      <border>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -821,7 +790,7 @@
       </border>
     </dxf>
     <dxf>
-      <border>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
           <color indexed="64"/>
         </left>
@@ -897,7 +866,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="TableStyleLight9 2" pivot="0" table="0" count="7">
+    <tableStyle name="TableStyleLight9 2" pivot="0" count="7">
       <tableStyleElement type="wholeTable" dxfId="16"/>
       <tableStyleElement type="firstColumn" dxfId="15"/>
       <tableStyleElement type="lastColumn" dxfId="14"/>
@@ -908,44 +877,44 @@
     </tableStyle>
   </tableStyles>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="B3:J100" tableType="worksheet" headerRowCount="1" insertRow="0" insertRowShift="0" totalsRowShown="0" published="0" tableBorderDxfId="9">
-  <sortState columnSort="0" caseSensitive="0" sortMethod="none" ref="B4:E6">
-    <sortCondition descending="1" sortBy="value" ref="B3:B65536" iconSet="3Arrows"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="B3:J100" totalsRowShown="0" tableBorderDxfId="9">
+  <sortState ref="B4:E6">
+    <sortCondition descending="1" ref="B3:B65536"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" name="Typography Name" totalsRowFunction="none"/>
-    <tableColumn id="2" name="Font" totalsRowFunction="none"/>
-    <tableColumn id="3" name="Size" totalsRowFunction="none"/>
-    <tableColumn id="4" name="Bpp" totalsRowFunction="none"/>
-    <tableColumn id="5" name="Fallback Character" totalsRowFunction="none"/>
-    <tableColumn id="6" name="Wildcard Characters" totalsRowFunction="none"/>
-    <tableColumn id="9" name="Widget Wildcard Characters" totalsRowFunction="none"/>
-    <tableColumn id="7" name="Wildcard Ranges" totalsRowFunction="none"/>
-    <tableColumn id="8" name="Ellipsis Character" totalsRowFunction="none"/>
+    <tableColumn id="1" name="Typography Name"/>
+    <tableColumn id="2" name="Font"/>
+    <tableColumn id="3" name="Size"/>
+    <tableColumn id="4" name="Bpp"/>
+    <tableColumn id="5" name="Fallback Character"/>
+    <tableColumn id="6" name="Wildcard Characters"/>
+    <tableColumn id="9" name="Widget Wildcard Characters"/>
+    <tableColumn id="7" name="Wildcard Ranges"/>
+    <tableColumn id="8" name="Ellipsis Character"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table3" displayName="Table3" ref="L4:P10" tableType="worksheet" headerRowCount="1" insertRow="0" insertRowShift="0" totalsRowShown="0" published="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table3" displayName="Table3" ref="L4:P10" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
   <tableColumns count="5">
-    <tableColumn id="1" name="Column" totalsRowFunction="none" dataDxfId="4"/>
-    <tableColumn id="2" name="Description" totalsRowFunction="none" dataDxfId="3"/>
-    <tableColumn id="3" name="Example 1" totalsRowFunction="none" dataDxfId="2"/>
-    <tableColumn id="4" name="Example 2" totalsRowFunction="none" dataDxfId="1"/>
-    <tableColumn id="5" name="Example 3" totalsRowFunction="none"/>
+    <tableColumn id="1" name="Column" dataDxfId="4"/>
+    <tableColumn id="2" name="Description" dataDxfId="3"/>
+    <tableColumn id="3" name="Example 1" dataDxfId="2"/>
+    <tableColumn id="4" name="Example 2" dataDxfId="1"/>
+    <tableColumn id="5" name="Example 3" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -995,8 +964,8 @@
     <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
-        <a:ea/>
-        <a:cs/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
@@ -1030,8 +999,8 @@
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
-        <a:ea/>
-        <a:cs/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
@@ -1066,108 +1035,169 @@
     </a:fontScheme>
     <a:fmtScheme name="Office">
       <a:fillStyleLst>
-        <a:gradFill flip="none" rotWithShape="1">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <gs>
+            <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="50000"/>
                 <a:satMod val="300000"/>
               </a:schemeClr>
-            </gs>
-            <gs pos="35000">
+            </a:gs>
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
                 <a:tint val="37000"/>
                 <a:satMod val="300000"/>
               </a:schemeClr>
-            </gs>
-            <gs pos="100000">
+            </a:gs>
+            <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
-            </gs>
+            </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
-        <a:gradFill flip="none" rotWithShape="1">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <gs>
+            <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:shade val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
-            </gs>
-            <gs pos="80000">
+            </a:gs>
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
                 <a:shade val="93000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
-            </gs>
-            <gs pos="100000">
+            </a:gs>
+            <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
-            </gs>
+            </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-      </a:fillStyleLst>
-      <a:bgFillStyleLst>
-        <a:gradFill flip="none" rotWithShape="1">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <gs>
+            <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="40000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
-            </gs>
-            <gs pos="40000">
+            </a:gs>
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
                 <a:tint val="45000"/>
                 <a:shade val="99000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
-            </gs>
-            <gs pos="100000">
+            </a:gs>
+            <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
-            </gs>
+            </a:gs>
           </a:gsLst>
           <a:path path="circle">
             <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
-        <a:gradFill flip="none" rotWithShape="1">
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <gs>
+            <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="80000"/>
                 <a:satMod val="300000"/>
               </a:schemeClr>
-            </gs>
-            <gs pos="100000">
+            </a:gs>
+            <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
-            </gs>
+            </a:gs>
           </a:gsLst>
           <a:path path="circle">
             <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
       </a:bgFillStyleLst>
-      <a:lnStyleLst/>
-      <a:effectStyleLst/>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults>
@@ -1178,23 +1208,24 @@
           <a:ext cx="1" cy="1"/>
         </a:xfrm>
         <a:custGeom>
-          <a:rect l="0" t="0" r="0" b="0"/>
           <a:avLst/>
           <a:gdLst/>
+          <a:ahLst/>
           <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst/>
         </a:custGeom>
         <a:solidFill>
-          <a:srgbClr val="090000"/>
+          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="090000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
         </a:solidFill>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:srgbClr val="400000"/>
+            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="400000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:round/>
-          <a:headEnd w="med" len="med"/>
-          <a:tailEnd w="med" len="med"/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
         </a:ln>
         <a:effectLst/>
         <a:extLst>
@@ -1209,7 +1240,7 @@
           </a:ext>
         </a:extLst>
       </a:spPr>
-      <a:bodyPr rot="0" vertOverflow="clip" vert="horz" wrap="square" lIns="18288" rtlCol="0" anchor="t" upright="1"/>
+      <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" upright="1"/>
       <a:lstStyle/>
     </a:spDef>
     <a:lnDef>
@@ -1219,23 +1250,24 @@
           <a:ext cx="1" cy="1"/>
         </a:xfrm>
         <a:custGeom>
-          <a:rect l="0" t="0" r="0" b="0"/>
           <a:avLst/>
           <a:gdLst/>
+          <a:ahLst/>
           <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst/>
         </a:custGeom>
         <a:solidFill>
-          <a:srgbClr val="090000"/>
+          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="090000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
         </a:solidFill>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:srgbClr val="400000"/>
+            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="400000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:round/>
-          <a:headEnd w="med" len="med"/>
-          <a:tailEnd w="med" len="med"/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
         </a:ln>
         <a:effectLst/>
         <a:extLst>
@@ -1250,7 +1282,7 @@
           </a:ext>
         </a:extLst>
       </a:spPr>
-      <a:bodyPr rot="0" vertOverflow="clip" vert="horz" wrap="square" lIns="18288" rtlCol="0" anchor="t" upright="1"/>
+      <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" upright="1"/>
       <a:lstStyle/>
     </a:lnDef>
   </a:objectDefaults>
@@ -1342,7 +1374,7 @@
         <v>39</v>
       </c>
       <c r="D4">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -1350,18 +1382,10 @@
       <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="G4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I4" t="s">
-        <v>42</v>
-      </c>
-      <c r="J4" t="s">
-        <v>44</v>
-      </c>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4"/>
       <c r="L4" s="4" t="s">
         <v>9</v>
       </c>
@@ -1394,18 +1418,10 @@
       <c r="F5" t="s">
         <v>17</v>
       </c>
-      <c r="G5" t="s">
-        <v>44</v>
-      </c>
-      <c r="H5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I5" t="s">
-        <v>44</v>
-      </c>
-      <c r="J5" t="s">
-        <v>44</v>
-      </c>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5"/>
       <c r="L5" s="7" t="s">
         <v>1</v>
       </c>
@@ -1436,18 +1452,10 @@
       <c r="F6" t="s">
         <v>17</v>
       </c>
-      <c r="G6" t="s">
-        <v>44</v>
-      </c>
-      <c r="H6" t="s">
-        <v>44</v>
-      </c>
-      <c r="I6" t="s">
-        <v>44</v>
-      </c>
-      <c r="J6" t="s">
-        <v>44</v>
-      </c>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6"/>
+      <c r="J6"/>
       <c r="L6" s="7" t="s">
         <v>2</v>
       </c>
@@ -1593,40 +1601,6 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4">
-      <c r="B4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" t="s">
-        <v>51</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Added menu and operating modes of the counter.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="49">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -141,13 +141,35 @@
   </si>
   <si>
     <t xml:space="preserve">Small</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIME INTERVAL/MODE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FREQUENCY MEASUREMENT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -419,127 +441,127 @@
     </border>
   </borders>
   <cellStyleXfs count="82">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyAlignment="0"/>
   </cellStyleXfs>
   <cellXfs count="26">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="81" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="81" applyFont="1" applyAlignment="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="81" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -547,91 +569,91 @@
   <cellStyles count="82">
     <cellStyle name="Accent1" xfId="81" builtinId="29"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="1"/>
-    <cellStyle name="Normal 10 2" xfId="2"/>
-    <cellStyle name="Normal 11" xfId="3"/>
-    <cellStyle name="Normal 12" xfId="4"/>
-    <cellStyle name="Normal 13" xfId="5"/>
-    <cellStyle name="Normal 14" xfId="6"/>
-    <cellStyle name="Normal 14 2" xfId="7"/>
-    <cellStyle name="Normal 15" xfId="8"/>
-    <cellStyle name="Normal 16" xfId="9"/>
-    <cellStyle name="Normal 16 2" xfId="10"/>
-    <cellStyle name="Normal 16 3" xfId="11"/>
-    <cellStyle name="Normal 17 2" xfId="12"/>
-    <cellStyle name="Normal 17 3" xfId="13"/>
-    <cellStyle name="Normal 2" xfId="14"/>
-    <cellStyle name="Normal 2 2" xfId="15"/>
-    <cellStyle name="Normal 2 3" xfId="16"/>
-    <cellStyle name="Normal 2 4" xfId="17"/>
-    <cellStyle name="Normal 2 5" xfId="18"/>
-    <cellStyle name="Normal 2 6" xfId="19"/>
-    <cellStyle name="Normal 2 7" xfId="20"/>
-    <cellStyle name="Normal 2 8" xfId="21"/>
-    <cellStyle name="Normal 2 9" xfId="22"/>
-    <cellStyle name="Normal 22" xfId="23"/>
-    <cellStyle name="Normal 22 10" xfId="24"/>
-    <cellStyle name="Normal 22 11" xfId="25"/>
-    <cellStyle name="Normal 22 12" xfId="26"/>
-    <cellStyle name="Normal 22 13" xfId="27"/>
-    <cellStyle name="Normal 22 14" xfId="28"/>
-    <cellStyle name="Normal 22 15" xfId="29"/>
-    <cellStyle name="Normal 22 16" xfId="30"/>
-    <cellStyle name="Normal 22 17" xfId="31"/>
-    <cellStyle name="Normal 22 18" xfId="32"/>
-    <cellStyle name="Normal 22 2" xfId="33"/>
-    <cellStyle name="Normal 22 3" xfId="34"/>
-    <cellStyle name="Normal 22 4" xfId="35"/>
-    <cellStyle name="Normal 22 5" xfId="36"/>
-    <cellStyle name="Normal 22 6" xfId="37"/>
-    <cellStyle name="Normal 22 7" xfId="38"/>
-    <cellStyle name="Normal 22 8" xfId="39"/>
-    <cellStyle name="Normal 22 9" xfId="40"/>
-    <cellStyle name="Normal 23 10" xfId="41"/>
-    <cellStyle name="Normal 23 11" xfId="42"/>
-    <cellStyle name="Normal 23 12" xfId="43"/>
-    <cellStyle name="Normal 23 13" xfId="44"/>
-    <cellStyle name="Normal 23 14" xfId="45"/>
-    <cellStyle name="Normal 23 15" xfId="46"/>
-    <cellStyle name="Normal 23 16" xfId="47"/>
-    <cellStyle name="Normal 23 17" xfId="48"/>
-    <cellStyle name="Normal 23 18" xfId="49"/>
-    <cellStyle name="Normal 23 2" xfId="50"/>
-    <cellStyle name="Normal 23 3" xfId="51"/>
-    <cellStyle name="Normal 23 4" xfId="52"/>
-    <cellStyle name="Normal 23 5" xfId="53"/>
-    <cellStyle name="Normal 23 6" xfId="54"/>
-    <cellStyle name="Normal 23 7" xfId="55"/>
-    <cellStyle name="Normal 23 8" xfId="56"/>
-    <cellStyle name="Normal 23 9" xfId="57"/>
-    <cellStyle name="Normal 25 10" xfId="58"/>
-    <cellStyle name="Normal 25 11" xfId="59"/>
-    <cellStyle name="Normal 25 12" xfId="60"/>
-    <cellStyle name="Normal 25 13" xfId="61"/>
-    <cellStyle name="Normal 25 14" xfId="62"/>
-    <cellStyle name="Normal 25 15" xfId="63"/>
-    <cellStyle name="Normal 25 16" xfId="64"/>
-    <cellStyle name="Normal 25 17" xfId="65"/>
-    <cellStyle name="Normal 25 2" xfId="66"/>
-    <cellStyle name="Normal 25 3" xfId="67"/>
-    <cellStyle name="Normal 25 4" xfId="68"/>
-    <cellStyle name="Normal 25 5" xfId="69"/>
-    <cellStyle name="Normal 25 6" xfId="70"/>
-    <cellStyle name="Normal 25 7" xfId="71"/>
-    <cellStyle name="Normal 25 8" xfId="72"/>
-    <cellStyle name="Normal 25 9" xfId="73"/>
-    <cellStyle name="Normal 3" xfId="74"/>
-    <cellStyle name="Normal 4" xfId="75"/>
-    <cellStyle name="Normal 5" xfId="76"/>
-    <cellStyle name="Normal 6" xfId="77"/>
-    <cellStyle name="Normal 7" xfId="78"/>
-    <cellStyle name="Normal 8" xfId="79"/>
-    <cellStyle name="Normal 9" xfId="80"/>
+    <cellStyle name="Normal 10" xfId="1" builtinId="0"/>
+    <cellStyle name="Normal 10 2" xfId="2" builtinId="0"/>
+    <cellStyle name="Normal 11" xfId="3" builtinId="0"/>
+    <cellStyle name="Normal 12" xfId="4" builtinId="0"/>
+    <cellStyle name="Normal 13" xfId="5" builtinId="0"/>
+    <cellStyle name="Normal 14" xfId="6" builtinId="0"/>
+    <cellStyle name="Normal 14 2" xfId="7" builtinId="0"/>
+    <cellStyle name="Normal 15" xfId="8" builtinId="0"/>
+    <cellStyle name="Normal 16" xfId="9" builtinId="0"/>
+    <cellStyle name="Normal 16 2" xfId="10" builtinId="0"/>
+    <cellStyle name="Normal 16 3" xfId="11" builtinId="0"/>
+    <cellStyle name="Normal 17 2" xfId="12" builtinId="0"/>
+    <cellStyle name="Normal 17 3" xfId="13" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="14" builtinId="0"/>
+    <cellStyle name="Normal 2 2" xfId="15" builtinId="0"/>
+    <cellStyle name="Normal 2 3" xfId="16" builtinId="0"/>
+    <cellStyle name="Normal 2 4" xfId="17" builtinId="0"/>
+    <cellStyle name="Normal 2 5" xfId="18" builtinId="0"/>
+    <cellStyle name="Normal 2 6" xfId="19" builtinId="0"/>
+    <cellStyle name="Normal 2 7" xfId="20" builtinId="0"/>
+    <cellStyle name="Normal 2 8" xfId="21" builtinId="0"/>
+    <cellStyle name="Normal 2 9" xfId="22" builtinId="0"/>
+    <cellStyle name="Normal 22" xfId="23" builtinId="0"/>
+    <cellStyle name="Normal 22 10" xfId="24" builtinId="0"/>
+    <cellStyle name="Normal 22 11" xfId="25" builtinId="0"/>
+    <cellStyle name="Normal 22 12" xfId="26" builtinId="0"/>
+    <cellStyle name="Normal 22 13" xfId="27" builtinId="0"/>
+    <cellStyle name="Normal 22 14" xfId="28" builtinId="0"/>
+    <cellStyle name="Normal 22 15" xfId="29" builtinId="0"/>
+    <cellStyle name="Normal 22 16" xfId="30" builtinId="0"/>
+    <cellStyle name="Normal 22 17" xfId="31" builtinId="0"/>
+    <cellStyle name="Normal 22 18" xfId="32" builtinId="0"/>
+    <cellStyle name="Normal 22 2" xfId="33" builtinId="0"/>
+    <cellStyle name="Normal 22 3" xfId="34" builtinId="0"/>
+    <cellStyle name="Normal 22 4" xfId="35" builtinId="0"/>
+    <cellStyle name="Normal 22 5" xfId="36" builtinId="0"/>
+    <cellStyle name="Normal 22 6" xfId="37" builtinId="0"/>
+    <cellStyle name="Normal 22 7" xfId="38" builtinId="0"/>
+    <cellStyle name="Normal 22 8" xfId="39" builtinId="0"/>
+    <cellStyle name="Normal 22 9" xfId="40" builtinId="0"/>
+    <cellStyle name="Normal 23 10" xfId="41" builtinId="0"/>
+    <cellStyle name="Normal 23 11" xfId="42" builtinId="0"/>
+    <cellStyle name="Normal 23 12" xfId="43" builtinId="0"/>
+    <cellStyle name="Normal 23 13" xfId="44" builtinId="0"/>
+    <cellStyle name="Normal 23 14" xfId="45" builtinId="0"/>
+    <cellStyle name="Normal 23 15" xfId="46" builtinId="0"/>
+    <cellStyle name="Normal 23 16" xfId="47" builtinId="0"/>
+    <cellStyle name="Normal 23 17" xfId="48" builtinId="0"/>
+    <cellStyle name="Normal 23 18" xfId="49" builtinId="0"/>
+    <cellStyle name="Normal 23 2" xfId="50" builtinId="0"/>
+    <cellStyle name="Normal 23 3" xfId="51" builtinId="0"/>
+    <cellStyle name="Normal 23 4" xfId="52" builtinId="0"/>
+    <cellStyle name="Normal 23 5" xfId="53" builtinId="0"/>
+    <cellStyle name="Normal 23 6" xfId="54" builtinId="0"/>
+    <cellStyle name="Normal 23 7" xfId="55" builtinId="0"/>
+    <cellStyle name="Normal 23 8" xfId="56" builtinId="0"/>
+    <cellStyle name="Normal 23 9" xfId="57" builtinId="0"/>
+    <cellStyle name="Normal 25 10" xfId="58" builtinId="0"/>
+    <cellStyle name="Normal 25 11" xfId="59" builtinId="0"/>
+    <cellStyle name="Normal 25 12" xfId="60" builtinId="0"/>
+    <cellStyle name="Normal 25 13" xfId="61" builtinId="0"/>
+    <cellStyle name="Normal 25 14" xfId="62" builtinId="0"/>
+    <cellStyle name="Normal 25 15" xfId="63" builtinId="0"/>
+    <cellStyle name="Normal 25 16" xfId="64" builtinId="0"/>
+    <cellStyle name="Normal 25 17" xfId="65" builtinId="0"/>
+    <cellStyle name="Normal 25 2" xfId="66" builtinId="0"/>
+    <cellStyle name="Normal 25 3" xfId="67" builtinId="0"/>
+    <cellStyle name="Normal 25 4" xfId="68" builtinId="0"/>
+    <cellStyle name="Normal 25 5" xfId="69" builtinId="0"/>
+    <cellStyle name="Normal 25 6" xfId="70" builtinId="0"/>
+    <cellStyle name="Normal 25 7" xfId="71" builtinId="0"/>
+    <cellStyle name="Normal 25 8" xfId="72" builtinId="0"/>
+    <cellStyle name="Normal 25 9" xfId="73" builtinId="0"/>
+    <cellStyle name="Normal 3" xfId="74" builtinId="0"/>
+    <cellStyle name="Normal 4" xfId="75" builtinId="0"/>
+    <cellStyle name="Normal 5" xfId="76" builtinId="0"/>
+    <cellStyle name="Normal 6" xfId="77" builtinId="0"/>
+    <cellStyle name="Normal 7" xfId="78" builtinId="0"/>
+    <cellStyle name="Normal 8" xfId="79" builtinId="0"/>
+    <cellStyle name="Normal 9" xfId="80" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="left"/>
+      <border>
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -651,8 +673,8 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="left"/>
+      <border>
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -674,8 +696,8 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="left"/>
+      <border>
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -697,7 +719,7 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <border>
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -722,7 +744,7 @@
       <font>
         <b/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
+      <border>
         <left/>
         <right style="thin">
           <color indexed="64"/>
@@ -749,7 +771,7 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <border>
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -772,7 +794,7 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <border>
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -790,7 +812,7 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <border>
         <left style="medium">
           <color indexed="64"/>
         </left>
@@ -866,7 +888,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="TableStyleLight9 2" pivot="0" count="7">
+    <tableStyle name="TableStyleLight9 2" pivot="0" table="0" count="7">
       <tableStyleElement type="wholeTable" dxfId="16"/>
       <tableStyleElement type="firstColumn" dxfId="15"/>
       <tableStyleElement type="lastColumn" dxfId="14"/>
@@ -877,44 +899,44 @@
     </tableStyle>
   </tableStyles>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="B3:J100" totalsRowShown="0" tableBorderDxfId="9">
-  <sortState ref="B4:E6">
-    <sortCondition descending="1" ref="B3:B65536"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="B3:J100" tableType="worksheet" headerRowCount="1" insertRow="0" insertRowShift="0" totalsRowShown="0" published="0" tableBorderDxfId="9">
+  <sortState columnSort="0" caseSensitive="0" sortMethod="none" ref="B4:E6">
+    <sortCondition descending="1" sortBy="value" ref="B3:B65536" iconSet="3Arrows"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" name="Typography Name"/>
-    <tableColumn id="2" name="Font"/>
-    <tableColumn id="3" name="Size"/>
-    <tableColumn id="4" name="Bpp"/>
-    <tableColumn id="5" name="Fallback Character"/>
-    <tableColumn id="6" name="Wildcard Characters"/>
-    <tableColumn id="9" name="Widget Wildcard Characters"/>
-    <tableColumn id="7" name="Wildcard Ranges"/>
-    <tableColumn id="8" name="Ellipsis Character"/>
+    <tableColumn id="1" name="Typography Name" totalsRowFunction="none"/>
+    <tableColumn id="2" name="Font" totalsRowFunction="none"/>
+    <tableColumn id="3" name="Size" totalsRowFunction="none"/>
+    <tableColumn id="4" name="Bpp" totalsRowFunction="none"/>
+    <tableColumn id="5" name="Fallback Character" totalsRowFunction="none"/>
+    <tableColumn id="6" name="Wildcard Characters" totalsRowFunction="none"/>
+    <tableColumn id="9" name="Widget Wildcard Characters" totalsRowFunction="none"/>
+    <tableColumn id="7" name="Wildcard Ranges" totalsRowFunction="none"/>
+    <tableColumn id="8" name="Ellipsis Character" totalsRowFunction="none"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table3" displayName="Table3" ref="L4:P10" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table3" displayName="Table3" ref="L4:P10" tableType="worksheet" headerRowCount="1" insertRow="0" insertRowShift="0" totalsRowShown="0" published="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
   <tableColumns count="5">
-    <tableColumn id="1" name="Column" dataDxfId="4"/>
-    <tableColumn id="2" name="Description" dataDxfId="3"/>
-    <tableColumn id="3" name="Example 1" dataDxfId="2"/>
-    <tableColumn id="4" name="Example 2" dataDxfId="1"/>
-    <tableColumn id="5" name="Example 3" dataDxfId="0"/>
+    <tableColumn id="1" name="Column" totalsRowFunction="none" dataDxfId="4"/>
+    <tableColumn id="2" name="Description" totalsRowFunction="none" dataDxfId="3"/>
+    <tableColumn id="3" name="Example 1" totalsRowFunction="none" dataDxfId="2"/>
+    <tableColumn id="4" name="Example 2" totalsRowFunction="none" dataDxfId="1"/>
+    <tableColumn id="5" name="Example 3" totalsRowFunction="none"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -964,8 +986,8 @@
     <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
+        <a:ea/>
+        <a:cs/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
@@ -999,8 +1021,8 @@
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
+        <a:ea/>
+        <a:cs/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
@@ -1035,169 +1057,108 @@
     </a:fontScheme>
     <a:fmtScheme name="Office">
       <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill flip="none" rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <gs>
               <a:schemeClr val="phClr">
                 <a:tint val="50000"/>
                 <a:satMod val="300000"/>
               </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
+            </gs>
+            <gs pos="35000">
               <a:schemeClr val="phClr">
                 <a:tint val="37000"/>
                 <a:satMod val="300000"/>
               </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
+            </gs>
+            <gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
-            </a:gs>
+            </gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill flip="none" rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <gs>
               <a:schemeClr val="phClr">
                 <a:shade val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
+            </gs>
+            <gs pos="80000">
               <a:schemeClr val="phClr">
                 <a:shade val="93000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
+            </gs>
+            <gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
-            </a:gs>
+            </gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+      </a:fillStyleLst>
+      <a:bgFillStyleLst>
+        <a:gradFill flip="none" rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <gs>
               <a:schemeClr val="phClr">
                 <a:tint val="40000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
+            </gs>
+            <gs pos="40000">
               <a:schemeClr val="phClr">
                 <a:tint val="45000"/>
                 <a:shade val="99000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
+            </gs>
+            <gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
-            </a:gs>
+            </gs>
           </a:gsLst>
           <a:path path="circle">
             <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill flip="none" rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <gs>
               <a:schemeClr val="phClr">
                 <a:tint val="80000"/>
                 <a:satMod val="300000"/>
               </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
+            </gs>
+            <gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
-            </a:gs>
+            </gs>
           </a:gsLst>
           <a:path path="circle">
             <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
       </a:bgFillStyleLst>
+      <a:lnStyleLst/>
+      <a:effectStyleLst/>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults>
@@ -1208,24 +1169,23 @@
           <a:ext cx="1" cy="1"/>
         </a:xfrm>
         <a:custGeom>
+          <a:rect l="0" t="0" r="0" b="0"/>
           <a:avLst/>
           <a:gdLst/>
-          <a:ahLst/>
           <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst/>
         </a:custGeom>
         <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="090000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+          <a:srgbClr val="090000"/>
         </a:solidFill>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="400000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+            <a:srgbClr val="400000"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:round/>
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="none" w="med" len="med"/>
+          <a:headEnd w="med" len="med"/>
+          <a:tailEnd w="med" len="med"/>
         </a:ln>
         <a:effectLst/>
         <a:extLst>
@@ -1240,7 +1200,7 @@
           </a:ext>
         </a:extLst>
       </a:spPr>
-      <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" upright="1"/>
+      <a:bodyPr rot="0" vertOverflow="clip" vert="horz" wrap="square" lIns="18288" rtlCol="0" anchor="t" upright="1"/>
       <a:lstStyle/>
     </a:spDef>
     <a:lnDef>
@@ -1250,24 +1210,23 @@
           <a:ext cx="1" cy="1"/>
         </a:xfrm>
         <a:custGeom>
+          <a:rect l="0" t="0" r="0" b="0"/>
           <a:avLst/>
           <a:gdLst/>
-          <a:ahLst/>
           <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst/>
         </a:custGeom>
         <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="090000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+          <a:srgbClr val="090000"/>
         </a:solidFill>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="400000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+            <a:srgbClr val="400000"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:round/>
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="none" w="med" len="med"/>
+          <a:headEnd w="med" len="med"/>
+          <a:tailEnd w="med" len="med"/>
         </a:ln>
         <a:effectLst/>
         <a:extLst>
@@ -1282,7 +1241,7 @@
           </a:ext>
         </a:extLst>
       </a:spPr>
-      <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" upright="1"/>
+      <a:bodyPr rot="0" vertOverflow="clip" vert="horz" wrap="square" lIns="18288" rtlCol="0" anchor="t" upright="1"/>
       <a:lstStyle/>
     </a:lnDef>
   </a:objectDefaults>
@@ -1382,10 +1341,18 @@
       <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="G4"/>
-      <c r="H4"/>
-      <c r="I4"/>
-      <c r="J4"/>
+      <c r="G4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" t="s">
+        <v>42</v>
+      </c>
       <c r="L4" s="4" t="s">
         <v>9</v>
       </c>
@@ -1418,10 +1385,18 @@
       <c r="F5" t="s">
         <v>17</v>
       </c>
-      <c r="G5"/>
-      <c r="H5"/>
-      <c r="I5"/>
-      <c r="J5"/>
+      <c r="G5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" t="s">
+        <v>42</v>
+      </c>
       <c r="L5" s="7" t="s">
         <v>1</v>
       </c>
@@ -1452,10 +1427,18 @@
       <c r="F6" t="s">
         <v>17</v>
       </c>
-      <c r="G6"/>
-      <c r="H6"/>
-      <c r="I6"/>
-      <c r="J6"/>
+      <c r="G6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" t="s">
+        <v>42</v>
+      </c>
       <c r="L6" s="7" t="s">
         <v>2</v>
       </c>
@@ -1601,6 +1584,40 @@
         <v>36</v>
       </c>
     </row>
+    <row r="4">
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Created configure template for TIME mode.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="60">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -162,6 +162,39 @@
   </si>
   <si>
     <t xml:space="preserve">FREQUENCY MEASUREMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIME INTERVAL/MODE: INDEPENDENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INPUT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLOSK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TI SETUP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SESSION SETUP</t>
   </si>
 </sst>
 </file>
@@ -1618,6 +1651,91 @@
         <v>48</v>
       </c>
     </row>
+    <row r="6">
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Created configure template for frequency.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="69">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -195,6 +195,33 @@
   </si>
   <si>
     <t xml:space="preserve">SESSION SETUP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLOck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLOCK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MES SETUP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId12</t>
   </si>
 </sst>
 </file>
@@ -1699,7 +1726,7 @@
         <v>45</v>
       </c>
       <c r="F8" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9">
@@ -1733,6 +1760,91 @@
         <v>45</v>
       </c>
       <c r="F10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added calibration button in menu.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="71">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -222,6 +222,12 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calibration</t>
   </si>
 </sst>
 </file>
@@ -1848,6 +1854,23 @@
         <v>59</v>
       </c>
     </row>
+    <row r="16">
+      <c r="B16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Added scroll wheel for channels in configure time mode.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1672" uniqueCount="82">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -228,6 +228,39 @@
   </si>
   <si>
     <t xml:space="preserve">Calibration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scrollWheel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roboto-Bold.ttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scrollWheelCenter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId18</t>
   </si>
 </sst>
 </file>
@@ -1414,7 +1447,7 @@
         <v>42</v>
       </c>
       <c r="I4" t="s">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="J4" t="s">
         <v>42</v>
@@ -1458,7 +1491,7 @@
         <v>42</v>
       </c>
       <c r="I5" t="s">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="J5" t="s">
         <v>42</v>
@@ -1500,7 +1533,7 @@
         <v>42</v>
       </c>
       <c r="I6" t="s">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="J6" t="s">
         <v>42</v>
@@ -1520,6 +1553,33 @@
       <c r="P6" s="10"/>
     </row>
     <row r="7" spans="2:16">
+      <c r="B7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7">
+        <v>25</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" t="s">
+        <v>80</v>
+      </c>
+      <c r="J7" t="s">
+        <v>42</v>
+      </c>
       <c r="L7" s="7" t="s">
         <v>7</v>
       </c>
@@ -1537,6 +1597,33 @@
       </c>
     </row>
     <row r="8" spans="2:16">
+      <c r="B8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8">
+        <v>35</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" t="s">
+        <v>80</v>
+      </c>
+      <c r="J8" t="s">
+        <v>42</v>
+      </c>
       <c r="L8" s="7" t="s">
         <v>8</v>
       </c>
@@ -1871,6 +1958,91 @@
         <v>70</v>
       </c>
     </row>
+    <row r="17">
+      <c r="B17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" t="s">
+        <v>45</v>
+      </c>
+      <c r="F21" t="s">
+        <v>75</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Created UI for input panel config in Time mode.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1672" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2692" uniqueCount="93">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -261,6 +261,39 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SLOPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THRESHOLD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Detect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Defined</t>
   </si>
 </sst>
 </file>
@@ -2043,6 +2076,108 @@
         <v>75</v>
       </c>
     </row>
+    <row r="22">
+      <c r="B22" t="s">
+        <v>82</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" t="s">
+        <v>45</v>
+      </c>
+      <c r="F23" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="s">
+        <v>86</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="s">
+        <v>88</v>
+      </c>
+      <c r="C25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" t="s">
+        <v>44</v>
+      </c>
+      <c r="E25" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" t="s">
+        <v>45</v>
+      </c>
+      <c r="F26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" t="s">
+        <v>45</v>
+      </c>
+      <c r="F27" t="s">
+        <v>92</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Added toggle button functionality.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2882" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3470" uniqueCount="97">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -300,6 +300,12 @@
   </si>
   <si>
     <t xml:space="preserve">100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Text&lt;value&gt;</t>
   </si>
 </sst>
 </file>
@@ -2201,6 +2207,23 @@
         <v>94</v>
       </c>
     </row>
+    <row r="29">
+      <c r="B29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" t="s">
+        <v>44</v>
+      </c>
+      <c r="E29" t="s">
+        <v>45</v>
+      </c>
+      <c r="F29" t="s">
+        <v>96</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Finished create INPUT panel configure for Time mode.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4094" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6518" uniqueCount="122">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -321,6 +321,83 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internal
+Quartz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internal
+Quartz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internal
+Quartz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internal
+Quartz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internal
+Rubid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">External</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internal
+Quartz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internal
+Rubid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internal
+Quartz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internal
+Rubid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internal
+Quartz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internal
+Rubid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt; mV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internal
+Quartz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internal
+Rubid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internal
+Quartz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internal
+Rubid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internal
+Quartz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Internal
+Rubid</t>
   </si>
 </sst>
 </file>
@@ -2168,7 +2245,7 @@
         <v>45</v>
       </c>
       <c r="F25" t="s">
-        <v>75</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26">
@@ -2219,7 +2296,7 @@
         <v>45</v>
       </c>
       <c r="F28" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
     </row>
     <row r="29">
@@ -2236,7 +2313,7 @@
         <v>45</v>
       </c>
       <c r="F29" t="s">
-        <v>96</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30">
@@ -2253,7 +2330,7 @@
         <v>45</v>
       </c>
       <c r="F30" t="s">
-        <v>98</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31">
@@ -2264,49 +2341,17 @@
         <v>38</v>
       </c>
       <c r="D31" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E31" t="s">
         <v>45</v>
       </c>
       <c r="F31" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="B32" t="s">
-        <v>100</v>
-      </c>
-      <c r="C32" t="s">
-        <v>38</v>
-      </c>
-      <c r="D32" t="s">
-        <v>44</v>
-      </c>
-      <c r="E32" t="s">
-        <v>45</v>
-      </c>
-      <c r="F32" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="B33" t="s">
-        <v>101</v>
-      </c>
-      <c r="C33" t="s">
-        <v>38</v>
-      </c>
-      <c r="D33" t="s">
-        <v>44</v>
-      </c>
-      <c r="E33" t="s">
-        <v>45</v>
-      </c>
-      <c r="F33" t="s">
-        <v>98</v>
-      </c>
-    </row>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32"/>
+    <row r="33"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Created clock panel config and scroll wheel for Ti setup panel.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6518" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7160" uniqueCount="123">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -398,6 +398,9 @@
   <si>
     <t xml:space="preserve">Internal
 Rubid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a-z,A-Z,0-9</t>
   </si>
 </sst>
 </file>
@@ -1584,7 +1587,7 @@
         <v>42</v>
       </c>
       <c r="I4" t="s">
-        <v>80</v>
+        <v>122</v>
       </c>
       <c r="J4" t="s">
         <v>42</v>
@@ -1628,7 +1631,7 @@
         <v>42</v>
       </c>
       <c r="I5" t="s">
-        <v>80</v>
+        <v>122</v>
       </c>
       <c r="J5" t="s">
         <v>42</v>
@@ -1670,7 +1673,7 @@
         <v>42</v>
       </c>
       <c r="I6" t="s">
-        <v>80</v>
+        <v>122</v>
       </c>
       <c r="J6" t="s">
         <v>42</v>
@@ -1712,7 +1715,7 @@
         <v>42</v>
       </c>
       <c r="I7" t="s">
-        <v>80</v>
+        <v>122</v>
       </c>
       <c r="J7" t="s">
         <v>42</v>
@@ -1756,7 +1759,7 @@
         <v>42</v>
       </c>
       <c r="I8" t="s">
-        <v>80</v>
+        <v>122</v>
       </c>
       <c r="J8" t="s">
         <v>42</v>
@@ -2313,7 +2316,7 @@
         <v>45</v>
       </c>
       <c r="F29" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30">
@@ -2330,7 +2333,7 @@
         <v>45</v>
       </c>
       <c r="F30" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31">
@@ -2350,7 +2353,23 @@
         <v>108</v>
       </c>
     </row>
-    <row r="32"/>
+    <row r="32">
+      <c r="B32" t="s">
+        <v>100</v>
+      </c>
+      <c r="C32" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" t="s">
+        <v>44</v>
+      </c>
+      <c r="E32" t="s">
+        <v>45</v>
+      </c>
+      <c r="F32" t="s">
+        <v>75</v>
+      </c>
+    </row>
     <row r="33"/>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Added info about state channel in Ti setup panel.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7160" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8094" uniqueCount="130">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -401,6 +401,27 @@
   </si>
   <si>
     <t xml:space="preserve">a-z,A-Z,0-9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">START - IN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STOP - IN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OFF</t>
   </si>
 </sst>
 </file>
@@ -2370,7 +2391,74 @@
         <v>75</v>
       </c>
     </row>
-    <row r="33"/>
+    <row r="33">
+      <c r="B33" t="s">
+        <v>101</v>
+      </c>
+      <c r="C33" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33" t="s">
+        <v>50</v>
+      </c>
+      <c r="E33" t="s">
+        <v>45</v>
+      </c>
+      <c r="F33" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="s">
+        <v>124</v>
+      </c>
+      <c r="C34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" t="s">
+        <v>50</v>
+      </c>
+      <c r="E34" t="s">
+        <v>45</v>
+      </c>
+      <c r="F34" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="s">
+        <v>126</v>
+      </c>
+      <c r="C35" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" t="s">
+        <v>44</v>
+      </c>
+      <c r="E35" t="s">
+        <v>45</v>
+      </c>
+      <c r="F35" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="s">
+        <v>127</v>
+      </c>
+      <c r="C36" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" t="s">
+        <v>44</v>
+      </c>
+      <c r="E36" t="s">
+        <v>45</v>
+      </c>
+      <c r="F36" t="s">
+        <v>129</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Added scroll wheel for start in selection.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8094" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8588" uniqueCount="132">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -422,6 +422,12 @@
   </si>
   <si>
     <t xml:space="preserve">OFF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId35</t>
   </si>
 </sst>
 </file>
@@ -2459,6 +2465,40 @@
         <v>129</v>
       </c>
     </row>
+    <row r="37">
+      <c r="B37" t="s">
+        <v>130</v>
+      </c>
+      <c r="C37" t="s">
+        <v>38</v>
+      </c>
+      <c r="D37" t="s">
+        <v>44</v>
+      </c>
+      <c r="E37" t="s">
+        <v>45</v>
+      </c>
+      <c r="F37" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" t="s">
+        <v>131</v>
+      </c>
+      <c r="C38" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" t="s">
+        <v>44</v>
+      </c>
+      <c r="E38" t="s">
+        <v>45</v>
+      </c>
+      <c r="F38" t="s">
+        <v>75</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Created UI for session setup panel config for Time mode interval.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8588" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11258" uniqueCount="159">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -428,6 +428,89 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TI MAX RANGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stamps Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meas Rate
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meas Rate
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meas Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt; ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Continuous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Repeat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt; s</t>
   </si>
 </sst>
 </file>
@@ -2499,6 +2582,261 @@
         <v>75</v>
       </c>
     </row>
+    <row r="39">
+      <c r="B39" t="s">
+        <v>132</v>
+      </c>
+      <c r="C39" t="s">
+        <v>38</v>
+      </c>
+      <c r="D39" t="s">
+        <v>50</v>
+      </c>
+      <c r="E39" t="s">
+        <v>45</v>
+      </c>
+      <c r="F39" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="B40" t="s">
+        <v>134</v>
+      </c>
+      <c r="C40" t="s">
+        <v>38</v>
+      </c>
+      <c r="D40" t="s">
+        <v>44</v>
+      </c>
+      <c r="E40" t="s">
+        <v>45</v>
+      </c>
+      <c r="F40" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="B41" t="s">
+        <v>138</v>
+      </c>
+      <c r="C41" t="s">
+        <v>38</v>
+      </c>
+      <c r="D41" t="s">
+        <v>50</v>
+      </c>
+      <c r="E41" t="s">
+        <v>45</v>
+      </c>
+      <c r="F41" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="B42" t="s">
+        <v>142</v>
+      </c>
+      <c r="C42" t="s">
+        <v>38</v>
+      </c>
+      <c r="D42" t="s">
+        <v>44</v>
+      </c>
+      <c r="E42" t="s">
+        <v>45</v>
+      </c>
+      <c r="F42" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="B43" t="s">
+        <v>144</v>
+      </c>
+      <c r="C43" t="s">
+        <v>38</v>
+      </c>
+      <c r="D43" t="s">
+        <v>44</v>
+      </c>
+      <c r="E43" t="s">
+        <v>45</v>
+      </c>
+      <c r="F43" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="B44" t="s">
+        <v>146</v>
+      </c>
+      <c r="C44" t="s">
+        <v>38</v>
+      </c>
+      <c r="D44" t="s">
+        <v>44</v>
+      </c>
+      <c r="E44" t="s">
+        <v>45</v>
+      </c>
+      <c r="F44" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="B45" t="s">
+        <v>147</v>
+      </c>
+      <c r="C45" t="s">
+        <v>38</v>
+      </c>
+      <c r="D45" t="s">
+        <v>50</v>
+      </c>
+      <c r="E45" t="s">
+        <v>45</v>
+      </c>
+      <c r="F45" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="B46" t="s">
+        <v>148</v>
+      </c>
+      <c r="C46" t="s">
+        <v>38</v>
+      </c>
+      <c r="D46" t="s">
+        <v>50</v>
+      </c>
+      <c r="E46" t="s">
+        <v>45</v>
+      </c>
+      <c r="F46" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="B47" t="s">
+        <v>149</v>
+      </c>
+      <c r="C47" t="s">
+        <v>38</v>
+      </c>
+      <c r="D47" t="s">
+        <v>50</v>
+      </c>
+      <c r="E47" t="s">
+        <v>45</v>
+      </c>
+      <c r="F47" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="B48" t="s">
+        <v>150</v>
+      </c>
+      <c r="C48" t="s">
+        <v>40</v>
+      </c>
+      <c r="D48" t="s">
+        <v>50</v>
+      </c>
+      <c r="E48" t="s">
+        <v>45</v>
+      </c>
+      <c r="F48" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="B49" t="s">
+        <v>152</v>
+      </c>
+      <c r="C49" t="s">
+        <v>38</v>
+      </c>
+      <c r="D49" t="s">
+        <v>50</v>
+      </c>
+      <c r="E49" t="s">
+        <v>45</v>
+      </c>
+      <c r="F49" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="B50" t="s">
+        <v>154</v>
+      </c>
+      <c r="C50" t="s">
+        <v>38</v>
+      </c>
+      <c r="D50" t="s">
+        <v>44</v>
+      </c>
+      <c r="E50" t="s">
+        <v>45</v>
+      </c>
+      <c r="F50" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="B51" t="s">
+        <v>155</v>
+      </c>
+      <c r="C51" t="s">
+        <v>38</v>
+      </c>
+      <c r="D51" t="s">
+        <v>50</v>
+      </c>
+      <c r="E51" t="s">
+        <v>45</v>
+      </c>
+      <c r="F51" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="B52" t="s">
+        <v>156</v>
+      </c>
+      <c r="C52" t="s">
+        <v>38</v>
+      </c>
+      <c r="D52" t="s">
+        <v>44</v>
+      </c>
+      <c r="E52" t="s">
+        <v>45</v>
+      </c>
+      <c r="F52" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="B53" t="s">
+        <v>157</v>
+      </c>
+      <c r="C53" t="s">
+        <v>38</v>
+      </c>
+      <c r="D53" t="s">
+        <v>50</v>
+      </c>
+      <c r="E53" t="s">
+        <v>45</v>
+      </c>
+      <c r="F53" t="s">
+        <v>102</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Added function declaration for toogle and radio buttons.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11258" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11598" uniqueCount="161">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -511,6 +511,12 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;value&gt; s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId53</t>
   </si>
 </sst>
 </file>
@@ -2601,41 +2607,41 @@
     </row>
     <row r="40">
       <c r="B40" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C40" t="s">
         <v>38</v>
       </c>
       <c r="D40" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E40" t="s">
         <v>45</v>
       </c>
       <c r="F40" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C41" t="s">
         <v>38</v>
       </c>
       <c r="D41" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E41" t="s">
         <v>45</v>
       </c>
       <c r="F41" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="C42" t="s">
         <v>38</v>
@@ -2647,46 +2653,46 @@
         <v>45</v>
       </c>
       <c r="F42" t="s">
-        <v>143</v>
+        <v>75</v>
       </c>
     </row>
     <row r="43">
       <c r="B43" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="C43" t="s">
         <v>38</v>
       </c>
       <c r="D43" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E43" t="s">
         <v>45</v>
       </c>
       <c r="F43" t="s">
-        <v>145</v>
+        <v>102</v>
       </c>
     </row>
     <row r="44">
       <c r="B44" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C44" t="s">
         <v>38</v>
       </c>
       <c r="D44" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E44" t="s">
         <v>45</v>
       </c>
       <c r="F44" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
     </row>
     <row r="45">
       <c r="B45" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C45" t="s">
         <v>38</v>
@@ -2698,15 +2704,15 @@
         <v>45</v>
       </c>
       <c r="F45" t="s">
-        <v>102</v>
+        <v>137</v>
       </c>
     </row>
     <row r="46">
       <c r="B46" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C46" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D46" t="s">
         <v>50</v>
@@ -2715,12 +2721,12 @@
         <v>45</v>
       </c>
       <c r="F46" t="s">
-        <v>102</v>
+        <v>151</v>
       </c>
     </row>
     <row r="47">
       <c r="B47" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C47" t="s">
         <v>38</v>
@@ -2732,29 +2738,29 @@
         <v>45</v>
       </c>
       <c r="F47" t="s">
-        <v>137</v>
+        <v>153</v>
       </c>
     </row>
     <row r="48">
       <c r="B48" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="C48" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D48" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E48" t="s">
         <v>45</v>
       </c>
       <c r="F48" t="s">
-        <v>151</v>
+        <v>75</v>
       </c>
     </row>
     <row r="49">
       <c r="B49" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C49" t="s">
         <v>38</v>
@@ -2766,12 +2772,12 @@
         <v>45</v>
       </c>
       <c r="F49" t="s">
-        <v>153</v>
+        <v>102</v>
       </c>
     </row>
     <row r="50">
       <c r="B50" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C50" t="s">
         <v>38</v>
@@ -2783,12 +2789,12 @@
         <v>45</v>
       </c>
       <c r="F50" t="s">
-        <v>75</v>
+        <v>158</v>
       </c>
     </row>
     <row r="51">
       <c r="B51" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C51" t="s">
         <v>38</v>
@@ -2805,24 +2811,24 @@
     </row>
     <row r="52">
       <c r="B52" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C52" t="s">
         <v>38</v>
       </c>
       <c r="D52" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E52" t="s">
         <v>45</v>
       </c>
       <c r="F52" t="s">
-        <v>158</v>
+        <v>135</v>
       </c>
     </row>
     <row r="53">
       <c r="B53" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C53" t="s">
         <v>38</v>
@@ -2834,7 +2840,7 @@
         <v>45</v>
       </c>
       <c r="F53" t="s">
-        <v>102</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added button for finish panel config.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11598" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11944" uniqueCount="163">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -517,6 +517,12 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value from main.c: &lt;value&gt;</t>
   </si>
 </sst>
 </file>
@@ -2843,6 +2849,23 @@
         <v>145</v>
       </c>
     </row>
+    <row r="54">
+      <c r="B54" t="s">
+        <v>161</v>
+      </c>
+      <c r="C54" t="s">
+        <v>38</v>
+      </c>
+      <c r="D54" t="s">
+        <v>50</v>
+      </c>
+      <c r="E54" t="s">
+        <v>45</v>
+      </c>
+      <c r="F54" t="s">
+        <v>162</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Created UI for panel input and clock for Grequency mode.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11944" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12738" uniqueCount="173">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -523,6 +523,36 @@
   </si>
   <si>
     <t xml:space="preserve">Value from main.c: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId64</t>
   </si>
 </sst>
 </file>
@@ -2866,6 +2896,176 @@
         <v>162</v>
       </c>
     </row>
+    <row r="55">
+      <c r="B55" t="s">
+        <v>163</v>
+      </c>
+      <c r="C55" t="s">
+        <v>38</v>
+      </c>
+      <c r="D55" t="s">
+        <v>50</v>
+      </c>
+      <c r="E55" t="s">
+        <v>45</v>
+      </c>
+      <c r="F55" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="B56" t="s">
+        <v>164</v>
+      </c>
+      <c r="C56" t="s">
+        <v>38</v>
+      </c>
+      <c r="D56" t="s">
+        <v>50</v>
+      </c>
+      <c r="E56" t="s">
+        <v>45</v>
+      </c>
+      <c r="F56" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="B57" t="s">
+        <v>165</v>
+      </c>
+      <c r="C57" t="s">
+        <v>38</v>
+      </c>
+      <c r="D57" t="s">
+        <v>44</v>
+      </c>
+      <c r="E57" t="s">
+        <v>45</v>
+      </c>
+      <c r="F57" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="B58" t="s">
+        <v>166</v>
+      </c>
+      <c r="C58" t="s">
+        <v>38</v>
+      </c>
+      <c r="D58" t="s">
+        <v>44</v>
+      </c>
+      <c r="E58" t="s">
+        <v>45</v>
+      </c>
+      <c r="F58" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="B59" t="s">
+        <v>167</v>
+      </c>
+      <c r="C59" t="s">
+        <v>38</v>
+      </c>
+      <c r="D59" t="s">
+        <v>50</v>
+      </c>
+      <c r="E59" t="s">
+        <v>45</v>
+      </c>
+      <c r="F59" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="B60" t="s">
+        <v>168</v>
+      </c>
+      <c r="C60" t="s">
+        <v>38</v>
+      </c>
+      <c r="D60" t="s">
+        <v>50</v>
+      </c>
+      <c r="E60" t="s">
+        <v>45</v>
+      </c>
+      <c r="F60" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="B61" t="s">
+        <v>169</v>
+      </c>
+      <c r="C61" t="s">
+        <v>38</v>
+      </c>
+      <c r="D61" t="s">
+        <v>50</v>
+      </c>
+      <c r="E61" t="s">
+        <v>45</v>
+      </c>
+      <c r="F61" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="B62" t="s">
+        <v>170</v>
+      </c>
+      <c r="C62" t="s">
+        <v>38</v>
+      </c>
+      <c r="D62" t="s">
+        <v>50</v>
+      </c>
+      <c r="E62" t="s">
+        <v>45</v>
+      </c>
+      <c r="F62" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="B63" t="s">
+        <v>171</v>
+      </c>
+      <c r="C63" t="s">
+        <v>38</v>
+      </c>
+      <c r="D63" t="s">
+        <v>44</v>
+      </c>
+      <c r="E63" t="s">
+        <v>45</v>
+      </c>
+      <c r="F63" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="B64" t="s">
+        <v>172</v>
+      </c>
+      <c r="C64" t="s">
+        <v>38</v>
+      </c>
+      <c r="D64" t="s">
+        <v>44</v>
+      </c>
+      <c r="E64" t="s">
+        <v>45</v>
+      </c>
+      <c r="F64" t="s">
+        <v>103</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Support for scroll wheel and channel objects has been added.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12738" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13562" uniqueCount="174">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -553,6 +553,9 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId65</t>
   </si>
 </sst>
 </file>
@@ -2196,7 +2199,7 @@
         <v>45</v>
       </c>
       <c r="F13" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14">
@@ -3064,6 +3067,23 @@
       </c>
       <c r="F64" t="s">
         <v>103</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="B65" t="s">
+        <v>173</v>
+      </c>
+      <c r="C65" t="s">
+        <v>38</v>
+      </c>
+      <c r="D65" t="s">
+        <v>44</v>
+      </c>
+      <c r="E65" t="s">
+        <v>45</v>
+      </c>
+      <c r="F65" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created UI for MES SETUP panel config.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13562" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15300" uniqueCount="182">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -556,6 +556,30 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HF INPUT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId71</t>
   </si>
 </sst>
 </file>
@@ -3086,6 +3110,108 @@
         <v>75</v>
       </c>
     </row>
+    <row r="66">
+      <c r="B66" t="s">
+        <v>174</v>
+      </c>
+      <c r="C66" t="s">
+        <v>38</v>
+      </c>
+      <c r="D66" t="s">
+        <v>50</v>
+      </c>
+      <c r="E66" t="s">
+        <v>45</v>
+      </c>
+      <c r="F66" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="B67" t="s">
+        <v>176</v>
+      </c>
+      <c r="C67" t="s">
+        <v>40</v>
+      </c>
+      <c r="D67" t="s">
+        <v>50</v>
+      </c>
+      <c r="E67" t="s">
+        <v>45</v>
+      </c>
+      <c r="F67" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="B68" t="s">
+        <v>177</v>
+      </c>
+      <c r="C68" t="s">
+        <v>40</v>
+      </c>
+      <c r="D68" t="s">
+        <v>50</v>
+      </c>
+      <c r="E68" t="s">
+        <v>45</v>
+      </c>
+      <c r="F68" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="B69" t="s">
+        <v>178</v>
+      </c>
+      <c r="C69" t="s">
+        <v>38</v>
+      </c>
+      <c r="D69" t="s">
+        <v>50</v>
+      </c>
+      <c r="E69" t="s">
+        <v>45</v>
+      </c>
+      <c r="F69" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="B70" t="s">
+        <v>180</v>
+      </c>
+      <c r="C70" t="s">
+        <v>38</v>
+      </c>
+      <c r="D70" t="s">
+        <v>44</v>
+      </c>
+      <c r="E70" t="s">
+        <v>45</v>
+      </c>
+      <c r="F70" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="B71" t="s">
+        <v>181</v>
+      </c>
+      <c r="C71" t="s">
+        <v>38</v>
+      </c>
+      <c r="D71" t="s">
+        <v>50</v>
+      </c>
+      <c r="E71" t="s">
+        <v>45</v>
+      </c>
+      <c r="F71" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Created UI for sessionsetup panel config and added template functions for this.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15300" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15820" uniqueCount="194">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -580,6 +580,42 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId74</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId76</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId77</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId81</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId82</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId83</t>
   </si>
 </sst>
 </file>
@@ -3212,6 +3248,210 @@
         <v>67</v>
       </c>
     </row>
+    <row r="72">
+      <c r="B72" t="s">
+        <v>182</v>
+      </c>
+      <c r="C72" t="s">
+        <v>38</v>
+      </c>
+      <c r="D72" t="s">
+        <v>50</v>
+      </c>
+      <c r="E72" t="s">
+        <v>45</v>
+      </c>
+      <c r="F72" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="B73" t="s">
+        <v>183</v>
+      </c>
+      <c r="C73" t="s">
+        <v>38</v>
+      </c>
+      <c r="D73" t="s">
+        <v>44</v>
+      </c>
+      <c r="E73" t="s">
+        <v>45</v>
+      </c>
+      <c r="F73" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="B74" t="s">
+        <v>184</v>
+      </c>
+      <c r="C74" t="s">
+        <v>38</v>
+      </c>
+      <c r="D74" t="s">
+        <v>50</v>
+      </c>
+      <c r="E74" t="s">
+        <v>45</v>
+      </c>
+      <c r="F74" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="B75" t="s">
+        <v>185</v>
+      </c>
+      <c r="C75" t="s">
+        <v>38</v>
+      </c>
+      <c r="D75" t="s">
+        <v>50</v>
+      </c>
+      <c r="E75" t="s">
+        <v>45</v>
+      </c>
+      <c r="F75" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="B76" t="s">
+        <v>186</v>
+      </c>
+      <c r="C76" t="s">
+        <v>40</v>
+      </c>
+      <c r="D76" t="s">
+        <v>50</v>
+      </c>
+      <c r="E76" t="s">
+        <v>45</v>
+      </c>
+      <c r="F76" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="B77" t="s">
+        <v>187</v>
+      </c>
+      <c r="C77" t="s">
+        <v>38</v>
+      </c>
+      <c r="D77" t="s">
+        <v>50</v>
+      </c>
+      <c r="E77" t="s">
+        <v>45</v>
+      </c>
+      <c r="F77" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="B78" t="s">
+        <v>188</v>
+      </c>
+      <c r="C78" t="s">
+        <v>38</v>
+      </c>
+      <c r="D78" t="s">
+        <v>44</v>
+      </c>
+      <c r="E78" t="s">
+        <v>45</v>
+      </c>
+      <c r="F78" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="B79" t="s">
+        <v>189</v>
+      </c>
+      <c r="C79" t="s">
+        <v>38</v>
+      </c>
+      <c r="D79" t="s">
+        <v>50</v>
+      </c>
+      <c r="E79" t="s">
+        <v>45</v>
+      </c>
+      <c r="F79" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="B80" t="s">
+        <v>190</v>
+      </c>
+      <c r="C80" t="s">
+        <v>38</v>
+      </c>
+      <c r="D80" t="s">
+        <v>44</v>
+      </c>
+      <c r="E80" t="s">
+        <v>45</v>
+      </c>
+      <c r="F80" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="B81" t="s">
+        <v>191</v>
+      </c>
+      <c r="C81" t="s">
+        <v>38</v>
+      </c>
+      <c r="D81" t="s">
+        <v>50</v>
+      </c>
+      <c r="E81" t="s">
+        <v>45</v>
+      </c>
+      <c r="F81" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="B82" t="s">
+        <v>192</v>
+      </c>
+      <c r="C82" t="s">
+        <v>38</v>
+      </c>
+      <c r="D82" t="s">
+        <v>50</v>
+      </c>
+      <c r="E82" t="s">
+        <v>45</v>
+      </c>
+      <c r="F82" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="B83" t="s">
+        <v>193</v>
+      </c>
+      <c r="C83" t="s">
+        <v>38</v>
+      </c>
+      <c r="D83" t="s">
+        <v>50</v>
+      </c>
+      <c r="E83" t="s">
+        <v>45</v>
+      </c>
+      <c r="F83" t="s">
+        <v>145</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Created finished config button.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15820" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16878" uniqueCount="196">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -616,6 +616,12 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId83</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId84</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId85</t>
   </si>
 </sst>
 </file>
@@ -3452,6 +3458,40 @@
         <v>145</v>
       </c>
     </row>
+    <row r="84">
+      <c r="B84" t="s">
+        <v>194</v>
+      </c>
+      <c r="C84" t="s">
+        <v>38</v>
+      </c>
+      <c r="D84" t="s">
+        <v>50</v>
+      </c>
+      <c r="E84" t="s">
+        <v>45</v>
+      </c>
+      <c r="F84" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="B85" t="s">
+        <v>195</v>
+      </c>
+      <c r="C85" t="s">
+        <v>38</v>
+      </c>
+      <c r="D85" t="s">
+        <v>50</v>
+      </c>
+      <c r="E85" t="s">
+        <v>45</v>
+      </c>
+      <c r="F85" t="s">
+        <v>162</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Removed radiobutton from input panel config.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16878" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17906" uniqueCount="196">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2474,7 +2474,7 @@
     </row>
     <row r="26">
       <c r="B26" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C26" t="s">
         <v>38</v>
@@ -2486,63 +2486,63 @@
         <v>45</v>
       </c>
       <c r="F26" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C27" t="s">
         <v>38</v>
       </c>
       <c r="D27" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E27" t="s">
         <v>45</v>
       </c>
       <c r="F27" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C28" t="s">
         <v>38</v>
       </c>
       <c r="D28" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E28" t="s">
         <v>45</v>
       </c>
       <c r="F28" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C29" t="s">
         <v>38</v>
       </c>
       <c r="D29" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E29" t="s">
         <v>45</v>
       </c>
       <c r="F29" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C30" t="s">
         <v>38</v>
@@ -2554,12 +2554,12 @@
         <v>45</v>
       </c>
       <c r="F30" t="s">
-        <v>107</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C31" t="s">
         <v>38</v>
@@ -2571,63 +2571,63 @@
         <v>45</v>
       </c>
       <c r="F31" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="C32" t="s">
         <v>38</v>
       </c>
       <c r="D32" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E32" t="s">
         <v>45</v>
       </c>
       <c r="F32" t="s">
-        <v>75</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
       <c r="C33" t="s">
         <v>38</v>
       </c>
       <c r="D33" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E33" t="s">
         <v>45</v>
       </c>
       <c r="F33" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
     </row>
     <row r="34">
       <c r="B34" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C34" t="s">
         <v>38</v>
       </c>
       <c r="D34" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E34" t="s">
         <v>45</v>
       </c>
       <c r="F34" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="C35" t="s">
         <v>38</v>
@@ -2639,12 +2639,12 @@
         <v>45</v>
       </c>
       <c r="F35" t="s">
-        <v>128</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36">
       <c r="B36" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C36" t="s">
         <v>38</v>
@@ -2656,114 +2656,114 @@
         <v>45</v>
       </c>
       <c r="F36" t="s">
-        <v>129</v>
+        <v>75</v>
       </c>
     </row>
     <row r="37">
       <c r="B37" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C37" t="s">
         <v>38</v>
       </c>
       <c r="D37" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E37" t="s">
         <v>45</v>
       </c>
       <c r="F37" t="s">
-        <v>75</v>
+        <v>133</v>
       </c>
     </row>
     <row r="38">
       <c r="B38" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="C38" t="s">
         <v>38</v>
       </c>
       <c r="D38" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E38" t="s">
         <v>45</v>
       </c>
       <c r="F38" t="s">
-        <v>75</v>
+        <v>141</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="C39" t="s">
         <v>38</v>
       </c>
       <c r="D39" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E39" t="s">
         <v>45</v>
       </c>
       <c r="F39" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="C40" t="s">
         <v>38</v>
       </c>
       <c r="D40" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E40" t="s">
         <v>45</v>
       </c>
       <c r="F40" t="s">
-        <v>141</v>
+        <v>75</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="C41" t="s">
         <v>38</v>
       </c>
       <c r="D41" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E41" t="s">
         <v>45</v>
       </c>
       <c r="F41" t="s">
-        <v>143</v>
+        <v>102</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C42" t="s">
         <v>38</v>
       </c>
       <c r="D42" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E42" t="s">
         <v>45</v>
       </c>
       <c r="F42" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
     </row>
     <row r="43">
       <c r="B43" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C43" t="s">
         <v>38</v>
@@ -2775,15 +2775,15 @@
         <v>45</v>
       </c>
       <c r="F43" t="s">
-        <v>102</v>
+        <v>137</v>
       </c>
     </row>
     <row r="44">
       <c r="B44" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C44" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D44" t="s">
         <v>50</v>
@@ -2792,12 +2792,12 @@
         <v>45</v>
       </c>
       <c r="F44" t="s">
-        <v>102</v>
+        <v>151</v>
       </c>
     </row>
     <row r="45">
       <c r="B45" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C45" t="s">
         <v>38</v>
@@ -2809,29 +2809,29 @@
         <v>45</v>
       </c>
       <c r="F45" t="s">
-        <v>137</v>
+        <v>153</v>
       </c>
     </row>
     <row r="46">
       <c r="B46" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="C46" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D46" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E46" t="s">
         <v>45</v>
       </c>
       <c r="F46" t="s">
-        <v>151</v>
+        <v>75</v>
       </c>
     </row>
     <row r="47">
       <c r="B47" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="C47" t="s">
         <v>38</v>
@@ -2843,12 +2843,12 @@
         <v>45</v>
       </c>
       <c r="F47" t="s">
-        <v>153</v>
+        <v>102</v>
       </c>
     </row>
     <row r="48">
       <c r="B48" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C48" t="s">
         <v>38</v>
@@ -2860,12 +2860,12 @@
         <v>45</v>
       </c>
       <c r="F48" t="s">
-        <v>75</v>
+        <v>158</v>
       </c>
     </row>
     <row r="49">
       <c r="B49" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C49" t="s">
         <v>38</v>
@@ -2882,24 +2882,24 @@
     </row>
     <row r="50">
       <c r="B50" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="C50" t="s">
         <v>38</v>
       </c>
       <c r="D50" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E50" t="s">
         <v>45</v>
       </c>
       <c r="F50" t="s">
-        <v>158</v>
+        <v>135</v>
       </c>
     </row>
     <row r="51">
       <c r="B51" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C51" t="s">
         <v>38</v>
@@ -2911,12 +2911,12 @@
         <v>45</v>
       </c>
       <c r="F51" t="s">
-        <v>102</v>
+        <v>145</v>
       </c>
     </row>
     <row r="52">
       <c r="B52" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C52" t="s">
         <v>38</v>
@@ -2928,12 +2928,12 @@
         <v>45</v>
       </c>
       <c r="F52" t="s">
-        <v>135</v>
+        <v>162</v>
       </c>
     </row>
     <row r="53">
       <c r="B53" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C53" t="s">
         <v>38</v>
@@ -2945,12 +2945,12 @@
         <v>45</v>
       </c>
       <c r="F53" t="s">
-        <v>145</v>
+        <v>85</v>
       </c>
     </row>
     <row r="54">
       <c r="B54" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C54" t="s">
         <v>38</v>
@@ -2962,131 +2962,131 @@
         <v>45</v>
       </c>
       <c r="F54" t="s">
-        <v>162</v>
+        <v>83</v>
       </c>
     </row>
     <row r="55">
       <c r="B55" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C55" t="s">
         <v>38</v>
       </c>
       <c r="D55" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E55" t="s">
         <v>45</v>
       </c>
       <c r="F55" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="56">
       <c r="B56" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C56" t="s">
         <v>38</v>
       </c>
       <c r="D56" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E56" t="s">
         <v>45</v>
       </c>
       <c r="F56" t="s">
-        <v>83</v>
+        <v>115</v>
       </c>
     </row>
     <row r="57">
       <c r="B57" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C57" t="s">
         <v>38</v>
       </c>
       <c r="D57" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E57" t="s">
         <v>45</v>
       </c>
       <c r="F57" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
     </row>
     <row r="58">
       <c r="B58" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C58" t="s">
         <v>38</v>
       </c>
       <c r="D58" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E58" t="s">
         <v>45</v>
       </c>
       <c r="F58" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="59">
       <c r="B59" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C59" t="s">
         <v>38</v>
       </c>
       <c r="D59" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E59" t="s">
         <v>45</v>
       </c>
       <c r="F59" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
     </row>
     <row r="60">
       <c r="B60" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="C60" t="s">
         <v>38</v>
       </c>
       <c r="D60" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E60" t="s">
         <v>45</v>
       </c>
       <c r="F60" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
     </row>
     <row r="61">
       <c r="B61" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="C61" t="s">
         <v>38</v>
       </c>
       <c r="D61" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E61" t="s">
         <v>45</v>
       </c>
       <c r="F61" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
     </row>
     <row r="62">
       <c r="B62" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C62" t="s">
         <v>38</v>
@@ -3098,83 +3098,83 @@
         <v>45</v>
       </c>
       <c r="F62" t="s">
-        <v>108</v>
+        <v>175</v>
       </c>
     </row>
     <row r="63">
       <c r="B63" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="C63" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D63" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E63" t="s">
         <v>45</v>
       </c>
       <c r="F63" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
     </row>
     <row r="64">
       <c r="B64" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="C64" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D64" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E64" t="s">
         <v>45</v>
       </c>
       <c r="F64" t="s">
-        <v>103</v>
+        <v>129</v>
       </c>
     </row>
     <row r="65">
       <c r="B65" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="C65" t="s">
         <v>38</v>
       </c>
       <c r="D65" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E65" t="s">
         <v>45</v>
       </c>
       <c r="F65" t="s">
-        <v>75</v>
+        <v>179</v>
       </c>
     </row>
     <row r="66">
       <c r="B66" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="C66" t="s">
         <v>38</v>
       </c>
       <c r="D66" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E66" t="s">
         <v>45</v>
       </c>
       <c r="F66" t="s">
-        <v>175</v>
+        <v>143</v>
       </c>
     </row>
     <row r="67">
       <c r="B67" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="C67" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D67" t="s">
         <v>50</v>
@@ -3183,15 +3183,15 @@
         <v>45</v>
       </c>
       <c r="F67" t="s">
-        <v>128</v>
+        <v>67</v>
       </c>
     </row>
     <row r="68">
       <c r="B68" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="C68" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D68" t="s">
         <v>50</v>
@@ -3200,46 +3200,46 @@
         <v>45</v>
       </c>
       <c r="F68" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
     </row>
     <row r="69">
       <c r="B69" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C69" t="s">
         <v>38</v>
       </c>
       <c r="D69" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E69" t="s">
         <v>45</v>
       </c>
       <c r="F69" t="s">
-        <v>179</v>
+        <v>75</v>
       </c>
     </row>
     <row r="70">
       <c r="B70" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="C70" t="s">
         <v>38</v>
       </c>
       <c r="D70" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E70" t="s">
         <v>45</v>
       </c>
       <c r="F70" t="s">
-        <v>143</v>
+        <v>102</v>
       </c>
     </row>
     <row r="71">
       <c r="B71" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="C71" t="s">
         <v>38</v>
@@ -3251,15 +3251,15 @@
         <v>45</v>
       </c>
       <c r="F71" t="s">
-        <v>67</v>
+        <v>137</v>
       </c>
     </row>
     <row r="72">
       <c r="B72" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="C72" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D72" t="s">
         <v>50</v>
@@ -3268,46 +3268,46 @@
         <v>45</v>
       </c>
       <c r="F72" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
     </row>
     <row r="73">
       <c r="B73" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="C73" t="s">
         <v>38</v>
       </c>
       <c r="D73" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E73" t="s">
         <v>45</v>
       </c>
       <c r="F73" t="s">
-        <v>75</v>
+        <v>153</v>
       </c>
     </row>
     <row r="74">
       <c r="B74" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="C74" t="s">
         <v>38</v>
       </c>
       <c r="D74" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E74" t="s">
         <v>45</v>
       </c>
       <c r="F74" t="s">
-        <v>102</v>
+        <v>75</v>
       </c>
     </row>
     <row r="75">
       <c r="B75" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="C75" t="s">
         <v>38</v>
@@ -3319,29 +3319,29 @@
         <v>45</v>
       </c>
       <c r="F75" t="s">
-        <v>137</v>
+        <v>102</v>
       </c>
     </row>
     <row r="76">
       <c r="B76" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="C76" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D76" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E76" t="s">
         <v>45</v>
       </c>
       <c r="F76" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
     </row>
     <row r="77">
       <c r="B77" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="C77" t="s">
         <v>38</v>
@@ -3353,29 +3353,29 @@
         <v>45</v>
       </c>
       <c r="F77" t="s">
-        <v>153</v>
+        <v>102</v>
       </c>
     </row>
     <row r="78">
       <c r="B78" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="C78" t="s">
         <v>38</v>
       </c>
       <c r="D78" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E78" t="s">
         <v>45</v>
       </c>
       <c r="F78" t="s">
-        <v>75</v>
+        <v>135</v>
       </c>
     </row>
     <row r="79">
       <c r="B79" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="C79" t="s">
         <v>38</v>
@@ -3387,29 +3387,29 @@
         <v>45</v>
       </c>
       <c r="F79" t="s">
-        <v>102</v>
+        <v>145</v>
       </c>
     </row>
     <row r="80">
       <c r="B80" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="C80" t="s">
         <v>38</v>
       </c>
       <c r="D80" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E80" t="s">
         <v>45</v>
       </c>
       <c r="F80" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
     </row>
     <row r="81">
       <c r="B81" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="C81" t="s">
         <v>38</v>
@@ -3421,77 +3421,13 @@
         <v>45</v>
       </c>
       <c r="F81" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="B82" t="s">
-        <v>192</v>
-      </c>
-      <c r="C82" t="s">
-        <v>38</v>
-      </c>
-      <c r="D82" t="s">
-        <v>50</v>
-      </c>
-      <c r="E82" t="s">
-        <v>45</v>
-      </c>
-      <c r="F82" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="B83" t="s">
-        <v>193</v>
-      </c>
-      <c r="C83" t="s">
-        <v>38</v>
-      </c>
-      <c r="D83" t="s">
-        <v>50</v>
-      </c>
-      <c r="E83" t="s">
-        <v>45</v>
-      </c>
-      <c r="F83" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="B84" t="s">
-        <v>194</v>
-      </c>
-      <c r="C84" t="s">
-        <v>38</v>
-      </c>
-      <c r="D84" t="s">
-        <v>50</v>
-      </c>
-      <c r="E84" t="s">
-        <v>45</v>
-      </c>
-      <c r="F84" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="85">
-      <c r="B85" t="s">
-        <v>195</v>
-      </c>
-      <c r="C85" t="s">
-        <v>38</v>
-      </c>
-      <c r="D85" t="s">
-        <v>50</v>
-      </c>
-      <c r="E85" t="s">
-        <v>45</v>
-      </c>
-      <c r="F85" t="s">
-        <v>162</v>
-      </c>
-    </row>
+    <row r="82"/>
+    <row r="83"/>
+    <row r="84"/>
+    <row r="85"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Developed slider for time session setup.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17906" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19370" uniqueCount="196">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2678,24 +2678,24 @@
     </row>
     <row r="38">
       <c r="B38" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C38" t="s">
         <v>38</v>
       </c>
       <c r="D38" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E38" t="s">
         <v>45</v>
       </c>
       <c r="F38" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="C39" t="s">
         <v>38</v>
@@ -2707,29 +2707,29 @@
         <v>45</v>
       </c>
       <c r="F39" t="s">
-        <v>143</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C40" t="s">
         <v>38</v>
       </c>
       <c r="D40" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E40" t="s">
         <v>45</v>
       </c>
       <c r="F40" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C41" t="s">
         <v>38</v>
@@ -2746,7 +2746,7 @@
     </row>
     <row r="42">
       <c r="B42" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C42" t="s">
         <v>38</v>
@@ -2758,15 +2758,15 @@
         <v>45</v>
       </c>
       <c r="F42" t="s">
-        <v>102</v>
+        <v>137</v>
       </c>
     </row>
     <row r="43">
       <c r="B43" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C43" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D43" t="s">
         <v>50</v>
@@ -2775,15 +2775,15 @@
         <v>45</v>
       </c>
       <c r="F43" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
     </row>
     <row r="44">
       <c r="B44" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C44" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D44" t="s">
         <v>50</v>
@@ -2792,46 +2792,46 @@
         <v>45</v>
       </c>
       <c r="F44" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="45">
       <c r="B45" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C45" t="s">
         <v>38</v>
       </c>
       <c r="D45" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E45" t="s">
         <v>45</v>
       </c>
       <c r="F45" t="s">
-        <v>153</v>
+        <v>75</v>
       </c>
     </row>
     <row r="46">
       <c r="B46" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C46" t="s">
         <v>38</v>
       </c>
       <c r="D46" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E46" t="s">
         <v>45</v>
       </c>
       <c r="F46" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
     </row>
     <row r="47">
       <c r="B47" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C47" t="s">
         <v>38</v>
@@ -2843,29 +2843,29 @@
         <v>45</v>
       </c>
       <c r="F47" t="s">
-        <v>102</v>
+        <v>135</v>
       </c>
     </row>
     <row r="48">
       <c r="B48" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="C48" t="s">
         <v>38</v>
       </c>
       <c r="D48" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E48" t="s">
         <v>45</v>
       </c>
       <c r="F48" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
     </row>
     <row r="49">
       <c r="B49" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C49" t="s">
         <v>38</v>
@@ -2877,12 +2877,12 @@
         <v>45</v>
       </c>
       <c r="F49" t="s">
-        <v>102</v>
+        <v>162</v>
       </c>
     </row>
     <row r="50">
       <c r="B50" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="C50" t="s">
         <v>38</v>
@@ -2894,12 +2894,12 @@
         <v>45</v>
       </c>
       <c r="F50" t="s">
-        <v>135</v>
+        <v>85</v>
       </c>
     </row>
     <row r="51">
       <c r="B51" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C51" t="s">
         <v>38</v>
@@ -2911,46 +2911,46 @@
         <v>45</v>
       </c>
       <c r="F51" t="s">
-        <v>145</v>
+        <v>83</v>
       </c>
     </row>
     <row r="52">
       <c r="B52" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="C52" t="s">
         <v>38</v>
       </c>
       <c r="D52" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E52" t="s">
         <v>45</v>
       </c>
       <c r="F52" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
     </row>
     <row r="53">
       <c r="B53" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C53" t="s">
         <v>38</v>
       </c>
       <c r="D53" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E53" t="s">
         <v>45</v>
       </c>
       <c r="F53" t="s">
-        <v>85</v>
+        <v>115</v>
       </c>
     </row>
     <row r="54">
       <c r="B54" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C54" t="s">
         <v>38</v>
@@ -2962,29 +2962,29 @@
         <v>45</v>
       </c>
       <c r="F54" t="s">
-        <v>83</v>
+        <v>102</v>
       </c>
     </row>
     <row r="55">
       <c r="B55" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="C55" t="s">
         <v>38</v>
       </c>
       <c r="D55" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E55" t="s">
         <v>45</v>
       </c>
       <c r="F55" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="56">
       <c r="B56" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="C56" t="s">
         <v>38</v>
@@ -2996,97 +2996,97 @@
         <v>45</v>
       </c>
       <c r="F56" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="57">
       <c r="B57" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="C57" t="s">
         <v>38</v>
       </c>
       <c r="D57" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E57" t="s">
         <v>45</v>
       </c>
       <c r="F57" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="58">
       <c r="B58" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="C58" t="s">
         <v>38</v>
       </c>
       <c r="D58" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E58" t="s">
         <v>45</v>
       </c>
       <c r="F58" t="s">
-        <v>108</v>
+        <v>75</v>
       </c>
     </row>
     <row r="59">
       <c r="B59" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="C59" t="s">
         <v>38</v>
       </c>
       <c r="D59" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E59" t="s">
         <v>45</v>
       </c>
       <c r="F59" t="s">
-        <v>107</v>
+        <v>175</v>
       </c>
     </row>
     <row r="60">
       <c r="B60" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="C60" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D60" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E60" t="s">
         <v>45</v>
       </c>
       <c r="F60" t="s">
-        <v>103</v>
+        <v>128</v>
       </c>
     </row>
     <row r="61">
       <c r="B61" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="C61" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D61" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E61" t="s">
         <v>45</v>
       </c>
       <c r="F61" t="s">
-        <v>75</v>
+        <v>129</v>
       </c>
     </row>
     <row r="62">
       <c r="B62" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C62" t="s">
         <v>38</v>
@@ -3098,32 +3098,32 @@
         <v>45</v>
       </c>
       <c r="F62" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="63">
       <c r="B63" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="C63" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D63" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E63" t="s">
         <v>45</v>
       </c>
       <c r="F63" t="s">
-        <v>128</v>
+        <v>143</v>
       </c>
     </row>
     <row r="64">
       <c r="B64" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="C64" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D64" t="s">
         <v>50</v>
@@ -3132,46 +3132,46 @@
         <v>45</v>
       </c>
       <c r="F64" t="s">
-        <v>129</v>
+        <v>67</v>
       </c>
     </row>
     <row r="65">
       <c r="B65" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C65" t="s">
         <v>38</v>
       </c>
       <c r="D65" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E65" t="s">
         <v>45</v>
       </c>
       <c r="F65" t="s">
-        <v>179</v>
+        <v>75</v>
       </c>
     </row>
     <row r="66">
       <c r="B66" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="C66" t="s">
         <v>38</v>
       </c>
       <c r="D66" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E66" t="s">
         <v>45</v>
       </c>
       <c r="F66" t="s">
-        <v>143</v>
+        <v>102</v>
       </c>
     </row>
     <row r="67">
       <c r="B67" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="C67" t="s">
         <v>38</v>
@@ -3183,15 +3183,15 @@
         <v>45</v>
       </c>
       <c r="F67" t="s">
-        <v>67</v>
+        <v>137</v>
       </c>
     </row>
     <row r="68">
       <c r="B68" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="C68" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D68" t="s">
         <v>50</v>
@@ -3200,46 +3200,46 @@
         <v>45</v>
       </c>
       <c r="F68" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
     </row>
     <row r="69">
       <c r="B69" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="C69" t="s">
         <v>38</v>
       </c>
       <c r="D69" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E69" t="s">
         <v>45</v>
       </c>
       <c r="F69" t="s">
-        <v>75</v>
+        <v>153</v>
       </c>
     </row>
     <row r="70">
       <c r="B70" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="C70" t="s">
         <v>38</v>
       </c>
       <c r="D70" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E70" t="s">
         <v>45</v>
       </c>
       <c r="F70" t="s">
-        <v>102</v>
+        <v>75</v>
       </c>
     </row>
     <row r="71">
       <c r="B71" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="C71" t="s">
         <v>38</v>
@@ -3251,15 +3251,15 @@
         <v>45</v>
       </c>
       <c r="F71" t="s">
-        <v>137</v>
+        <v>102</v>
       </c>
     </row>
     <row r="72">
       <c r="B72" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="C72" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D72" t="s">
         <v>50</v>
@@ -3268,12 +3268,12 @@
         <v>45</v>
       </c>
       <c r="F72" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
     </row>
     <row r="73">
       <c r="B73" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="C73" t="s">
         <v>38</v>
@@ -3285,29 +3285,29 @@
         <v>45</v>
       </c>
       <c r="F73" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="74">
       <c r="B74" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="C74" t="s">
         <v>38</v>
       </c>
       <c r="D74" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E74" t="s">
         <v>45</v>
       </c>
       <c r="F74" t="s">
-        <v>75</v>
+        <v>162</v>
       </c>
     </row>
     <row r="75">
       <c r="B75" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="C75" t="s">
         <v>38</v>
@@ -3319,111 +3319,15 @@
         <v>45</v>
       </c>
       <c r="F75" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="B76" t="s">
-        <v>190</v>
-      </c>
-      <c r="C76" t="s">
-        <v>38</v>
-      </c>
-      <c r="D76" t="s">
-        <v>44</v>
-      </c>
-      <c r="E76" t="s">
-        <v>45</v>
-      </c>
-      <c r="F76" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="77">
-      <c r="B77" t="s">
-        <v>191</v>
-      </c>
-      <c r="C77" t="s">
-        <v>38</v>
-      </c>
-      <c r="D77" t="s">
-        <v>50</v>
-      </c>
-      <c r="E77" t="s">
-        <v>45</v>
-      </c>
-      <c r="F77" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="78">
-      <c r="B78" t="s">
-        <v>192</v>
-      </c>
-      <c r="C78" t="s">
-        <v>38</v>
-      </c>
-      <c r="D78" t="s">
-        <v>50</v>
-      </c>
-      <c r="E78" t="s">
-        <v>45</v>
-      </c>
-      <c r="F78" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="B79" t="s">
-        <v>193</v>
-      </c>
-      <c r="C79" t="s">
-        <v>38</v>
-      </c>
-      <c r="D79" t="s">
-        <v>50</v>
-      </c>
-      <c r="E79" t="s">
-        <v>45</v>
-      </c>
-      <c r="F79" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="80">
-      <c r="B80" t="s">
-        <v>194</v>
-      </c>
-      <c r="C80" t="s">
-        <v>38</v>
-      </c>
-      <c r="D80" t="s">
-        <v>50</v>
-      </c>
-      <c r="E80" t="s">
-        <v>45</v>
-      </c>
-      <c r="F80" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="81">
-      <c r="B81" t="s">
-        <v>195</v>
-      </c>
-      <c r="C81" t="s">
-        <v>38</v>
-      </c>
-      <c r="D81" t="s">
-        <v>50</v>
-      </c>
-      <c r="E81" t="s">
-        <v>45</v>
-      </c>
-      <c r="F81" t="s">
-        <v>162</v>
-      </c>
-    </row>
+    <row r="76"/>
+    <row r="77"/>
+    <row r="78"/>
+    <row r="79"/>
+    <row r="80"/>
+    <row r="81"/>
     <row r="82"/>
     <row r="83"/>
     <row r="84"/>

</xml_diff>

<commit_message>
Added new task and semaphore (rename function).
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19370" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19824" uniqueCount="196">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -2865,7 +2865,7 @@
     </row>
     <row r="49">
       <c r="B49" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C49" t="s">
         <v>38</v>
@@ -2877,12 +2877,12 @@
         <v>45</v>
       </c>
       <c r="F49" t="s">
-        <v>162</v>
+        <v>85</v>
       </c>
     </row>
     <row r="50">
       <c r="B50" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C50" t="s">
         <v>38</v>
@@ -2894,29 +2894,29 @@
         <v>45</v>
       </c>
       <c r="F50" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="51">
       <c r="B51" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C51" t="s">
         <v>38</v>
       </c>
       <c r="D51" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E51" t="s">
         <v>45</v>
       </c>
       <c r="F51" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="52">
       <c r="B52" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C52" t="s">
         <v>38</v>
@@ -2928,29 +2928,29 @@
         <v>45</v>
       </c>
       <c r="F52" t="s">
-        <v>87</v>
+        <v>115</v>
       </c>
     </row>
     <row r="53">
       <c r="B53" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C53" t="s">
         <v>38</v>
       </c>
       <c r="D53" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E53" t="s">
         <v>45</v>
       </c>
       <c r="F53" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
     </row>
     <row r="54">
       <c r="B54" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C54" t="s">
         <v>38</v>
@@ -2962,29 +2962,29 @@
         <v>45</v>
       </c>
       <c r="F54" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
     </row>
     <row r="55">
       <c r="B55" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C55" t="s">
         <v>38</v>
       </c>
       <c r="D55" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E55" t="s">
         <v>45</v>
       </c>
       <c r="F55" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="56">
       <c r="B56" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C56" t="s">
         <v>38</v>
@@ -2996,12 +2996,12 @@
         <v>45</v>
       </c>
       <c r="F56" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="57">
       <c r="B57" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C57" t="s">
         <v>38</v>
@@ -3013,32 +3013,32 @@
         <v>45</v>
       </c>
       <c r="F57" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
     </row>
     <row r="58">
       <c r="B58" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C58" t="s">
         <v>38</v>
       </c>
       <c r="D58" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E58" t="s">
         <v>45</v>
       </c>
       <c r="F58" t="s">
-        <v>75</v>
+        <v>175</v>
       </c>
     </row>
     <row r="59">
       <c r="B59" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C59" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D59" t="s">
         <v>50</v>
@@ -3047,12 +3047,12 @@
         <v>45</v>
       </c>
       <c r="F59" t="s">
-        <v>175</v>
+        <v>128</v>
       </c>
     </row>
     <row r="60">
       <c r="B60" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C60" t="s">
         <v>40</v>
@@ -3064,15 +3064,15 @@
         <v>45</v>
       </c>
       <c r="F60" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="61">
       <c r="B61" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C61" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D61" t="s">
         <v>50</v>
@@ -3081,80 +3081,80 @@
         <v>45</v>
       </c>
       <c r="F61" t="s">
-        <v>129</v>
+        <v>179</v>
       </c>
     </row>
     <row r="62">
       <c r="B62" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C62" t="s">
         <v>38</v>
       </c>
       <c r="D62" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E62" t="s">
         <v>45</v>
       </c>
       <c r="F62" t="s">
-        <v>179</v>
+        <v>143</v>
       </c>
     </row>
     <row r="63">
       <c r="B63" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C63" t="s">
         <v>38</v>
       </c>
       <c r="D63" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E63" t="s">
         <v>45</v>
       </c>
       <c r="F63" t="s">
-        <v>143</v>
+        <v>67</v>
       </c>
     </row>
     <row r="64">
       <c r="B64" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C64" t="s">
         <v>38</v>
       </c>
       <c r="D64" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E64" t="s">
         <v>45</v>
       </c>
       <c r="F64" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
     </row>
     <row r="65">
       <c r="B65" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C65" t="s">
         <v>38</v>
       </c>
       <c r="D65" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E65" t="s">
         <v>45</v>
       </c>
       <c r="F65" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
     </row>
     <row r="66">
       <c r="B66" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C66" t="s">
         <v>38</v>
@@ -3166,15 +3166,15 @@
         <v>45</v>
       </c>
       <c r="F66" t="s">
-        <v>102</v>
+        <v>137</v>
       </c>
     </row>
     <row r="67">
       <c r="B67" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C67" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D67" t="s">
         <v>50</v>
@@ -3183,15 +3183,15 @@
         <v>45</v>
       </c>
       <c r="F67" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
     </row>
     <row r="68">
       <c r="B68" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C68" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D68" t="s">
         <v>50</v>
@@ -3200,46 +3200,46 @@
         <v>45</v>
       </c>
       <c r="F68" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="69">
       <c r="B69" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C69" t="s">
         <v>38</v>
       </c>
       <c r="D69" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E69" t="s">
         <v>45</v>
       </c>
       <c r="F69" t="s">
-        <v>153</v>
+        <v>75</v>
       </c>
     </row>
     <row r="70">
       <c r="B70" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C70" t="s">
         <v>38</v>
       </c>
       <c r="D70" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E70" t="s">
         <v>45</v>
       </c>
       <c r="F70" t="s">
-        <v>75</v>
+        <v>102</v>
       </c>
     </row>
     <row r="71">
       <c r="B71" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="C71" t="s">
         <v>38</v>
@@ -3251,12 +3251,12 @@
         <v>45</v>
       </c>
       <c r="F71" t="s">
-        <v>102</v>
+        <v>135</v>
       </c>
     </row>
     <row r="72">
       <c r="B72" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C72" t="s">
         <v>38</v>
@@ -3268,60 +3268,12 @@
         <v>45</v>
       </c>
       <c r="F72" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="B73" t="s">
-        <v>193</v>
-      </c>
-      <c r="C73" t="s">
-        <v>38</v>
-      </c>
-      <c r="D73" t="s">
-        <v>50</v>
-      </c>
-      <c r="E73" t="s">
-        <v>45</v>
-      </c>
-      <c r="F73" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="74">
-      <c r="B74" t="s">
-        <v>194</v>
-      </c>
-      <c r="C74" t="s">
-        <v>38</v>
-      </c>
-      <c r="D74" t="s">
-        <v>50</v>
-      </c>
-      <c r="E74" t="s">
-        <v>45</v>
-      </c>
-      <c r="F74" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="B75" t="s">
-        <v>195</v>
-      </c>
-      <c r="C75" t="s">
-        <v>38</v>
-      </c>
-      <c r="D75" t="s">
-        <v>50</v>
-      </c>
-      <c r="E75" t="s">
-        <v>45</v>
-      </c>
-      <c r="F75" t="s">
-        <v>162</v>
-      </c>
-    </row>
+    <row r="73"/>
+    <row r="74"/>
+    <row r="75"/>
     <row r="76"/>
     <row r="77"/>
     <row r="78"/>

</xml_diff>

<commit_message>
Edited session setup panel for time and frequency config.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19824" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20750" uniqueCount="201">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -622,6 +622,21 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId85</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stamps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId87</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId88</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId89</t>
   </si>
 </sst>
 </file>
@@ -2831,7 +2846,7 @@
     </row>
     <row r="47">
       <c r="B47" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="C47" t="s">
         <v>38</v>
@@ -2843,12 +2858,12 @@
         <v>45</v>
       </c>
       <c r="F47" t="s">
-        <v>135</v>
+        <v>85</v>
       </c>
     </row>
     <row r="48">
       <c r="B48" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="C48" t="s">
         <v>38</v>
@@ -2860,114 +2875,114 @@
         <v>45</v>
       </c>
       <c r="F48" t="s">
-        <v>145</v>
+        <v>83</v>
       </c>
     </row>
     <row r="49">
       <c r="B49" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C49" t="s">
         <v>38</v>
       </c>
       <c r="D49" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E49" t="s">
         <v>45</v>
       </c>
       <c r="F49" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="50">
       <c r="B50" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C50" t="s">
         <v>38</v>
       </c>
       <c r="D50" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E50" t="s">
         <v>45</v>
       </c>
       <c r="F50" t="s">
-        <v>83</v>
+        <v>115</v>
       </c>
     </row>
     <row r="51">
       <c r="B51" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C51" t="s">
         <v>38</v>
       </c>
       <c r="D51" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E51" t="s">
         <v>45</v>
       </c>
       <c r="F51" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
     </row>
     <row r="52">
       <c r="B52" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C52" t="s">
         <v>38</v>
       </c>
       <c r="D52" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E52" t="s">
         <v>45</v>
       </c>
       <c r="F52" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="53">
       <c r="B53" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C53" t="s">
         <v>38</v>
       </c>
       <c r="D53" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E53" t="s">
         <v>45</v>
       </c>
       <c r="F53" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
     </row>
     <row r="54">
       <c r="B54" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C54" t="s">
         <v>38</v>
       </c>
       <c r="D54" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E54" t="s">
         <v>45</v>
       </c>
       <c r="F54" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
     <row r="55">
       <c r="B55" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C55" t="s">
         <v>38</v>
@@ -2979,49 +2994,49 @@
         <v>45</v>
       </c>
       <c r="F55" t="s">
-        <v>107</v>
+        <v>75</v>
       </c>
     </row>
     <row r="56">
       <c r="B56" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C56" t="s">
         <v>38</v>
       </c>
       <c r="D56" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E56" t="s">
         <v>45</v>
       </c>
       <c r="F56" t="s">
-        <v>103</v>
+        <v>175</v>
       </c>
     </row>
     <row r="57">
       <c r="B57" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="C57" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D57" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E57" t="s">
         <v>45</v>
       </c>
       <c r="F57" t="s">
-        <v>75</v>
+        <v>128</v>
       </c>
     </row>
     <row r="58">
       <c r="B58" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C58" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D58" t="s">
         <v>50</v>
@@ -3030,15 +3045,15 @@
         <v>45</v>
       </c>
       <c r="F58" t="s">
-        <v>175</v>
+        <v>129</v>
       </c>
     </row>
     <row r="59">
       <c r="B59" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C59" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D59" t="s">
         <v>50</v>
@@ -3047,29 +3062,29 @@
         <v>45</v>
       </c>
       <c r="F59" t="s">
-        <v>128</v>
+        <v>179</v>
       </c>
     </row>
     <row r="60">
       <c r="B60" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C60" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D60" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E60" t="s">
         <v>45</v>
       </c>
       <c r="F60" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
     </row>
     <row r="61">
       <c r="B61" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="C61" t="s">
         <v>38</v>
@@ -3081,12 +3096,12 @@
         <v>45</v>
       </c>
       <c r="F61" t="s">
-        <v>179</v>
+        <v>67</v>
       </c>
     </row>
     <row r="62">
       <c r="B62" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="C62" t="s">
         <v>38</v>
@@ -3098,12 +3113,12 @@
         <v>45</v>
       </c>
       <c r="F62" t="s">
-        <v>143</v>
+        <v>75</v>
       </c>
     </row>
     <row r="63">
       <c r="B63" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C63" t="s">
         <v>38</v>
@@ -3115,32 +3130,32 @@
         <v>45</v>
       </c>
       <c r="F63" t="s">
-        <v>67</v>
+        <v>102</v>
       </c>
     </row>
     <row r="64">
       <c r="B64" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C64" t="s">
         <v>38</v>
       </c>
       <c r="D64" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E64" t="s">
         <v>45</v>
       </c>
       <c r="F64" t="s">
-        <v>75</v>
+        <v>137</v>
       </c>
     </row>
     <row r="65">
       <c r="B65" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C65" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D65" t="s">
         <v>50</v>
@@ -3149,12 +3164,12 @@
         <v>45</v>
       </c>
       <c r="F65" t="s">
-        <v>102</v>
+        <v>151</v>
       </c>
     </row>
     <row r="66">
       <c r="B66" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C66" t="s">
         <v>38</v>
@@ -3166,29 +3181,29 @@
         <v>45</v>
       </c>
       <c r="F66" t="s">
-        <v>137</v>
+        <v>153</v>
       </c>
     </row>
     <row r="67">
       <c r="B67" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C67" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D67" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E67" t="s">
         <v>45</v>
       </c>
       <c r="F67" t="s">
-        <v>151</v>
+        <v>75</v>
       </c>
     </row>
     <row r="68">
       <c r="B68" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C68" t="s">
         <v>38</v>
@@ -3200,12 +3215,12 @@
         <v>45</v>
       </c>
       <c r="F68" t="s">
-        <v>153</v>
+        <v>102</v>
       </c>
     </row>
     <row r="69">
       <c r="B69" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="C69" t="s">
         <v>38</v>
@@ -3217,62 +3232,94 @@
         <v>45</v>
       </c>
       <c r="F69" t="s">
-        <v>75</v>
+        <v>135</v>
       </c>
     </row>
     <row r="70">
       <c r="B70" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="C70" t="s">
         <v>38</v>
       </c>
       <c r="D70" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E70" t="s">
         <v>45</v>
       </c>
       <c r="F70" t="s">
-        <v>102</v>
+        <v>145</v>
       </c>
     </row>
     <row r="71">
       <c r="B71" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="C71" t="s">
         <v>38</v>
       </c>
       <c r="D71" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E71" t="s">
         <v>45</v>
       </c>
       <c r="F71" t="s">
-        <v>135</v>
+        <v>197</v>
       </c>
     </row>
     <row r="72">
       <c r="B72" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="C72" t="s">
         <v>38</v>
       </c>
       <c r="D72" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E72" t="s">
         <v>45</v>
       </c>
       <c r="F72" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="B73" t="s">
+        <v>199</v>
+      </c>
+      <c r="C73" t="s">
+        <v>38</v>
+      </c>
+      <c r="D73" t="s">
+        <v>44</v>
+      </c>
+      <c r="E73" t="s">
+        <v>45</v>
+      </c>
+      <c r="F73" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="73"/>
-    <row r="74"/>
+    <row r="74">
+      <c r="B74" t="s">
+        <v>200</v>
+      </c>
+      <c r="C74" t="s">
+        <v>38</v>
+      </c>
+      <c r="D74" t="s">
+        <v>44</v>
+      </c>
+      <c r="E74" t="s">
+        <v>45</v>
+      </c>
+      <c r="F74" t="s">
+        <v>197</v>
+      </c>
+    </row>
     <row r="75"/>
     <row r="76"/>
     <row r="77"/>

</xml_diff>

<commit_message>
Created panel for display measure for time mode.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20750" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29176" uniqueCount="273">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -637,6 +637,222 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId89</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TI 1 (IN&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN&lt;value&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">displayMeas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId92</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TI 2 (IN&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId93</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId94</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TI 3 (IN&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TI 4 (IN&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId97</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId98</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TI 5 (IN&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TI 6 (IN&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TI 7 (IN&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">displayLabel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">displaylabelBold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verdanab.ttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId104</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN&lt;value&gt;: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stamps </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId106</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId107</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId108</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId109</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StdDev</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId113</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId114</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId116</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId117</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId118</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId119</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId121</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId122</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId124</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId127</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId128</t>
+  </si>
+  <si>
+    <t xml:space="preserve">displayMeasValue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId129</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId130</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId131</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId132</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId133</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId134</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId135</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId136</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId137</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId138</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId139</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId140</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId141</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId142</t>
   </si>
 </sst>
 </file>
@@ -2015,6 +2231,33 @@
       <c r="P8" s="10"/>
     </row>
     <row r="9" spans="2:16">
+      <c r="B9" t="s">
+        <v>205</v>
+      </c>
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9">
+        <v>22</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" t="s">
+        <v>122</v>
+      </c>
+      <c r="J9" t="s">
+        <v>42</v>
+      </c>
       <c r="L9" s="11" t="s">
         <v>6</v>
       </c>
@@ -2032,6 +2275,33 @@
       </c>
     </row>
     <row r="10" spans="2:16">
+      <c r="B10" t="s">
+        <v>224</v>
+      </c>
+      <c r="C10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10">
+        <v>15</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" t="s">
+        <v>42</v>
+      </c>
       <c r="L10" s="11" t="s">
         <v>28</v>
       </c>
@@ -2047,9 +2317,63 @@
       <c r="P10" s="14"/>
     </row>
     <row r="11" spans="2:16">
+      <c r="B11" t="s">
+        <v>225</v>
+      </c>
+      <c r="C11" t="s">
+        <v>226</v>
+      </c>
+      <c r="D11">
+        <v>15</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" t="s">
+        <v>42</v>
+      </c>
+      <c r="J11" t="s">
+        <v>42</v>
+      </c>
       <c r="L11" s="15"/>
     </row>
     <row r="12" spans="2:16">
+      <c r="B12" t="s">
+        <v>257</v>
+      </c>
+      <c r="C12" t="s">
+        <v>226</v>
+      </c>
+      <c r="D12">
+        <v>18</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" t="s">
+        <v>42</v>
+      </c>
       <c r="M12" s="16" t="s">
         <v>27</v>
       </c>
@@ -3320,17 +3644,907 @@
         <v>197</v>
       </c>
     </row>
-    <row r="75"/>
-    <row r="76"/>
-    <row r="77"/>
-    <row r="78"/>
-    <row r="79"/>
-    <row r="80"/>
-    <row r="81"/>
-    <row r="82"/>
-    <row r="83"/>
-    <row r="84"/>
-    <row r="85"/>
+    <row r="75">
+      <c r="B75" t="s">
+        <v>201</v>
+      </c>
+      <c r="C75" t="s">
+        <v>205</v>
+      </c>
+      <c r="D75" t="s">
+        <v>50</v>
+      </c>
+      <c r="E75" t="s">
+        <v>45</v>
+      </c>
+      <c r="F75" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="B76" t="s">
+        <v>203</v>
+      </c>
+      <c r="C76" t="s">
+        <v>205</v>
+      </c>
+      <c r="D76" t="s">
+        <v>50</v>
+      </c>
+      <c r="E76" t="s">
+        <v>45</v>
+      </c>
+      <c r="F76" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="B77" t="s">
+        <v>206</v>
+      </c>
+      <c r="C77" t="s">
+        <v>205</v>
+      </c>
+      <c r="D77" t="s">
+        <v>50</v>
+      </c>
+      <c r="E77" t="s">
+        <v>45</v>
+      </c>
+      <c r="F77" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="B78" t="s">
+        <v>208</v>
+      </c>
+      <c r="C78" t="s">
+        <v>205</v>
+      </c>
+      <c r="D78" t="s">
+        <v>50</v>
+      </c>
+      <c r="E78" t="s">
+        <v>45</v>
+      </c>
+      <c r="F78" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="B79" t="s">
+        <v>209</v>
+      </c>
+      <c r="C79" t="s">
+        <v>205</v>
+      </c>
+      <c r="D79" t="s">
+        <v>50</v>
+      </c>
+      <c r="E79" t="s">
+        <v>45</v>
+      </c>
+      <c r="F79" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="B80" t="s">
+        <v>211</v>
+      </c>
+      <c r="C80" t="s">
+        <v>205</v>
+      </c>
+      <c r="D80" t="s">
+        <v>50</v>
+      </c>
+      <c r="E80" t="s">
+        <v>45</v>
+      </c>
+      <c r="F80" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="B81" t="s">
+        <v>212</v>
+      </c>
+      <c r="C81" t="s">
+        <v>205</v>
+      </c>
+      <c r="D81" t="s">
+        <v>50</v>
+      </c>
+      <c r="E81" t="s">
+        <v>45</v>
+      </c>
+      <c r="F81" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="B82" t="s">
+        <v>214</v>
+      </c>
+      <c r="C82" t="s">
+        <v>205</v>
+      </c>
+      <c r="D82" t="s">
+        <v>50</v>
+      </c>
+      <c r="E82" t="s">
+        <v>45</v>
+      </c>
+      <c r="F82" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="B83" t="s">
+        <v>215</v>
+      </c>
+      <c r="C83" t="s">
+        <v>205</v>
+      </c>
+      <c r="D83" t="s">
+        <v>50</v>
+      </c>
+      <c r="E83" t="s">
+        <v>45</v>
+      </c>
+      <c r="F83" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="B84" t="s">
+        <v>217</v>
+      </c>
+      <c r="C84" t="s">
+        <v>205</v>
+      </c>
+      <c r="D84" t="s">
+        <v>50</v>
+      </c>
+      <c r="E84" t="s">
+        <v>45</v>
+      </c>
+      <c r="F84" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="B85" t="s">
+        <v>218</v>
+      </c>
+      <c r="C85" t="s">
+        <v>205</v>
+      </c>
+      <c r="D85" t="s">
+        <v>50</v>
+      </c>
+      <c r="E85" t="s">
+        <v>45</v>
+      </c>
+      <c r="F85" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="B86" t="s">
+        <v>220</v>
+      </c>
+      <c r="C86" t="s">
+        <v>205</v>
+      </c>
+      <c r="D86" t="s">
+        <v>50</v>
+      </c>
+      <c r="E86" t="s">
+        <v>45</v>
+      </c>
+      <c r="F86" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="B87" t="s">
+        <v>221</v>
+      </c>
+      <c r="C87" t="s">
+        <v>205</v>
+      </c>
+      <c r="D87" t="s">
+        <v>50</v>
+      </c>
+      <c r="E87" t="s">
+        <v>45</v>
+      </c>
+      <c r="F87" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="B88" t="s">
+        <v>223</v>
+      </c>
+      <c r="C88" t="s">
+        <v>205</v>
+      </c>
+      <c r="D88" t="s">
+        <v>50</v>
+      </c>
+      <c r="E88" t="s">
+        <v>45</v>
+      </c>
+      <c r="F88" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="B89" t="s">
+        <v>227</v>
+      </c>
+      <c r="C89" t="s">
+        <v>224</v>
+      </c>
+      <c r="D89" t="s">
+        <v>50</v>
+      </c>
+      <c r="E89" t="s">
+        <v>45</v>
+      </c>
+      <c r="F89" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="B90" t="s">
+        <v>229</v>
+      </c>
+      <c r="C90" t="s">
+        <v>225</v>
+      </c>
+      <c r="D90" t="s">
+        <v>50</v>
+      </c>
+      <c r="E90" t="s">
+        <v>45</v>
+      </c>
+      <c r="F90" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="B91" t="s">
+        <v>231</v>
+      </c>
+      <c r="C91" t="s">
+        <v>225</v>
+      </c>
+      <c r="D91" t="s">
+        <v>50</v>
+      </c>
+      <c r="E91" t="s">
+        <v>45</v>
+      </c>
+      <c r="F91" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="B92" t="s">
+        <v>233</v>
+      </c>
+      <c r="C92" t="s">
+        <v>224</v>
+      </c>
+      <c r="D92" t="s">
+        <v>50</v>
+      </c>
+      <c r="E92" t="s">
+        <v>45</v>
+      </c>
+      <c r="F92" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="B93" t="s">
+        <v>234</v>
+      </c>
+      <c r="C93" t="s">
+        <v>224</v>
+      </c>
+      <c r="D93" t="s">
+        <v>44</v>
+      </c>
+      <c r="E93" t="s">
+        <v>45</v>
+      </c>
+      <c r="F93" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="B94" t="s">
+        <v>235</v>
+      </c>
+      <c r="C94" t="s">
+        <v>205</v>
+      </c>
+      <c r="D94" t="s">
+        <v>50</v>
+      </c>
+      <c r="E94" t="s">
+        <v>45</v>
+      </c>
+      <c r="F94" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="B95" t="s">
+        <v>237</v>
+      </c>
+      <c r="C95" t="s">
+        <v>205</v>
+      </c>
+      <c r="D95" t="s">
+        <v>50</v>
+      </c>
+      <c r="E95" t="s">
+        <v>45</v>
+      </c>
+      <c r="F95" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="B96" t="s">
+        <v>239</v>
+      </c>
+      <c r="C96" t="s">
+        <v>224</v>
+      </c>
+      <c r="D96" t="s">
+        <v>50</v>
+      </c>
+      <c r="E96" t="s">
+        <v>45</v>
+      </c>
+      <c r="F96" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="B97" t="s">
+        <v>240</v>
+      </c>
+      <c r="C97" t="s">
+        <v>224</v>
+      </c>
+      <c r="D97" t="s">
+        <v>50</v>
+      </c>
+      <c r="E97" t="s">
+        <v>45</v>
+      </c>
+      <c r="F97" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="B98" t="s">
+        <v>241</v>
+      </c>
+      <c r="C98" t="s">
+        <v>224</v>
+      </c>
+      <c r="D98" t="s">
+        <v>50</v>
+      </c>
+      <c r="E98" t="s">
+        <v>45</v>
+      </c>
+      <c r="F98" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="B99" t="s">
+        <v>242</v>
+      </c>
+      <c r="C99" t="s">
+        <v>224</v>
+      </c>
+      <c r="D99" t="s">
+        <v>50</v>
+      </c>
+      <c r="E99" t="s">
+        <v>45</v>
+      </c>
+      <c r="F99" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="B100" t="s">
+        <v>243</v>
+      </c>
+      <c r="C100" t="s">
+        <v>224</v>
+      </c>
+      <c r="D100" t="s">
+        <v>50</v>
+      </c>
+      <c r="E100" t="s">
+        <v>45</v>
+      </c>
+      <c r="F100" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="B101" t="s">
+        <v>244</v>
+      </c>
+      <c r="C101" t="s">
+        <v>224</v>
+      </c>
+      <c r="D101" t="s">
+        <v>50</v>
+      </c>
+      <c r="E101" t="s">
+        <v>45</v>
+      </c>
+      <c r="F101" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="B102" t="s">
+        <v>245</v>
+      </c>
+      <c r="C102" t="s">
+        <v>224</v>
+      </c>
+      <c r="D102" t="s">
+        <v>50</v>
+      </c>
+      <c r="E102" t="s">
+        <v>45</v>
+      </c>
+      <c r="F102" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="B103" t="s">
+        <v>246</v>
+      </c>
+      <c r="C103" t="s">
+        <v>224</v>
+      </c>
+      <c r="D103" t="s">
+        <v>50</v>
+      </c>
+      <c r="E103" t="s">
+        <v>45</v>
+      </c>
+      <c r="F103" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="B104" t="s">
+        <v>247</v>
+      </c>
+      <c r="C104" t="s">
+        <v>224</v>
+      </c>
+      <c r="D104" t="s">
+        <v>50</v>
+      </c>
+      <c r="E104" t="s">
+        <v>45</v>
+      </c>
+      <c r="F104" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="B105" t="s">
+        <v>248</v>
+      </c>
+      <c r="C105" t="s">
+        <v>224</v>
+      </c>
+      <c r="D105" t="s">
+        <v>50</v>
+      </c>
+      <c r="E105" t="s">
+        <v>45</v>
+      </c>
+      <c r="F105" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="B106" t="s">
+        <v>249</v>
+      </c>
+      <c r="C106" t="s">
+        <v>224</v>
+      </c>
+      <c r="D106" t="s">
+        <v>50</v>
+      </c>
+      <c r="E106" t="s">
+        <v>45</v>
+      </c>
+      <c r="F106" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="B107" t="s">
+        <v>250</v>
+      </c>
+      <c r="C107" t="s">
+        <v>224</v>
+      </c>
+      <c r="D107" t="s">
+        <v>50</v>
+      </c>
+      <c r="E107" t="s">
+        <v>45</v>
+      </c>
+      <c r="F107" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="B108" t="s">
+        <v>251</v>
+      </c>
+      <c r="C108" t="s">
+        <v>224</v>
+      </c>
+      <c r="D108" t="s">
+        <v>44</v>
+      </c>
+      <c r="E108" t="s">
+        <v>45</v>
+      </c>
+      <c r="F108" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="B109" t="s">
+        <v>252</v>
+      </c>
+      <c r="C109" t="s">
+        <v>224</v>
+      </c>
+      <c r="D109" t="s">
+        <v>44</v>
+      </c>
+      <c r="E109" t="s">
+        <v>45</v>
+      </c>
+      <c r="F109" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="B110" t="s">
+        <v>253</v>
+      </c>
+      <c r="C110" t="s">
+        <v>224</v>
+      </c>
+      <c r="D110" t="s">
+        <v>44</v>
+      </c>
+      <c r="E110" t="s">
+        <v>45</v>
+      </c>
+      <c r="F110" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="B111" t="s">
+        <v>254</v>
+      </c>
+      <c r="C111" t="s">
+        <v>224</v>
+      </c>
+      <c r="D111" t="s">
+        <v>44</v>
+      </c>
+      <c r="E111" t="s">
+        <v>45</v>
+      </c>
+      <c r="F111" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="B112" t="s">
+        <v>255</v>
+      </c>
+      <c r="C112" t="s">
+        <v>224</v>
+      </c>
+      <c r="D112" t="s">
+        <v>44</v>
+      </c>
+      <c r="E112" t="s">
+        <v>45</v>
+      </c>
+      <c r="F112" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="B113" t="s">
+        <v>256</v>
+      </c>
+      <c r="C113" t="s">
+        <v>224</v>
+      </c>
+      <c r="D113" t="s">
+        <v>44</v>
+      </c>
+      <c r="E113" t="s">
+        <v>45</v>
+      </c>
+      <c r="F113" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="B114" t="s">
+        <v>258</v>
+      </c>
+      <c r="C114" t="s">
+        <v>257</v>
+      </c>
+      <c r="D114" t="s">
+        <v>259</v>
+      </c>
+      <c r="E114" t="s">
+        <v>45</v>
+      </c>
+      <c r="F114" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="B115" t="s">
+        <v>260</v>
+      </c>
+      <c r="C115" t="s">
+        <v>257</v>
+      </c>
+      <c r="D115" t="s">
+        <v>259</v>
+      </c>
+      <c r="E115" t="s">
+        <v>45</v>
+      </c>
+      <c r="F115" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="B116" t="s">
+        <v>261</v>
+      </c>
+      <c r="C116" t="s">
+        <v>257</v>
+      </c>
+      <c r="D116" t="s">
+        <v>259</v>
+      </c>
+      <c r="E116" t="s">
+        <v>45</v>
+      </c>
+      <c r="F116" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="B117" t="s">
+        <v>262</v>
+      </c>
+      <c r="C117" t="s">
+        <v>257</v>
+      </c>
+      <c r="D117" t="s">
+        <v>259</v>
+      </c>
+      <c r="E117" t="s">
+        <v>45</v>
+      </c>
+      <c r="F117" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="B118" t="s">
+        <v>263</v>
+      </c>
+      <c r="C118" t="s">
+        <v>257</v>
+      </c>
+      <c r="D118" t="s">
+        <v>259</v>
+      </c>
+      <c r="E118" t="s">
+        <v>45</v>
+      </c>
+      <c r="F118" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="B119" t="s">
+        <v>264</v>
+      </c>
+      <c r="C119" t="s">
+        <v>257</v>
+      </c>
+      <c r="D119" t="s">
+        <v>259</v>
+      </c>
+      <c r="E119" t="s">
+        <v>45</v>
+      </c>
+      <c r="F119" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="B120" t="s">
+        <v>265</v>
+      </c>
+      <c r="C120" t="s">
+        <v>257</v>
+      </c>
+      <c r="D120" t="s">
+        <v>259</v>
+      </c>
+      <c r="E120" t="s">
+        <v>45</v>
+      </c>
+      <c r="F120" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="B121" t="s">
+        <v>266</v>
+      </c>
+      <c r="C121" t="s">
+        <v>257</v>
+      </c>
+      <c r="D121" t="s">
+        <v>259</v>
+      </c>
+      <c r="E121" t="s">
+        <v>45</v>
+      </c>
+      <c r="F121" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="B122" t="s">
+        <v>267</v>
+      </c>
+      <c r="C122" t="s">
+        <v>257</v>
+      </c>
+      <c r="D122" t="s">
+        <v>259</v>
+      </c>
+      <c r="E122" t="s">
+        <v>45</v>
+      </c>
+      <c r="F122" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="B123" t="s">
+        <v>268</v>
+      </c>
+      <c r="C123" t="s">
+        <v>257</v>
+      </c>
+      <c r="D123" t="s">
+        <v>259</v>
+      </c>
+      <c r="E123" t="s">
+        <v>45</v>
+      </c>
+      <c r="F123" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="B124" t="s">
+        <v>269</v>
+      </c>
+      <c r="C124" t="s">
+        <v>257</v>
+      </c>
+      <c r="D124" t="s">
+        <v>259</v>
+      </c>
+      <c r="E124" t="s">
+        <v>45</v>
+      </c>
+      <c r="F124" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="B125" t="s">
+        <v>270</v>
+      </c>
+      <c r="C125" t="s">
+        <v>257</v>
+      </c>
+      <c r="D125" t="s">
+        <v>259</v>
+      </c>
+      <c r="E125" t="s">
+        <v>45</v>
+      </c>
+      <c r="F125" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="B126" t="s">
+        <v>271</v>
+      </c>
+      <c r="C126" t="s">
+        <v>257</v>
+      </c>
+      <c r="D126" t="s">
+        <v>259</v>
+      </c>
+      <c r="E126" t="s">
+        <v>45</v>
+      </c>
+      <c r="F126" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="B127" t="s">
+        <v>272</v>
+      </c>
+      <c r="C127" t="s">
+        <v>257</v>
+      </c>
+      <c r="D127" t="s">
+        <v>259</v>
+      </c>
+      <c r="E127" t="s">
+        <v>45</v>
+      </c>
+      <c r="F127" t="s">
+        <v>75</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Developed UI for display measure for time mode.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29176" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32676" uniqueCount="289">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -853,6 +853,54 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId142</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IN&lt;value&gt;: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId143</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId144</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId145</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId146</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId147</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId148</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId149</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId151</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId152</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId153</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId154</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId155</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId156</t>
+  </si>
+  <si>
+    <t xml:space="preserve">. ,' '</t>
   </si>
 </sst>
 </file>
@@ -2033,7 +2081,7 @@
         <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>42</v>
+        <v>288</v>
       </c>
       <c r="H4" t="s">
         <v>42</v>
@@ -2077,7 +2125,7 @@
         <v>17</v>
       </c>
       <c r="G5" t="s">
-        <v>42</v>
+        <v>288</v>
       </c>
       <c r="H5" t="s">
         <v>42</v>
@@ -2119,7 +2167,7 @@
         <v>17</v>
       </c>
       <c r="G6" t="s">
-        <v>42</v>
+        <v>288</v>
       </c>
       <c r="H6" t="s">
         <v>42</v>
@@ -2161,7 +2209,7 @@
         <v>17</v>
       </c>
       <c r="G7" t="s">
-        <v>42</v>
+        <v>288</v>
       </c>
       <c r="H7" t="s">
         <v>42</v>
@@ -2205,7 +2253,7 @@
         <v>17</v>
       </c>
       <c r="G8" t="s">
-        <v>42</v>
+        <v>288</v>
       </c>
       <c r="H8" t="s">
         <v>42</v>
@@ -2247,7 +2295,7 @@
         <v>17</v>
       </c>
       <c r="G9" t="s">
-        <v>42</v>
+        <v>288</v>
       </c>
       <c r="H9" t="s">
         <v>42</v>
@@ -2291,13 +2339,13 @@
         <v>17</v>
       </c>
       <c r="G10" t="s">
-        <v>42</v>
+        <v>288</v>
       </c>
       <c r="H10" t="s">
         <v>42</v>
       </c>
       <c r="I10" t="s">
-        <v>42</v>
+        <v>122</v>
       </c>
       <c r="J10" t="s">
         <v>42</v>
@@ -2333,13 +2381,13 @@
         <v>17</v>
       </c>
       <c r="G11" t="s">
-        <v>42</v>
+        <v>288</v>
       </c>
       <c r="H11" t="s">
         <v>42</v>
       </c>
       <c r="I11" t="s">
-        <v>42</v>
+        <v>122</v>
       </c>
       <c r="J11" t="s">
         <v>42</v>
@@ -2363,13 +2411,13 @@
         <v>17</v>
       </c>
       <c r="G12" t="s">
-        <v>42</v>
+        <v>288</v>
       </c>
       <c r="H12" t="s">
         <v>42</v>
       </c>
       <c r="I12" t="s">
-        <v>42</v>
+        <v>122</v>
       </c>
       <c r="J12" t="s">
         <v>42</v>
@@ -3896,7 +3944,7 @@
         <v>45</v>
       </c>
       <c r="F89" t="s">
-        <v>228</v>
+        <v>273</v>
       </c>
     </row>
     <row r="90">
@@ -3947,7 +3995,7 @@
         <v>45</v>
       </c>
       <c r="F92" t="s">
-        <v>228</v>
+        <v>273</v>
       </c>
     </row>
     <row r="93">
@@ -4015,7 +4063,7 @@
         <v>45</v>
       </c>
       <c r="F96" t="s">
-        <v>228</v>
+        <v>273</v>
       </c>
     </row>
     <row r="97">
@@ -4032,7 +4080,7 @@
         <v>45</v>
       </c>
       <c r="F97" t="s">
-        <v>228</v>
+        <v>273</v>
       </c>
     </row>
     <row r="98">
@@ -4049,7 +4097,7 @@
         <v>45</v>
       </c>
       <c r="F98" t="s">
-        <v>228</v>
+        <v>273</v>
       </c>
     </row>
     <row r="99">
@@ -4066,7 +4114,7 @@
         <v>45</v>
       </c>
       <c r="F99" t="s">
-        <v>228</v>
+        <v>273</v>
       </c>
     </row>
     <row r="100">
@@ -4083,7 +4131,7 @@
         <v>45</v>
       </c>
       <c r="F100" t="s">
-        <v>228</v>
+        <v>273</v>
       </c>
     </row>
     <row r="101">
@@ -4100,7 +4148,7 @@
         <v>45</v>
       </c>
       <c r="F101" t="s">
-        <v>228</v>
+        <v>273</v>
       </c>
     </row>
     <row r="102">
@@ -4117,7 +4165,7 @@
         <v>45</v>
       </c>
       <c r="F102" t="s">
-        <v>228</v>
+        <v>273</v>
       </c>
     </row>
     <row r="103">
@@ -4134,7 +4182,7 @@
         <v>45</v>
       </c>
       <c r="F103" t="s">
-        <v>228</v>
+        <v>273</v>
       </c>
     </row>
     <row r="104">
@@ -4151,7 +4199,7 @@
         <v>45</v>
       </c>
       <c r="F104" t="s">
-        <v>228</v>
+        <v>273</v>
       </c>
     </row>
     <row r="105">
@@ -4168,7 +4216,7 @@
         <v>45</v>
       </c>
       <c r="F105" t="s">
-        <v>228</v>
+        <v>273</v>
       </c>
     </row>
     <row r="106">
@@ -4185,7 +4233,7 @@
         <v>45</v>
       </c>
       <c r="F106" t="s">
-        <v>228</v>
+        <v>273</v>
       </c>
     </row>
     <row r="107">
@@ -4202,7 +4250,7 @@
         <v>45</v>
       </c>
       <c r="F107" t="s">
-        <v>228</v>
+        <v>273</v>
       </c>
     </row>
     <row r="108">
@@ -4542,6 +4590,244 @@
         <v>45</v>
       </c>
       <c r="F127" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="B128" t="s">
+        <v>274</v>
+      </c>
+      <c r="C128" t="s">
+        <v>224</v>
+      </c>
+      <c r="D128" t="s">
+        <v>44</v>
+      </c>
+      <c r="E128" t="s">
+        <v>45</v>
+      </c>
+      <c r="F128" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="B129" t="s">
+        <v>275</v>
+      </c>
+      <c r="C129" t="s">
+        <v>224</v>
+      </c>
+      <c r="D129" t="s">
+        <v>44</v>
+      </c>
+      <c r="E129" t="s">
+        <v>45</v>
+      </c>
+      <c r="F129" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="B130" t="s">
+        <v>276</v>
+      </c>
+      <c r="C130" t="s">
+        <v>224</v>
+      </c>
+      <c r="D130" t="s">
+        <v>44</v>
+      </c>
+      <c r="E130" t="s">
+        <v>45</v>
+      </c>
+      <c r="F130" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="B131" t="s">
+        <v>277</v>
+      </c>
+      <c r="C131" t="s">
+        <v>224</v>
+      </c>
+      <c r="D131" t="s">
+        <v>44</v>
+      </c>
+      <c r="E131" t="s">
+        <v>45</v>
+      </c>
+      <c r="F131" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="B132" t="s">
+        <v>278</v>
+      </c>
+      <c r="C132" t="s">
+        <v>224</v>
+      </c>
+      <c r="D132" t="s">
+        <v>44</v>
+      </c>
+      <c r="E132" t="s">
+        <v>45</v>
+      </c>
+      <c r="F132" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="B133" t="s">
+        <v>279</v>
+      </c>
+      <c r="C133" t="s">
+        <v>224</v>
+      </c>
+      <c r="D133" t="s">
+        <v>44</v>
+      </c>
+      <c r="E133" t="s">
+        <v>45</v>
+      </c>
+      <c r="F133" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="B134" t="s">
+        <v>280</v>
+      </c>
+      <c r="C134" t="s">
+        <v>224</v>
+      </c>
+      <c r="D134" t="s">
+        <v>44</v>
+      </c>
+      <c r="E134" t="s">
+        <v>45</v>
+      </c>
+      <c r="F134" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="B135" t="s">
+        <v>281</v>
+      </c>
+      <c r="C135" t="s">
+        <v>224</v>
+      </c>
+      <c r="D135" t="s">
+        <v>44</v>
+      </c>
+      <c r="E135" t="s">
+        <v>45</v>
+      </c>
+      <c r="F135" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="B136" t="s">
+        <v>282</v>
+      </c>
+      <c r="C136" t="s">
+        <v>224</v>
+      </c>
+      <c r="D136" t="s">
+        <v>44</v>
+      </c>
+      <c r="E136" t="s">
+        <v>45</v>
+      </c>
+      <c r="F136" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="B137" t="s">
+        <v>283</v>
+      </c>
+      <c r="C137" t="s">
+        <v>224</v>
+      </c>
+      <c r="D137" t="s">
+        <v>44</v>
+      </c>
+      <c r="E137" t="s">
+        <v>45</v>
+      </c>
+      <c r="F137" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="B138" t="s">
+        <v>284</v>
+      </c>
+      <c r="C138" t="s">
+        <v>224</v>
+      </c>
+      <c r="D138" t="s">
+        <v>44</v>
+      </c>
+      <c r="E138" t="s">
+        <v>45</v>
+      </c>
+      <c r="F138" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="B139" t="s">
+        <v>285</v>
+      </c>
+      <c r="C139" t="s">
+        <v>224</v>
+      </c>
+      <c r="D139" t="s">
+        <v>44</v>
+      </c>
+      <c r="E139" t="s">
+        <v>45</v>
+      </c>
+      <c r="F139" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="B140" t="s">
+        <v>286</v>
+      </c>
+      <c r="C140" t="s">
+        <v>224</v>
+      </c>
+      <c r="D140" t="s">
+        <v>44</v>
+      </c>
+      <c r="E140" t="s">
+        <v>45</v>
+      </c>
+      <c r="F140" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="B141" t="s">
+        <v>287</v>
+      </c>
+      <c r="C141" t="s">
+        <v>224</v>
+      </c>
+      <c r="D141" t="s">
+        <v>44</v>
+      </c>
+      <c r="E141" t="s">
+        <v>45</v>
+      </c>
+      <c r="F141" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added label for unit.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32676" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35700" uniqueCount="328">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -901,6 +901,123 @@
   </si>
   <si>
     <t xml:space="preserve">. ,' '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId157</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId158</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId159</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId160</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId161</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId162</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId163</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId164</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId165</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId166</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId167</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId168</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId169</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId170</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId171</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId172</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId173</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId174</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId175</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId176</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId177</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId178</t>
+  </si>
+  <si>
+    <t xml:space="preserve">us</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId179</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId180</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId181</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId182</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId183</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId184</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId185</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId186</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId187</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId188</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId189</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId190</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId191</t>
   </si>
 </sst>
 </file>
@@ -4831,6 +4948,601 @@
         <v>75</v>
       </c>
     </row>
+    <row r="142">
+      <c r="B142" t="s">
+        <v>289</v>
+      </c>
+      <c r="C142" t="s">
+        <v>224</v>
+      </c>
+      <c r="D142" t="s">
+        <v>50</v>
+      </c>
+      <c r="E142" t="s">
+        <v>45</v>
+      </c>
+      <c r="F142" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="B143" t="s">
+        <v>291</v>
+      </c>
+      <c r="C143" t="s">
+        <v>224</v>
+      </c>
+      <c r="D143" t="s">
+        <v>50</v>
+      </c>
+      <c r="E143" t="s">
+        <v>45</v>
+      </c>
+      <c r="F143" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="B144" t="s">
+        <v>292</v>
+      </c>
+      <c r="C144" t="s">
+        <v>224</v>
+      </c>
+      <c r="D144" t="s">
+        <v>50</v>
+      </c>
+      <c r="E144" t="s">
+        <v>45</v>
+      </c>
+      <c r="F144" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="B145" t="s">
+        <v>293</v>
+      </c>
+      <c r="C145" t="s">
+        <v>224</v>
+      </c>
+      <c r="D145" t="s">
+        <v>50</v>
+      </c>
+      <c r="E145" t="s">
+        <v>45</v>
+      </c>
+      <c r="F145" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="B146" t="s">
+        <v>294</v>
+      </c>
+      <c r="C146" t="s">
+        <v>224</v>
+      </c>
+      <c r="D146" t="s">
+        <v>50</v>
+      </c>
+      <c r="E146" t="s">
+        <v>45</v>
+      </c>
+      <c r="F146" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="B147" t="s">
+        <v>295</v>
+      </c>
+      <c r="C147" t="s">
+        <v>224</v>
+      </c>
+      <c r="D147" t="s">
+        <v>50</v>
+      </c>
+      <c r="E147" t="s">
+        <v>45</v>
+      </c>
+      <c r="F147" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="B148" t="s">
+        <v>296</v>
+      </c>
+      <c r="C148" t="s">
+        <v>224</v>
+      </c>
+      <c r="D148" t="s">
+        <v>50</v>
+      </c>
+      <c r="E148" t="s">
+        <v>45</v>
+      </c>
+      <c r="F148" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="B149" t="s">
+        <v>297</v>
+      </c>
+      <c r="C149" t="s">
+        <v>224</v>
+      </c>
+      <c r="D149" t="s">
+        <v>44</v>
+      </c>
+      <c r="E149" t="s">
+        <v>45</v>
+      </c>
+      <c r="F149" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="B150" t="s">
+        <v>298</v>
+      </c>
+      <c r="C150" t="s">
+        <v>224</v>
+      </c>
+      <c r="D150" t="s">
+        <v>44</v>
+      </c>
+      <c r="E150" t="s">
+        <v>45</v>
+      </c>
+      <c r="F150" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="B151" t="s">
+        <v>299</v>
+      </c>
+      <c r="C151" t="s">
+        <v>224</v>
+      </c>
+      <c r="D151" t="s">
+        <v>44</v>
+      </c>
+      <c r="E151" t="s">
+        <v>45</v>
+      </c>
+      <c r="F151" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="B152" t="s">
+        <v>300</v>
+      </c>
+      <c r="C152" t="s">
+        <v>224</v>
+      </c>
+      <c r="D152" t="s">
+        <v>44</v>
+      </c>
+      <c r="E152" t="s">
+        <v>45</v>
+      </c>
+      <c r="F152" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="B153" t="s">
+        <v>301</v>
+      </c>
+      <c r="C153" t="s">
+        <v>224</v>
+      </c>
+      <c r="D153" t="s">
+        <v>44</v>
+      </c>
+      <c r="E153" t="s">
+        <v>45</v>
+      </c>
+      <c r="F153" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="B154" t="s">
+        <v>302</v>
+      </c>
+      <c r="C154" t="s">
+        <v>224</v>
+      </c>
+      <c r="D154" t="s">
+        <v>44</v>
+      </c>
+      <c r="E154" t="s">
+        <v>45</v>
+      </c>
+      <c r="F154" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="B155" t="s">
+        <v>303</v>
+      </c>
+      <c r="C155" t="s">
+        <v>224</v>
+      </c>
+      <c r="D155" t="s">
+        <v>44</v>
+      </c>
+      <c r="E155" t="s">
+        <v>45</v>
+      </c>
+      <c r="F155" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="B156" t="s">
+        <v>304</v>
+      </c>
+      <c r="C156" t="s">
+        <v>224</v>
+      </c>
+      <c r="D156" t="s">
+        <v>44</v>
+      </c>
+      <c r="E156" t="s">
+        <v>45</v>
+      </c>
+      <c r="F156" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="B157" t="s">
+        <v>306</v>
+      </c>
+      <c r="C157" t="s">
+        <v>224</v>
+      </c>
+      <c r="D157" t="s">
+        <v>44</v>
+      </c>
+      <c r="E157" t="s">
+        <v>45</v>
+      </c>
+      <c r="F157" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="B158" t="s">
+        <v>307</v>
+      </c>
+      <c r="C158" t="s">
+        <v>224</v>
+      </c>
+      <c r="D158" t="s">
+        <v>44</v>
+      </c>
+      <c r="E158" t="s">
+        <v>45</v>
+      </c>
+      <c r="F158" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="B159" t="s">
+        <v>308</v>
+      </c>
+      <c r="C159" t="s">
+        <v>224</v>
+      </c>
+      <c r="D159" t="s">
+        <v>44</v>
+      </c>
+      <c r="E159" t="s">
+        <v>45</v>
+      </c>
+      <c r="F159" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="B160" t="s">
+        <v>309</v>
+      </c>
+      <c r="C160" t="s">
+        <v>224</v>
+      </c>
+      <c r="D160" t="s">
+        <v>44</v>
+      </c>
+      <c r="E160" t="s">
+        <v>45</v>
+      </c>
+      <c r="F160" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="B161" t="s">
+        <v>310</v>
+      </c>
+      <c r="C161" t="s">
+        <v>224</v>
+      </c>
+      <c r="D161" t="s">
+        <v>44</v>
+      </c>
+      <c r="E161" t="s">
+        <v>45</v>
+      </c>
+      <c r="F161" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="B162" t="s">
+        <v>311</v>
+      </c>
+      <c r="C162" t="s">
+        <v>224</v>
+      </c>
+      <c r="D162" t="s">
+        <v>44</v>
+      </c>
+      <c r="E162" t="s">
+        <v>45</v>
+      </c>
+      <c r="F162" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="B163" t="s">
+        <v>312</v>
+      </c>
+      <c r="C163" t="s">
+        <v>224</v>
+      </c>
+      <c r="D163" t="s">
+        <v>44</v>
+      </c>
+      <c r="E163" t="s">
+        <v>45</v>
+      </c>
+      <c r="F163" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="B164" t="s">
+        <v>314</v>
+      </c>
+      <c r="C164" t="s">
+        <v>224</v>
+      </c>
+      <c r="D164" t="s">
+        <v>44</v>
+      </c>
+      <c r="E164" t="s">
+        <v>45</v>
+      </c>
+      <c r="F164" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="B165" t="s">
+        <v>315</v>
+      </c>
+      <c r="C165" t="s">
+        <v>224</v>
+      </c>
+      <c r="D165" t="s">
+        <v>44</v>
+      </c>
+      <c r="E165" t="s">
+        <v>45</v>
+      </c>
+      <c r="F165" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="B166" t="s">
+        <v>316</v>
+      </c>
+      <c r="C166" t="s">
+        <v>224</v>
+      </c>
+      <c r="D166" t="s">
+        <v>44</v>
+      </c>
+      <c r="E166" t="s">
+        <v>45</v>
+      </c>
+      <c r="F166" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="B167" t="s">
+        <v>317</v>
+      </c>
+      <c r="C167" t="s">
+        <v>224</v>
+      </c>
+      <c r="D167" t="s">
+        <v>44</v>
+      </c>
+      <c r="E167" t="s">
+        <v>45</v>
+      </c>
+      <c r="F167" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="B168" t="s">
+        <v>318</v>
+      </c>
+      <c r="C168" t="s">
+        <v>224</v>
+      </c>
+      <c r="D168" t="s">
+        <v>44</v>
+      </c>
+      <c r="E168" t="s">
+        <v>45</v>
+      </c>
+      <c r="F168" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="B169" t="s">
+        <v>319</v>
+      </c>
+      <c r="C169" t="s">
+        <v>224</v>
+      </c>
+      <c r="D169" t="s">
+        <v>44</v>
+      </c>
+      <c r="E169" t="s">
+        <v>45</v>
+      </c>
+      <c r="F169" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="B170" t="s">
+        <v>320</v>
+      </c>
+      <c r="C170" t="s">
+        <v>224</v>
+      </c>
+      <c r="D170" t="s">
+        <v>44</v>
+      </c>
+      <c r="E170" t="s">
+        <v>45</v>
+      </c>
+      <c r="F170" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="B171" t="s">
+        <v>322</v>
+      </c>
+      <c r="C171" t="s">
+        <v>224</v>
+      </c>
+      <c r="D171" t="s">
+        <v>44</v>
+      </c>
+      <c r="E171" t="s">
+        <v>45</v>
+      </c>
+      <c r="F171" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="B172" t="s">
+        <v>323</v>
+      </c>
+      <c r="C172" t="s">
+        <v>224</v>
+      </c>
+      <c r="D172" t="s">
+        <v>44</v>
+      </c>
+      <c r="E172" t="s">
+        <v>45</v>
+      </c>
+      <c r="F172" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="B173" t="s">
+        <v>324</v>
+      </c>
+      <c r="C173" t="s">
+        <v>224</v>
+      </c>
+      <c r="D173" t="s">
+        <v>44</v>
+      </c>
+      <c r="E173" t="s">
+        <v>45</v>
+      </c>
+      <c r="F173" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="B174" t="s">
+        <v>325</v>
+      </c>
+      <c r="C174" t="s">
+        <v>224</v>
+      </c>
+      <c r="D174" t="s">
+        <v>44</v>
+      </c>
+      <c r="E174" t="s">
+        <v>45</v>
+      </c>
+      <c r="F174" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="B175" t="s">
+        <v>326</v>
+      </c>
+      <c r="C175" t="s">
+        <v>224</v>
+      </c>
+      <c r="D175" t="s">
+        <v>44</v>
+      </c>
+      <c r="E175" t="s">
+        <v>45</v>
+      </c>
+      <c r="F175" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="B176" t="s">
+        <v>327</v>
+      </c>
+      <c r="C176" t="s">
+        <v>224</v>
+      </c>
+      <c r="D176" t="s">
+        <v>44</v>
+      </c>
+      <c r="E176" t="s">
+        <v>45</v>
+      </c>
+      <c r="F176" t="s">
+        <v>321</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Developed UI for display measures Frequency Mode.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36848" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57600" uniqueCount="448">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1063,6 +1063,321 @@
   </si>
   <si>
     <t xml:space="preserve">TI 7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId199</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(IN&lt;value&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId201</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId202</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId203</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId205</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freq 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId207</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freq 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId208</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freq 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId209</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freq 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId210</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freq 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId211</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freq 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId212</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freq 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId213</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId214</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freq 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId215</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId216</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId217</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId218</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId219</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId220</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId221</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId222</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId223</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId224</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId225</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId226</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId227</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId228</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId229</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId230</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId231</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId232</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId233</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId235</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId236</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId237</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId238</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId239</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId240</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId241</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId242</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId243</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId244</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId245</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId246</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId247</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId248</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId249</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uHz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId251</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId252</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId253</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId254</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId255</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId256</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId257</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mHz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId258</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId259</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId260</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId261</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId262</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId263</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId264</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId265</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kHz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId266</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId267</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId268</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId269</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId270</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId271</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId272</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId273</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MHz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId274</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId275</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId276</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId277</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId278</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId279</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId280</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId281</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Text &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GHz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId282</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId283</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId284</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId285</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId286</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId287</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId288</t>
   </si>
 </sst>
 </file>
@@ -5707,6 +6022,1536 @@
         <v>342</v>
       </c>
     </row>
+    <row r="184">
+      <c r="B184" t="s">
+        <v>343</v>
+      </c>
+      <c r="C184" t="s">
+        <v>205</v>
+      </c>
+      <c r="D184" t="s">
+        <v>50</v>
+      </c>
+      <c r="E184" t="s">
+        <v>45</v>
+      </c>
+      <c r="F184" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="B185" t="s">
+        <v>345</v>
+      </c>
+      <c r="C185" t="s">
+        <v>205</v>
+      </c>
+      <c r="D185" t="s">
+        <v>50</v>
+      </c>
+      <c r="E185" t="s">
+        <v>45</v>
+      </c>
+      <c r="F185" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="B186" t="s">
+        <v>346</v>
+      </c>
+      <c r="C186" t="s">
+        <v>205</v>
+      </c>
+      <c r="D186" t="s">
+        <v>50</v>
+      </c>
+      <c r="E186" t="s">
+        <v>45</v>
+      </c>
+      <c r="F186" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="B187" t="s">
+        <v>347</v>
+      </c>
+      <c r="C187" t="s">
+        <v>205</v>
+      </c>
+      <c r="D187" t="s">
+        <v>50</v>
+      </c>
+      <c r="E187" t="s">
+        <v>45</v>
+      </c>
+      <c r="F187" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="B188" t="s">
+        <v>348</v>
+      </c>
+      <c r="C188" t="s">
+        <v>205</v>
+      </c>
+      <c r="D188" t="s">
+        <v>50</v>
+      </c>
+      <c r="E188" t="s">
+        <v>45</v>
+      </c>
+      <c r="F188" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="B189" t="s">
+        <v>349</v>
+      </c>
+      <c r="C189" t="s">
+        <v>205</v>
+      </c>
+      <c r="D189" t="s">
+        <v>50</v>
+      </c>
+      <c r="E189" t="s">
+        <v>45</v>
+      </c>
+      <c r="F189" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="B190" t="s">
+        <v>350</v>
+      </c>
+      <c r="C190" t="s">
+        <v>205</v>
+      </c>
+      <c r="D190" t="s">
+        <v>50</v>
+      </c>
+      <c r="E190" t="s">
+        <v>45</v>
+      </c>
+      <c r="F190" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="B191" t="s">
+        <v>351</v>
+      </c>
+      <c r="C191" t="s">
+        <v>205</v>
+      </c>
+      <c r="D191" t="s">
+        <v>50</v>
+      </c>
+      <c r="E191" t="s">
+        <v>45</v>
+      </c>
+      <c r="F191" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="B192" t="s">
+        <v>353</v>
+      </c>
+      <c r="C192" t="s">
+        <v>205</v>
+      </c>
+      <c r="D192" t="s">
+        <v>50</v>
+      </c>
+      <c r="E192" t="s">
+        <v>45</v>
+      </c>
+      <c r="F192" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="B193" t="s">
+        <v>355</v>
+      </c>
+      <c r="C193" t="s">
+        <v>205</v>
+      </c>
+      <c r="D193" t="s">
+        <v>50</v>
+      </c>
+      <c r="E193" t="s">
+        <v>45</v>
+      </c>
+      <c r="F193" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="B194" t="s">
+        <v>357</v>
+      </c>
+      <c r="C194" t="s">
+        <v>205</v>
+      </c>
+      <c r="D194" t="s">
+        <v>50</v>
+      </c>
+      <c r="E194" t="s">
+        <v>45</v>
+      </c>
+      <c r="F194" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="B195" t="s">
+        <v>359</v>
+      </c>
+      <c r="C195" t="s">
+        <v>205</v>
+      </c>
+      <c r="D195" t="s">
+        <v>50</v>
+      </c>
+      <c r="E195" t="s">
+        <v>45</v>
+      </c>
+      <c r="F195" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="B196" t="s">
+        <v>361</v>
+      </c>
+      <c r="C196" t="s">
+        <v>205</v>
+      </c>
+      <c r="D196" t="s">
+        <v>50</v>
+      </c>
+      <c r="E196" t="s">
+        <v>45</v>
+      </c>
+      <c r="F196" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="B197" t="s">
+        <v>363</v>
+      </c>
+      <c r="C197" t="s">
+        <v>205</v>
+      </c>
+      <c r="D197" t="s">
+        <v>50</v>
+      </c>
+      <c r="E197" t="s">
+        <v>45</v>
+      </c>
+      <c r="F197" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="B198" t="s">
+        <v>365</v>
+      </c>
+      <c r="C198" t="s">
+        <v>205</v>
+      </c>
+      <c r="D198" t="s">
+        <v>50</v>
+      </c>
+      <c r="E198" t="s">
+        <v>45</v>
+      </c>
+      <c r="F198" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="B199" t="s">
+        <v>366</v>
+      </c>
+      <c r="C199" t="s">
+        <v>205</v>
+      </c>
+      <c r="D199" t="s">
+        <v>50</v>
+      </c>
+      <c r="E199" t="s">
+        <v>45</v>
+      </c>
+      <c r="F199" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="B200" t="s">
+        <v>368</v>
+      </c>
+      <c r="C200" t="s">
+        <v>225</v>
+      </c>
+      <c r="D200" t="s">
+        <v>50</v>
+      </c>
+      <c r="E200" t="s">
+        <v>45</v>
+      </c>
+      <c r="F200" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="B201" t="s">
+        <v>369</v>
+      </c>
+      <c r="C201" t="s">
+        <v>205</v>
+      </c>
+      <c r="D201" t="s">
+        <v>50</v>
+      </c>
+      <c r="E201" t="s">
+        <v>45</v>
+      </c>
+      <c r="F201" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="B202" t="s">
+        <v>370</v>
+      </c>
+      <c r="C202" t="s">
+        <v>205</v>
+      </c>
+      <c r="D202" t="s">
+        <v>50</v>
+      </c>
+      <c r="E202" t="s">
+        <v>45</v>
+      </c>
+      <c r="F202" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="B203" t="s">
+        <v>371</v>
+      </c>
+      <c r="C203" t="s">
+        <v>224</v>
+      </c>
+      <c r="D203" t="s">
+        <v>44</v>
+      </c>
+      <c r="E203" t="s">
+        <v>45</v>
+      </c>
+      <c r="F203" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="B204" t="s">
+        <v>372</v>
+      </c>
+      <c r="C204" t="s">
+        <v>224</v>
+      </c>
+      <c r="D204" t="s">
+        <v>44</v>
+      </c>
+      <c r="E204" t="s">
+        <v>45</v>
+      </c>
+      <c r="F204" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="B205" t="s">
+        <v>373</v>
+      </c>
+      <c r="C205" t="s">
+        <v>224</v>
+      </c>
+      <c r="D205" t="s">
+        <v>44</v>
+      </c>
+      <c r="E205" t="s">
+        <v>45</v>
+      </c>
+      <c r="F205" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="B206" t="s">
+        <v>374</v>
+      </c>
+      <c r="C206" t="s">
+        <v>224</v>
+      </c>
+      <c r="D206" t="s">
+        <v>44</v>
+      </c>
+      <c r="E206" t="s">
+        <v>45</v>
+      </c>
+      <c r="F206" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="B207" t="s">
+        <v>375</v>
+      </c>
+      <c r="C207" t="s">
+        <v>224</v>
+      </c>
+      <c r="D207" t="s">
+        <v>44</v>
+      </c>
+      <c r="E207" t="s">
+        <v>45</v>
+      </c>
+      <c r="F207" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="B208" t="s">
+        <v>376</v>
+      </c>
+      <c r="C208" t="s">
+        <v>224</v>
+      </c>
+      <c r="D208" t="s">
+        <v>44</v>
+      </c>
+      <c r="E208" t="s">
+        <v>45</v>
+      </c>
+      <c r="F208" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="B209" t="s">
+        <v>377</v>
+      </c>
+      <c r="C209" t="s">
+        <v>224</v>
+      </c>
+      <c r="D209" t="s">
+        <v>44</v>
+      </c>
+      <c r="E209" t="s">
+        <v>45</v>
+      </c>
+      <c r="F209" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="B210" t="s">
+        <v>378</v>
+      </c>
+      <c r="C210" t="s">
+        <v>224</v>
+      </c>
+      <c r="D210" t="s">
+        <v>44</v>
+      </c>
+      <c r="E210" t="s">
+        <v>45</v>
+      </c>
+      <c r="F210" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="B211" t="s">
+        <v>379</v>
+      </c>
+      <c r="C211" t="s">
+        <v>257</v>
+      </c>
+      <c r="D211" t="s">
+        <v>259</v>
+      </c>
+      <c r="E211" t="s">
+        <v>45</v>
+      </c>
+      <c r="F211" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="B212" t="s">
+        <v>380</v>
+      </c>
+      <c r="C212" t="s">
+        <v>257</v>
+      </c>
+      <c r="D212" t="s">
+        <v>259</v>
+      </c>
+      <c r="E212" t="s">
+        <v>45</v>
+      </c>
+      <c r="F212" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="B213" t="s">
+        <v>381</v>
+      </c>
+      <c r="C213" t="s">
+        <v>257</v>
+      </c>
+      <c r="D213" t="s">
+        <v>259</v>
+      </c>
+      <c r="E213" t="s">
+        <v>45</v>
+      </c>
+      <c r="F213" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="B214" t="s">
+        <v>382</v>
+      </c>
+      <c r="C214" t="s">
+        <v>257</v>
+      </c>
+      <c r="D214" t="s">
+        <v>259</v>
+      </c>
+      <c r="E214" t="s">
+        <v>45</v>
+      </c>
+      <c r="F214" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="B215" t="s">
+        <v>383</v>
+      </c>
+      <c r="C215" t="s">
+        <v>257</v>
+      </c>
+      <c r="D215" t="s">
+        <v>259</v>
+      </c>
+      <c r="E215" t="s">
+        <v>45</v>
+      </c>
+      <c r="F215" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="B216" t="s">
+        <v>384</v>
+      </c>
+      <c r="C216" t="s">
+        <v>257</v>
+      </c>
+      <c r="D216" t="s">
+        <v>259</v>
+      </c>
+      <c r="E216" t="s">
+        <v>45</v>
+      </c>
+      <c r="F216" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="B217" t="s">
+        <v>385</v>
+      </c>
+      <c r="C217" t="s">
+        <v>257</v>
+      </c>
+      <c r="D217" t="s">
+        <v>259</v>
+      </c>
+      <c r="E217" t="s">
+        <v>45</v>
+      </c>
+      <c r="F217" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="B218" t="s">
+        <v>386</v>
+      </c>
+      <c r="C218" t="s">
+        <v>257</v>
+      </c>
+      <c r="D218" t="s">
+        <v>259</v>
+      </c>
+      <c r="E218" t="s">
+        <v>45</v>
+      </c>
+      <c r="F218" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="B219" t="s">
+        <v>387</v>
+      </c>
+      <c r="C219" t="s">
+        <v>257</v>
+      </c>
+      <c r="D219" t="s">
+        <v>259</v>
+      </c>
+      <c r="E219" t="s">
+        <v>45</v>
+      </c>
+      <c r="F219" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="B220" t="s">
+        <v>388</v>
+      </c>
+      <c r="C220" t="s">
+        <v>257</v>
+      </c>
+      <c r="D220" t="s">
+        <v>259</v>
+      </c>
+      <c r="E220" t="s">
+        <v>45</v>
+      </c>
+      <c r="F220" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="B221" t="s">
+        <v>389</v>
+      </c>
+      <c r="C221" t="s">
+        <v>257</v>
+      </c>
+      <c r="D221" t="s">
+        <v>259</v>
+      </c>
+      <c r="E221" t="s">
+        <v>45</v>
+      </c>
+      <c r="F221" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="B222" t="s">
+        <v>390</v>
+      </c>
+      <c r="C222" t="s">
+        <v>257</v>
+      </c>
+      <c r="D222" t="s">
+        <v>259</v>
+      </c>
+      <c r="E222" t="s">
+        <v>45</v>
+      </c>
+      <c r="F222" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="B223" t="s">
+        <v>391</v>
+      </c>
+      <c r="C223" t="s">
+        <v>257</v>
+      </c>
+      <c r="D223" t="s">
+        <v>259</v>
+      </c>
+      <c r="E223" t="s">
+        <v>45</v>
+      </c>
+      <c r="F223" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="B224" t="s">
+        <v>392</v>
+      </c>
+      <c r="C224" t="s">
+        <v>257</v>
+      </c>
+      <c r="D224" t="s">
+        <v>259</v>
+      </c>
+      <c r="E224" t="s">
+        <v>45</v>
+      </c>
+      <c r="F224" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="B225" t="s">
+        <v>393</v>
+      </c>
+      <c r="C225" t="s">
+        <v>257</v>
+      </c>
+      <c r="D225" t="s">
+        <v>259</v>
+      </c>
+      <c r="E225" t="s">
+        <v>45</v>
+      </c>
+      <c r="F225" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="B226" t="s">
+        <v>394</v>
+      </c>
+      <c r="C226" t="s">
+        <v>257</v>
+      </c>
+      <c r="D226" t="s">
+        <v>259</v>
+      </c>
+      <c r="E226" t="s">
+        <v>45</v>
+      </c>
+      <c r="F226" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="B227" t="s">
+        <v>395</v>
+      </c>
+      <c r="C227" t="s">
+        <v>224</v>
+      </c>
+      <c r="D227" t="s">
+        <v>50</v>
+      </c>
+      <c r="E227" t="s">
+        <v>45</v>
+      </c>
+      <c r="F227" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="B228" t="s">
+        <v>396</v>
+      </c>
+      <c r="C228" t="s">
+        <v>224</v>
+      </c>
+      <c r="D228" t="s">
+        <v>50</v>
+      </c>
+      <c r="E228" t="s">
+        <v>45</v>
+      </c>
+      <c r="F228" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="B229" t="s">
+        <v>397</v>
+      </c>
+      <c r="C229" t="s">
+        <v>224</v>
+      </c>
+      <c r="D229" t="s">
+        <v>50</v>
+      </c>
+      <c r="E229" t="s">
+        <v>45</v>
+      </c>
+      <c r="F229" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="B230" t="s">
+        <v>398</v>
+      </c>
+      <c r="C230" t="s">
+        <v>224</v>
+      </c>
+      <c r="D230" t="s">
+        <v>50</v>
+      </c>
+      <c r="E230" t="s">
+        <v>45</v>
+      </c>
+      <c r="F230" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="B231" t="s">
+        <v>399</v>
+      </c>
+      <c r="C231" t="s">
+        <v>224</v>
+      </c>
+      <c r="D231" t="s">
+        <v>50</v>
+      </c>
+      <c r="E231" t="s">
+        <v>45</v>
+      </c>
+      <c r="F231" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="B232" t="s">
+        <v>400</v>
+      </c>
+      <c r="C232" t="s">
+        <v>224</v>
+      </c>
+      <c r="D232" t="s">
+        <v>50</v>
+      </c>
+      <c r="E232" t="s">
+        <v>45</v>
+      </c>
+      <c r="F232" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="B233" t="s">
+        <v>401</v>
+      </c>
+      <c r="C233" t="s">
+        <v>224</v>
+      </c>
+      <c r="D233" t="s">
+        <v>50</v>
+      </c>
+      <c r="E233" t="s">
+        <v>45</v>
+      </c>
+      <c r="F233" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="B234" t="s">
+        <v>402</v>
+      </c>
+      <c r="C234" t="s">
+        <v>224</v>
+      </c>
+      <c r="D234" t="s">
+        <v>50</v>
+      </c>
+      <c r="E234" t="s">
+        <v>45</v>
+      </c>
+      <c r="F234" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="B235" t="s">
+        <v>404</v>
+      </c>
+      <c r="C235" t="s">
+        <v>224</v>
+      </c>
+      <c r="D235" t="s">
+        <v>50</v>
+      </c>
+      <c r="E235" t="s">
+        <v>45</v>
+      </c>
+      <c r="F235" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="B236" t="s">
+        <v>405</v>
+      </c>
+      <c r="C236" t="s">
+        <v>224</v>
+      </c>
+      <c r="D236" t="s">
+        <v>50</v>
+      </c>
+      <c r="E236" t="s">
+        <v>45</v>
+      </c>
+      <c r="F236" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="B237" t="s">
+        <v>406</v>
+      </c>
+      <c r="C237" t="s">
+        <v>224</v>
+      </c>
+      <c r="D237" t="s">
+        <v>50</v>
+      </c>
+      <c r="E237" t="s">
+        <v>45</v>
+      </c>
+      <c r="F237" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="B238" t="s">
+        <v>407</v>
+      </c>
+      <c r="C238" t="s">
+        <v>224</v>
+      </c>
+      <c r="D238" t="s">
+        <v>50</v>
+      </c>
+      <c r="E238" t="s">
+        <v>45</v>
+      </c>
+      <c r="F238" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="B239" t="s">
+        <v>408</v>
+      </c>
+      <c r="C239" t="s">
+        <v>224</v>
+      </c>
+      <c r="D239" t="s">
+        <v>50</v>
+      </c>
+      <c r="E239" t="s">
+        <v>45</v>
+      </c>
+      <c r="F239" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="B240" t="s">
+        <v>409</v>
+      </c>
+      <c r="C240" t="s">
+        <v>224</v>
+      </c>
+      <c r="D240" t="s">
+        <v>50</v>
+      </c>
+      <c r="E240" t="s">
+        <v>45</v>
+      </c>
+      <c r="F240" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="B241" t="s">
+        <v>410</v>
+      </c>
+      <c r="C241" t="s">
+        <v>224</v>
+      </c>
+      <c r="D241" t="s">
+        <v>50</v>
+      </c>
+      <c r="E241" t="s">
+        <v>45</v>
+      </c>
+      <c r="F241" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="B242" t="s">
+        <v>411</v>
+      </c>
+      <c r="C242" t="s">
+        <v>224</v>
+      </c>
+      <c r="D242" t="s">
+        <v>50</v>
+      </c>
+      <c r="E242" t="s">
+        <v>45</v>
+      </c>
+      <c r="F242" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="B243" t="s">
+        <v>413</v>
+      </c>
+      <c r="C243" t="s">
+        <v>224</v>
+      </c>
+      <c r="D243" t="s">
+        <v>50</v>
+      </c>
+      <c r="E243" t="s">
+        <v>45</v>
+      </c>
+      <c r="F243" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="B244" t="s">
+        <v>414</v>
+      </c>
+      <c r="C244" t="s">
+        <v>224</v>
+      </c>
+      <c r="D244" t="s">
+        <v>50</v>
+      </c>
+      <c r="E244" t="s">
+        <v>45</v>
+      </c>
+      <c r="F244" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="B245" t="s">
+        <v>415</v>
+      </c>
+      <c r="C245" t="s">
+        <v>224</v>
+      </c>
+      <c r="D245" t="s">
+        <v>50</v>
+      </c>
+      <c r="E245" t="s">
+        <v>45</v>
+      </c>
+      <c r="F245" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="B246" t="s">
+        <v>416</v>
+      </c>
+      <c r="C246" t="s">
+        <v>224</v>
+      </c>
+      <c r="D246" t="s">
+        <v>50</v>
+      </c>
+      <c r="E246" t="s">
+        <v>45</v>
+      </c>
+      <c r="F246" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="B247" t="s">
+        <v>417</v>
+      </c>
+      <c r="C247" t="s">
+        <v>224</v>
+      </c>
+      <c r="D247" t="s">
+        <v>50</v>
+      </c>
+      <c r="E247" t="s">
+        <v>45</v>
+      </c>
+      <c r="F247" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="B248" t="s">
+        <v>418</v>
+      </c>
+      <c r="C248" t="s">
+        <v>224</v>
+      </c>
+      <c r="D248" t="s">
+        <v>50</v>
+      </c>
+      <c r="E248" t="s">
+        <v>45</v>
+      </c>
+      <c r="F248" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="B249" t="s">
+        <v>419</v>
+      </c>
+      <c r="C249" t="s">
+        <v>224</v>
+      </c>
+      <c r="D249" t="s">
+        <v>50</v>
+      </c>
+      <c r="E249" t="s">
+        <v>45</v>
+      </c>
+      <c r="F249" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="B250" t="s">
+        <v>420</v>
+      </c>
+      <c r="C250" t="s">
+        <v>224</v>
+      </c>
+      <c r="D250" t="s">
+        <v>50</v>
+      </c>
+      <c r="E250" t="s">
+        <v>45</v>
+      </c>
+      <c r="F250" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="B251" t="s">
+        <v>422</v>
+      </c>
+      <c r="C251" t="s">
+        <v>224</v>
+      </c>
+      <c r="D251" t="s">
+        <v>50</v>
+      </c>
+      <c r="E251" t="s">
+        <v>45</v>
+      </c>
+      <c r="F251" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="B252" t="s">
+        <v>423</v>
+      </c>
+      <c r="C252" t="s">
+        <v>224</v>
+      </c>
+      <c r="D252" t="s">
+        <v>50</v>
+      </c>
+      <c r="E252" t="s">
+        <v>45</v>
+      </c>
+      <c r="F252" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="B253" t="s">
+        <v>424</v>
+      </c>
+      <c r="C253" t="s">
+        <v>224</v>
+      </c>
+      <c r="D253" t="s">
+        <v>50</v>
+      </c>
+      <c r="E253" t="s">
+        <v>45</v>
+      </c>
+      <c r="F253" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="B254" t="s">
+        <v>425</v>
+      </c>
+      <c r="C254" t="s">
+        <v>224</v>
+      </c>
+      <c r="D254" t="s">
+        <v>50</v>
+      </c>
+      <c r="E254" t="s">
+        <v>45</v>
+      </c>
+      <c r="F254" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="B255" t="s">
+        <v>426</v>
+      </c>
+      <c r="C255" t="s">
+        <v>224</v>
+      </c>
+      <c r="D255" t="s">
+        <v>50</v>
+      </c>
+      <c r="E255" t="s">
+        <v>45</v>
+      </c>
+      <c r="F255" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="B256" t="s">
+        <v>427</v>
+      </c>
+      <c r="C256" t="s">
+        <v>224</v>
+      </c>
+      <c r="D256" t="s">
+        <v>50</v>
+      </c>
+      <c r="E256" t="s">
+        <v>45</v>
+      </c>
+      <c r="F256" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="B257" t="s">
+        <v>428</v>
+      </c>
+      <c r="C257" t="s">
+        <v>224</v>
+      </c>
+      <c r="D257" t="s">
+        <v>50</v>
+      </c>
+      <c r="E257" t="s">
+        <v>45</v>
+      </c>
+      <c r="F257" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="B258" t="s">
+        <v>429</v>
+      </c>
+      <c r="C258" t="s">
+        <v>224</v>
+      </c>
+      <c r="D258" t="s">
+        <v>50</v>
+      </c>
+      <c r="E258" t="s">
+        <v>45</v>
+      </c>
+      <c r="F258" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="B259" t="s">
+        <v>431</v>
+      </c>
+      <c r="C259" t="s">
+        <v>224</v>
+      </c>
+      <c r="D259" t="s">
+        <v>50</v>
+      </c>
+      <c r="E259" t="s">
+        <v>45</v>
+      </c>
+      <c r="F259" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="B260" t="s">
+        <v>432</v>
+      </c>
+      <c r="C260" t="s">
+        <v>224</v>
+      </c>
+      <c r="D260" t="s">
+        <v>50</v>
+      </c>
+      <c r="E260" t="s">
+        <v>45</v>
+      </c>
+      <c r="F260" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="B261" t="s">
+        <v>433</v>
+      </c>
+      <c r="C261" t="s">
+        <v>224</v>
+      </c>
+      <c r="D261" t="s">
+        <v>50</v>
+      </c>
+      <c r="E261" t="s">
+        <v>45</v>
+      </c>
+      <c r="F261" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="B262" t="s">
+        <v>434</v>
+      </c>
+      <c r="C262" t="s">
+        <v>224</v>
+      </c>
+      <c r="D262" t="s">
+        <v>50</v>
+      </c>
+      <c r="E262" t="s">
+        <v>45</v>
+      </c>
+      <c r="F262" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="B263" t="s">
+        <v>435</v>
+      </c>
+      <c r="C263" t="s">
+        <v>224</v>
+      </c>
+      <c r="D263" t="s">
+        <v>50</v>
+      </c>
+      <c r="E263" t="s">
+        <v>45</v>
+      </c>
+      <c r="F263" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="B264" t="s">
+        <v>436</v>
+      </c>
+      <c r="C264" t="s">
+        <v>224</v>
+      </c>
+      <c r="D264" t="s">
+        <v>50</v>
+      </c>
+      <c r="E264" t="s">
+        <v>45</v>
+      </c>
+      <c r="F264" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="B265" t="s">
+        <v>437</v>
+      </c>
+      <c r="C265" t="s">
+        <v>224</v>
+      </c>
+      <c r="D265" t="s">
+        <v>50</v>
+      </c>
+      <c r="E265" t="s">
+        <v>45</v>
+      </c>
+      <c r="F265" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="B266" t="s">
+        <v>438</v>
+      </c>
+      <c r="C266" t="s">
+        <v>224</v>
+      </c>
+      <c r="D266" t="s">
+        <v>50</v>
+      </c>
+      <c r="E266" t="s">
+        <v>45</v>
+      </c>
+      <c r="F266" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="B267" t="s">
+        <v>441</v>
+      </c>
+      <c r="C267" t="s">
+        <v>224</v>
+      </c>
+      <c r="D267" t="s">
+        <v>50</v>
+      </c>
+      <c r="E267" t="s">
+        <v>45</v>
+      </c>
+      <c r="F267" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="B268" t="s">
+        <v>442</v>
+      </c>
+      <c r="C268" t="s">
+        <v>224</v>
+      </c>
+      <c r="D268" t="s">
+        <v>50</v>
+      </c>
+      <c r="E268" t="s">
+        <v>45</v>
+      </c>
+      <c r="F268" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="B269" t="s">
+        <v>443</v>
+      </c>
+      <c r="C269" t="s">
+        <v>224</v>
+      </c>
+      <c r="D269" t="s">
+        <v>50</v>
+      </c>
+      <c r="E269" t="s">
+        <v>45</v>
+      </c>
+      <c r="F269" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="B270" t="s">
+        <v>444</v>
+      </c>
+      <c r="C270" t="s">
+        <v>224</v>
+      </c>
+      <c r="D270" t="s">
+        <v>50</v>
+      </c>
+      <c r="E270" t="s">
+        <v>45</v>
+      </c>
+      <c r="F270" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="B271" t="s">
+        <v>445</v>
+      </c>
+      <c r="C271" t="s">
+        <v>224</v>
+      </c>
+      <c r="D271" t="s">
+        <v>50</v>
+      </c>
+      <c r="E271" t="s">
+        <v>45</v>
+      </c>
+      <c r="F271" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="B272" t="s">
+        <v>446</v>
+      </c>
+      <c r="C272" t="s">
+        <v>224</v>
+      </c>
+      <c r="D272" t="s">
+        <v>50</v>
+      </c>
+      <c r="E272" t="s">
+        <v>45</v>
+      </c>
+      <c r="F272" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="B273" t="s">
+        <v>447</v>
+      </c>
+      <c r="C273" t="s">
+        <v>224</v>
+      </c>
+      <c r="D273" t="s">
+        <v>50</v>
+      </c>
+      <c r="E273" t="s">
+        <v>45</v>
+      </c>
+      <c r="F273" t="s">
+        <v>440</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Reorganized unit label in frequency UI.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67584" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70336" uniqueCount="452">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -6416,13 +6416,13 @@
         <v>224</v>
       </c>
       <c r="D206" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E206" t="s">
         <v>45</v>
       </c>
       <c r="F206" t="s">
-        <v>403</v>
+        <v>75</v>
       </c>
     </row>
     <row r="207">
@@ -6433,13 +6433,13 @@
         <v>224</v>
       </c>
       <c r="D207" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E207" t="s">
         <v>45</v>
       </c>
       <c r="F207" t="s">
-        <v>403</v>
+        <v>75</v>
       </c>
     </row>
     <row r="208">
@@ -6450,13 +6450,13 @@
         <v>224</v>
       </c>
       <c r="D208" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E208" t="s">
         <v>45</v>
       </c>
       <c r="F208" t="s">
-        <v>403</v>
+        <v>75</v>
       </c>
     </row>
     <row r="209">
@@ -6467,13 +6467,13 @@
         <v>224</v>
       </c>
       <c r="D209" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E209" t="s">
         <v>45</v>
       </c>
       <c r="F209" t="s">
-        <v>403</v>
+        <v>75</v>
       </c>
     </row>
     <row r="210">
@@ -6484,13 +6484,13 @@
         <v>224</v>
       </c>
       <c r="D210" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E210" t="s">
         <v>45</v>
       </c>
       <c r="F210" t="s">
-        <v>403</v>
+        <v>75</v>
       </c>
     </row>
     <row r="211">
@@ -6501,13 +6501,13 @@
         <v>224</v>
       </c>
       <c r="D211" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E211" t="s">
         <v>45</v>
       </c>
       <c r="F211" t="s">
-        <v>403</v>
+        <v>75</v>
       </c>
     </row>
     <row r="212">
@@ -6518,13 +6518,13 @@
         <v>224</v>
       </c>
       <c r="D212" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E212" t="s">
         <v>45</v>
       </c>
       <c r="F212" t="s">
-        <v>403</v>
+        <v>75</v>
       </c>
     </row>
     <row r="213">
@@ -6535,559 +6535,175 @@
         <v>224</v>
       </c>
       <c r="D213" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E213" t="s">
         <v>45</v>
       </c>
       <c r="F213" t="s">
-        <v>403</v>
+        <v>75</v>
       </c>
     </row>
     <row r="214">
       <c r="B214" t="s">
-        <v>411</v>
+        <v>420</v>
       </c>
       <c r="C214" t="s">
         <v>224</v>
       </c>
       <c r="D214" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E214" t="s">
         <v>45</v>
       </c>
       <c r="F214" t="s">
-        <v>412</v>
+        <v>75</v>
       </c>
     </row>
     <row r="215">
       <c r="B215" t="s">
-        <v>413</v>
+        <v>422</v>
       </c>
       <c r="C215" t="s">
         <v>224</v>
       </c>
       <c r="D215" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E215" t="s">
         <v>45</v>
       </c>
       <c r="F215" t="s">
-        <v>412</v>
+        <v>75</v>
       </c>
     </row>
     <row r="216">
       <c r="B216" t="s">
-        <v>414</v>
+        <v>423</v>
       </c>
       <c r="C216" t="s">
         <v>224</v>
       </c>
       <c r="D216" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E216" t="s">
         <v>45</v>
       </c>
       <c r="F216" t="s">
-        <v>412</v>
+        <v>75</v>
       </c>
     </row>
     <row r="217">
       <c r="B217" t="s">
-        <v>415</v>
+        <v>424</v>
       </c>
       <c r="C217" t="s">
         <v>224</v>
       </c>
       <c r="D217" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E217" t="s">
         <v>45</v>
       </c>
       <c r="F217" t="s">
-        <v>412</v>
+        <v>75</v>
       </c>
     </row>
     <row r="218">
       <c r="B218" t="s">
-        <v>416</v>
+        <v>425</v>
       </c>
       <c r="C218" t="s">
         <v>224</v>
       </c>
       <c r="D218" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E218" t="s">
         <v>45</v>
       </c>
       <c r="F218" t="s">
-        <v>412</v>
+        <v>75</v>
       </c>
     </row>
     <row r="219">
       <c r="B219" t="s">
-        <v>417</v>
+        <v>426</v>
       </c>
       <c r="C219" t="s">
         <v>224</v>
       </c>
       <c r="D219" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E219" t="s">
         <v>45</v>
       </c>
       <c r="F219" t="s">
-        <v>412</v>
+        <v>75</v>
       </c>
     </row>
     <row r="220">
       <c r="B220" t="s">
-        <v>418</v>
+        <v>427</v>
       </c>
       <c r="C220" t="s">
         <v>224</v>
       </c>
       <c r="D220" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E220" t="s">
         <v>45</v>
       </c>
       <c r="F220" t="s">
-        <v>412</v>
+        <v>75</v>
       </c>
     </row>
     <row r="221">
       <c r="B221" t="s">
-        <v>419</v>
+        <v>428</v>
       </c>
       <c r="C221" t="s">
         <v>224</v>
       </c>
       <c r="D221" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E221" t="s">
         <v>45</v>
       </c>
       <c r="F221" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="222">
-      <c r="B222" t="s">
-        <v>420</v>
-      </c>
-      <c r="C222" t="s">
-        <v>224</v>
-      </c>
-      <c r="D222" t="s">
-        <v>50</v>
-      </c>
-      <c r="E222" t="s">
-        <v>45</v>
-      </c>
-      <c r="F222" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="223">
-      <c r="B223" t="s">
-        <v>422</v>
-      </c>
-      <c r="C223" t="s">
-        <v>224</v>
-      </c>
-      <c r="D223" t="s">
-        <v>50</v>
-      </c>
-      <c r="E223" t="s">
-        <v>45</v>
-      </c>
-      <c r="F223" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="224">
-      <c r="B224" t="s">
-        <v>423</v>
-      </c>
-      <c r="C224" t="s">
-        <v>224</v>
-      </c>
-      <c r="D224" t="s">
-        <v>50</v>
-      </c>
-      <c r="E224" t="s">
-        <v>45</v>
-      </c>
-      <c r="F224" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="225">
-      <c r="B225" t="s">
-        <v>424</v>
-      </c>
-      <c r="C225" t="s">
-        <v>224</v>
-      </c>
-      <c r="D225" t="s">
-        <v>50</v>
-      </c>
-      <c r="E225" t="s">
-        <v>45</v>
-      </c>
-      <c r="F225" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="226">
-      <c r="B226" t="s">
-        <v>425</v>
-      </c>
-      <c r="C226" t="s">
-        <v>224</v>
-      </c>
-      <c r="D226" t="s">
-        <v>50</v>
-      </c>
-      <c r="E226" t="s">
-        <v>45</v>
-      </c>
-      <c r="F226" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="227">
-      <c r="B227" t="s">
-        <v>426</v>
-      </c>
-      <c r="C227" t="s">
-        <v>224</v>
-      </c>
-      <c r="D227" t="s">
-        <v>50</v>
-      </c>
-      <c r="E227" t="s">
-        <v>45</v>
-      </c>
-      <c r="F227" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="228">
-      <c r="B228" t="s">
-        <v>427</v>
-      </c>
-      <c r="C228" t="s">
-        <v>224</v>
-      </c>
-      <c r="D228" t="s">
-        <v>50</v>
-      </c>
-      <c r="E228" t="s">
-        <v>45</v>
-      </c>
-      <c r="F228" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="229">
-      <c r="B229" t="s">
-        <v>428</v>
-      </c>
-      <c r="C229" t="s">
-        <v>224</v>
-      </c>
-      <c r="D229" t="s">
-        <v>50</v>
-      </c>
-      <c r="E229" t="s">
-        <v>45</v>
-      </c>
-      <c r="F229" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="230">
-      <c r="B230" t="s">
-        <v>429</v>
-      </c>
-      <c r="C230" t="s">
-        <v>224</v>
-      </c>
-      <c r="D230" t="s">
-        <v>50</v>
-      </c>
-      <c r="E230" t="s">
-        <v>45</v>
-      </c>
-      <c r="F230" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="231">
-      <c r="B231" t="s">
-        <v>431</v>
-      </c>
-      <c r="C231" t="s">
-        <v>224</v>
-      </c>
-      <c r="D231" t="s">
-        <v>50</v>
-      </c>
-      <c r="E231" t="s">
-        <v>45</v>
-      </c>
-      <c r="F231" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="232">
-      <c r="B232" t="s">
-        <v>432</v>
-      </c>
-      <c r="C232" t="s">
-        <v>224</v>
-      </c>
-      <c r="D232" t="s">
-        <v>50</v>
-      </c>
-      <c r="E232" t="s">
-        <v>45</v>
-      </c>
-      <c r="F232" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="233">
-      <c r="B233" t="s">
-        <v>433</v>
-      </c>
-      <c r="C233" t="s">
-        <v>224</v>
-      </c>
-      <c r="D233" t="s">
-        <v>50</v>
-      </c>
-      <c r="E233" t="s">
-        <v>45</v>
-      </c>
-      <c r="F233" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="234">
-      <c r="B234" t="s">
-        <v>434</v>
-      </c>
-      <c r="C234" t="s">
-        <v>224</v>
-      </c>
-      <c r="D234" t="s">
-        <v>50</v>
-      </c>
-      <c r="E234" t="s">
-        <v>45</v>
-      </c>
-      <c r="F234" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="235">
-      <c r="B235" t="s">
-        <v>435</v>
-      </c>
-      <c r="C235" t="s">
-        <v>224</v>
-      </c>
-      <c r="D235" t="s">
-        <v>50</v>
-      </c>
-      <c r="E235" t="s">
-        <v>45</v>
-      </c>
-      <c r="F235" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="236">
-      <c r="B236" t="s">
-        <v>436</v>
-      </c>
-      <c r="C236" t="s">
-        <v>224</v>
-      </c>
-      <c r="D236" t="s">
-        <v>50</v>
-      </c>
-      <c r="E236" t="s">
-        <v>45</v>
-      </c>
-      <c r="F236" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="237">
-      <c r="B237" t="s">
-        <v>437</v>
-      </c>
-      <c r="C237" t="s">
-        <v>224</v>
-      </c>
-      <c r="D237" t="s">
-        <v>50</v>
-      </c>
-      <c r="E237" t="s">
-        <v>45</v>
-      </c>
-      <c r="F237" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="238">
-      <c r="B238" t="s">
-        <v>438</v>
-      </c>
-      <c r="C238" t="s">
-        <v>224</v>
-      </c>
-      <c r="D238" t="s">
-        <v>50</v>
-      </c>
-      <c r="E238" t="s">
-        <v>45</v>
-      </c>
-      <c r="F238" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="239">
-      <c r="B239" t="s">
-        <v>441</v>
-      </c>
-      <c r="C239" t="s">
-        <v>224</v>
-      </c>
-      <c r="D239" t="s">
-        <v>50</v>
-      </c>
-      <c r="E239" t="s">
-        <v>45</v>
-      </c>
-      <c r="F239" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="240">
-      <c r="B240" t="s">
-        <v>442</v>
-      </c>
-      <c r="C240" t="s">
-        <v>224</v>
-      </c>
-      <c r="D240" t="s">
-        <v>50</v>
-      </c>
-      <c r="E240" t="s">
-        <v>45</v>
-      </c>
-      <c r="F240" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="241">
-      <c r="B241" t="s">
-        <v>443</v>
-      </c>
-      <c r="C241" t="s">
-        <v>224</v>
-      </c>
-      <c r="D241" t="s">
-        <v>50</v>
-      </c>
-      <c r="E241" t="s">
-        <v>45</v>
-      </c>
-      <c r="F241" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="242">
-      <c r="B242" t="s">
-        <v>444</v>
-      </c>
-      <c r="C242" t="s">
-        <v>224</v>
-      </c>
-      <c r="D242" t="s">
-        <v>50</v>
-      </c>
-      <c r="E242" t="s">
-        <v>45</v>
-      </c>
-      <c r="F242" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="243">
-      <c r="B243" t="s">
-        <v>445</v>
-      </c>
-      <c r="C243" t="s">
-        <v>224</v>
-      </c>
-      <c r="D243" t="s">
-        <v>50</v>
-      </c>
-      <c r="E243" t="s">
-        <v>45</v>
-      </c>
-      <c r="F243" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="244">
-      <c r="B244" t="s">
-        <v>446</v>
-      </c>
-      <c r="C244" t="s">
-        <v>224</v>
-      </c>
-      <c r="D244" t="s">
-        <v>50</v>
-      </c>
-      <c r="E244" t="s">
-        <v>45</v>
-      </c>
-      <c r="F244" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="245">
-      <c r="B245" t="s">
-        <v>447</v>
-      </c>
-      <c r="C245" t="s">
-        <v>224</v>
-      </c>
-      <c r="D245" t="s">
-        <v>50</v>
-      </c>
-      <c r="E245" t="s">
-        <v>45</v>
-      </c>
-      <c r="F245" t="s">
-        <v>440</v>
-      </c>
-    </row>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="222"/>
+    <row r="223"/>
+    <row r="224"/>
+    <row r="225"/>
+    <row r="226"/>
+    <row r="227"/>
+    <row r="228"/>
+    <row r="229"/>
+    <row r="230"/>
+    <row r="231"/>
+    <row r="232"/>
+    <row r="233"/>
+    <row r="234"/>
+    <row r="235"/>
+    <row r="236"/>
+    <row r="237"/>
+    <row r="238"/>
+    <row r="239"/>
+    <row r="240"/>
+    <row r="241"/>
+    <row r="242"/>
+    <row r="243"/>
+    <row r="244"/>
+    <row r="245"/>
     <row r="246"/>
     <row r="247"/>
     <row r="248"/>

</xml_diff>

<commit_message>
Added button for repeat mode.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70336" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73106" uniqueCount="452">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -6680,8 +6680,40 @@
         <v>75</v>
       </c>
     </row>
-    <row r="222"/>
-    <row r="223"/>
+    <row r="222">
+      <c r="B222" t="s">
+        <v>429</v>
+      </c>
+      <c r="C222" t="s">
+        <v>38</v>
+      </c>
+      <c r="D222" t="s">
+        <v>44</v>
+      </c>
+      <c r="E222" t="s">
+        <v>45</v>
+      </c>
+      <c r="F222" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="B223" t="s">
+        <v>431</v>
+      </c>
+      <c r="C223" t="s">
+        <v>38</v>
+      </c>
+      <c r="D223" t="s">
+        <v>44</v>
+      </c>
+      <c r="E223" t="s">
+        <v>45</v>
+      </c>
+      <c r="F223" t="s">
+        <v>153</v>
+      </c>
+    </row>
     <row r="224"/>
     <row r="225"/>
     <row r="226"/>

</xml_diff>

<commit_message>
Added label to calibration screen UI.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73106" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74506" uniqueCount="454">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1390,6 +1390,12 @@
   </si>
   <si>
     <t xml:space="preserve">0x20-0x7E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MTC 108</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multichannel Time/Frequency Counter</t>
   </si>
 </sst>
 </file>
@@ -6714,8 +6720,40 @@
         <v>153</v>
       </c>
     </row>
-    <row r="224"/>
-    <row r="225"/>
+    <row r="224">
+      <c r="B224" t="s">
+        <v>432</v>
+      </c>
+      <c r="C224" t="s">
+        <v>40</v>
+      </c>
+      <c r="D224" t="s">
+        <v>50</v>
+      </c>
+      <c r="E224" t="s">
+        <v>45</v>
+      </c>
+      <c r="F224" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="B225" t="s">
+        <v>433</v>
+      </c>
+      <c r="C225" t="s">
+        <v>38</v>
+      </c>
+      <c r="D225" t="s">
+        <v>50</v>
+      </c>
+      <c r="E225" t="s">
+        <v>45</v>
+      </c>
+      <c r="F225" t="s">
+        <v>453</v>
+      </c>
+    </row>
     <row r="226"/>
     <row r="227"/>
     <row r="228"/>

</xml_diff>

<commit_message>
Developed graph for display measurement stamps in time mode.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74506" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81758" uniqueCount="480">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1396,6 +1396,84 @@
   </si>
   <si>
     <t xml:space="preserve">Multichannel Time/Frequency Counter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-., 0123456789</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ti 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ti 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ti 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ti 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ti 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ti 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ti 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Graph with the measurement values from stamps mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time interval 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time interval 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time interval 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId290</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time interval 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId291</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time interval 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId292</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time interval 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId293</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time interval 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId294</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Graph - Time interval 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId295</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId296</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Graph - Time interval  &lt;value&gt;</t>
   </si>
 </sst>
 </file>
@@ -2837,7 +2915,7 @@
         <v>288</v>
       </c>
       <c r="H10" t="s">
-        <v>42</v>
+        <v>454</v>
       </c>
       <c r="I10" t="s">
         <v>122</v>
@@ -6754,17 +6832,193 @@
         <v>453</v>
       </c>
     </row>
-    <row r="226"/>
-    <row r="227"/>
-    <row r="228"/>
-    <row r="229"/>
-    <row r="230"/>
-    <row r="231"/>
-    <row r="232"/>
-    <row r="233"/>
-    <row r="234"/>
-    <row r="235"/>
-    <row r="236"/>
+    <row r="226">
+      <c r="B226" t="s">
+        <v>445</v>
+      </c>
+      <c r="C226" t="s">
+        <v>205</v>
+      </c>
+      <c r="D226" t="s">
+        <v>50</v>
+      </c>
+      <c r="E226" t="s">
+        <v>45</v>
+      </c>
+      <c r="F226" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="B227" t="s">
+        <v>446</v>
+      </c>
+      <c r="C227" t="s">
+        <v>38</v>
+      </c>
+      <c r="D227" t="s">
+        <v>44</v>
+      </c>
+      <c r="E227" t="s">
+        <v>45</v>
+      </c>
+      <c r="F227" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="B228" t="s">
+        <v>447</v>
+      </c>
+      <c r="C228" t="s">
+        <v>38</v>
+      </c>
+      <c r="D228" t="s">
+        <v>44</v>
+      </c>
+      <c r="E228" t="s">
+        <v>45</v>
+      </c>
+      <c r="F228" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="B229" t="s">
+        <v>448</v>
+      </c>
+      <c r="C229" t="s">
+        <v>38</v>
+      </c>
+      <c r="D229" t="s">
+        <v>44</v>
+      </c>
+      <c r="E229" t="s">
+        <v>45</v>
+      </c>
+      <c r="F229" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="B230" t="s">
+        <v>467</v>
+      </c>
+      <c r="C230" t="s">
+        <v>38</v>
+      </c>
+      <c r="D230" t="s">
+        <v>44</v>
+      </c>
+      <c r="E230" t="s">
+        <v>45</v>
+      </c>
+      <c r="F230" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="B231" t="s">
+        <v>469</v>
+      </c>
+      <c r="C231" t="s">
+        <v>38</v>
+      </c>
+      <c r="D231" t="s">
+        <v>44</v>
+      </c>
+      <c r="E231" t="s">
+        <v>45</v>
+      </c>
+      <c r="F231" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="B232" t="s">
+        <v>471</v>
+      </c>
+      <c r="C232" t="s">
+        <v>38</v>
+      </c>
+      <c r="D232" t="s">
+        <v>44</v>
+      </c>
+      <c r="E232" t="s">
+        <v>45</v>
+      </c>
+      <c r="F232" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="B233" t="s">
+        <v>473</v>
+      </c>
+      <c r="C233" t="s">
+        <v>38</v>
+      </c>
+      <c r="D233" t="s">
+        <v>44</v>
+      </c>
+      <c r="E233" t="s">
+        <v>45</v>
+      </c>
+      <c r="F233" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="B234" t="s">
+        <v>475</v>
+      </c>
+      <c r="C234" t="s">
+        <v>205</v>
+      </c>
+      <c r="D234" t="s">
+        <v>50</v>
+      </c>
+      <c r="E234" t="s">
+        <v>45</v>
+      </c>
+      <c r="F234" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="B235" t="s">
+        <v>477</v>
+      </c>
+      <c r="C235" t="s">
+        <v>224</v>
+      </c>
+      <c r="D235" t="s">
+        <v>50</v>
+      </c>
+      <c r="E235" t="s">
+        <v>45</v>
+      </c>
+      <c r="F235" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="B236" t="s">
+        <v>478</v>
+      </c>
+      <c r="C236" t="s">
+        <v>224</v>
+      </c>
+      <c r="D236" t="s">
+        <v>259</v>
+      </c>
+      <c r="E236" t="s">
+        <v>45</v>
+      </c>
+      <c r="F236" t="s">
+        <v>455</v>
+      </c>
+    </row>
     <row r="237"/>
     <row r="238"/>
     <row r="239"/>

</xml_diff>

<commit_message>
Developed screen for graoh for frequency mode.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81758" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84816" uniqueCount="501">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1474,6 +1474,69 @@
   </si>
   <si>
     <t xml:space="preserve">Graph - Time interval  &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId297</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId298</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frequency measurement 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId299</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frequency measurement 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frequency measurement 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId301</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frequency measurement 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId302</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frequency measurement 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId303</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frequency measurement 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId304</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frequency measurement 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId305</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Frequency measurement 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId306</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Graph - Frequency Measurement &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId307</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId308</t>
   </si>
 </sst>
 </file>
@@ -7019,18 +7082,210 @@
         <v>455</v>
       </c>
     </row>
-    <row r="237"/>
-    <row r="238"/>
-    <row r="239"/>
-    <row r="240"/>
-    <row r="241"/>
-    <row r="242"/>
-    <row r="243"/>
-    <row r="244"/>
-    <row r="245"/>
-    <row r="246"/>
-    <row r="247"/>
-    <row r="248"/>
+    <row r="237">
+      <c r="B237" t="s">
+        <v>480</v>
+      </c>
+      <c r="C237" t="s">
+        <v>205</v>
+      </c>
+      <c r="D237" t="s">
+        <v>50</v>
+      </c>
+      <c r="E237" t="s">
+        <v>45</v>
+      </c>
+      <c r="F237" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="B238" t="s">
+        <v>481</v>
+      </c>
+      <c r="C238" t="s">
+        <v>38</v>
+      </c>
+      <c r="D238" t="s">
+        <v>44</v>
+      </c>
+      <c r="E238" t="s">
+        <v>45</v>
+      </c>
+      <c r="F238" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="B239" t="s">
+        <v>483</v>
+      </c>
+      <c r="C239" t="s">
+        <v>38</v>
+      </c>
+      <c r="D239" t="s">
+        <v>44</v>
+      </c>
+      <c r="E239" t="s">
+        <v>45</v>
+      </c>
+      <c r="F239" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="B240" t="s">
+        <v>485</v>
+      </c>
+      <c r="C240" t="s">
+        <v>38</v>
+      </c>
+      <c r="D240" t="s">
+        <v>44</v>
+      </c>
+      <c r="E240" t="s">
+        <v>45</v>
+      </c>
+      <c r="F240" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="B241" t="s">
+        <v>487</v>
+      </c>
+      <c r="C241" t="s">
+        <v>38</v>
+      </c>
+      <c r="D241" t="s">
+        <v>44</v>
+      </c>
+      <c r="E241" t="s">
+        <v>45</v>
+      </c>
+      <c r="F241" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="B242" t="s">
+        <v>489</v>
+      </c>
+      <c r="C242" t="s">
+        <v>38</v>
+      </c>
+      <c r="D242" t="s">
+        <v>44</v>
+      </c>
+      <c r="E242" t="s">
+        <v>45</v>
+      </c>
+      <c r="F242" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="B243" t="s">
+        <v>491</v>
+      </c>
+      <c r="C243" t="s">
+        <v>38</v>
+      </c>
+      <c r="D243" t="s">
+        <v>44</v>
+      </c>
+      <c r="E243" t="s">
+        <v>45</v>
+      </c>
+      <c r="F243" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="B244" t="s">
+        <v>493</v>
+      </c>
+      <c r="C244" t="s">
+        <v>38</v>
+      </c>
+      <c r="D244" t="s">
+        <v>44</v>
+      </c>
+      <c r="E244" t="s">
+        <v>45</v>
+      </c>
+      <c r="F244" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="B245" t="s">
+        <v>495</v>
+      </c>
+      <c r="C245" t="s">
+        <v>38</v>
+      </c>
+      <c r="D245" t="s">
+        <v>44</v>
+      </c>
+      <c r="E245" t="s">
+        <v>45</v>
+      </c>
+      <c r="F245" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="B246" t="s">
+        <v>497</v>
+      </c>
+      <c r="C246" t="s">
+        <v>205</v>
+      </c>
+      <c r="D246" t="s">
+        <v>50</v>
+      </c>
+      <c r="E246" t="s">
+        <v>45</v>
+      </c>
+      <c r="F246" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="B247" t="s">
+        <v>499</v>
+      </c>
+      <c r="C247" t="s">
+        <v>224</v>
+      </c>
+      <c r="D247" t="s">
+        <v>50</v>
+      </c>
+      <c r="E247" t="s">
+        <v>45</v>
+      </c>
+      <c r="F247" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="B248" t="s">
+        <v>500</v>
+      </c>
+      <c r="C248" t="s">
+        <v>224</v>
+      </c>
+      <c r="D248" t="s">
+        <v>259</v>
+      </c>
+      <c r="E248" t="s">
+        <v>45</v>
+      </c>
+      <c r="F248" t="s">
+        <v>455</v>
+      </c>
+    </row>
     <row r="249"/>
     <row r="250"/>
     <row r="251"/>

</xml_diff>

<commit_message>
Reorganized elements in UI.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86342" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87850" uniqueCount="501">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -3548,24 +3548,24 @@
     </row>
     <row r="29">
       <c r="B29" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C29" t="s">
         <v>38</v>
       </c>
       <c r="D29" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E29" t="s">
         <v>45</v>
       </c>
       <c r="F29" t="s">
-        <v>75</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="s">
-        <v>101</v>
+        <v>124</v>
       </c>
       <c r="C30" t="s">
         <v>38</v>
@@ -3577,29 +3577,29 @@
         <v>45</v>
       </c>
       <c r="F30" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="C31" t="s">
         <v>38</v>
       </c>
       <c r="D31" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E31" t="s">
         <v>45</v>
       </c>
       <c r="F31" t="s">
-        <v>125</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C32" t="s">
         <v>38</v>
@@ -3611,29 +3611,29 @@
         <v>45</v>
       </c>
       <c r="F32" t="s">
-        <v>128</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="C33" t="s">
         <v>38</v>
       </c>
       <c r="D33" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E33" t="s">
         <v>45</v>
       </c>
       <c r="F33" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34">
       <c r="B34" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="C34" t="s">
         <v>38</v>
@@ -3645,12 +3645,12 @@
         <v>45</v>
       </c>
       <c r="F34" t="s">
-        <v>75</v>
+        <v>143</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" t="s">
-        <v>131</v>
+        <v>146</v>
       </c>
       <c r="C35" t="s">
         <v>38</v>
@@ -3667,7 +3667,7 @@
     </row>
     <row r="36">
       <c r="B36" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="C36" t="s">
         <v>38</v>
@@ -3679,49 +3679,49 @@
         <v>45</v>
       </c>
       <c r="F36" t="s">
-        <v>133</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37">
       <c r="B37" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="C37" t="s">
         <v>38</v>
       </c>
       <c r="D37" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E37" t="s">
         <v>45</v>
       </c>
       <c r="F37" t="s">
-        <v>143</v>
+        <v>102</v>
       </c>
     </row>
     <row r="38">
       <c r="B38" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C38" t="s">
         <v>38</v>
       </c>
       <c r="D38" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E38" t="s">
         <v>45</v>
       </c>
       <c r="F38" t="s">
-        <v>75</v>
+        <v>137</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C39" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D39" t="s">
         <v>50</v>
@@ -3730,12 +3730,12 @@
         <v>45</v>
       </c>
       <c r="F39" t="s">
-        <v>102</v>
+        <v>151</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="C40" t="s">
         <v>38</v>
@@ -3747,32 +3747,32 @@
         <v>45</v>
       </c>
       <c r="F40" t="s">
-        <v>102</v>
+        <v>153</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="C41" t="s">
         <v>38</v>
       </c>
       <c r="D41" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E41" t="s">
         <v>45</v>
       </c>
       <c r="F41" t="s">
-        <v>137</v>
+        <v>75</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C42" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D42" t="s">
         <v>50</v>
@@ -3781,12 +3781,12 @@
         <v>45</v>
       </c>
       <c r="F42" t="s">
-        <v>151</v>
+        <v>102</v>
       </c>
     </row>
     <row r="43">
       <c r="B43" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="C43" t="s">
         <v>38</v>
@@ -3798,63 +3798,63 @@
         <v>45</v>
       </c>
       <c r="F43" t="s">
-        <v>153</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44">
       <c r="B44" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="C44" t="s">
         <v>38</v>
       </c>
       <c r="D44" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E44" t="s">
         <v>45</v>
       </c>
       <c r="F44" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
     </row>
     <row r="45">
       <c r="B45" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="C45" t="s">
         <v>38</v>
       </c>
       <c r="D45" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E45" t="s">
         <v>45</v>
       </c>
       <c r="F45" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
     </row>
     <row r="46">
       <c r="B46" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C46" t="s">
         <v>38</v>
       </c>
       <c r="D46" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E46" t="s">
         <v>45</v>
       </c>
       <c r="F46" t="s">
-        <v>85</v>
+        <v>115</v>
       </c>
     </row>
     <row r="47">
       <c r="B47" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="C47" t="s">
         <v>38</v>
@@ -3866,29 +3866,29 @@
         <v>45</v>
       </c>
       <c r="F47" t="s">
-        <v>83</v>
+        <v>102</v>
       </c>
     </row>
     <row r="48">
       <c r="B48" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="C48" t="s">
         <v>38</v>
       </c>
       <c r="D48" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E48" t="s">
         <v>45</v>
       </c>
       <c r="F48" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
     </row>
     <row r="49">
       <c r="B49" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="C49" t="s">
         <v>38</v>
@@ -3900,29 +3900,29 @@
         <v>45</v>
       </c>
       <c r="F49" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="50">
       <c r="B50" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="C50" t="s">
         <v>38</v>
       </c>
       <c r="D50" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E50" t="s">
         <v>45</v>
       </c>
       <c r="F50" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="51">
       <c r="B51" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C51" t="s">
         <v>38</v>
@@ -3934,46 +3934,46 @@
         <v>45</v>
       </c>
       <c r="F51" t="s">
-        <v>108</v>
+        <v>175</v>
       </c>
     </row>
     <row r="52">
       <c r="B52" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="C52" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D52" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E52" t="s">
         <v>45</v>
       </c>
       <c r="F52" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
     </row>
     <row r="53">
       <c r="B53" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="C53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D53" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E53" t="s">
         <v>45</v>
       </c>
       <c r="F53" t="s">
-        <v>103</v>
+        <v>129</v>
       </c>
     </row>
     <row r="54">
       <c r="B54" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C54" t="s">
         <v>38</v>
@@ -3985,32 +3985,32 @@
         <v>45</v>
       </c>
       <c r="F54" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
     </row>
     <row r="55">
       <c r="B55" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="C55" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D55" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E55" t="s">
         <v>45</v>
       </c>
       <c r="F55" t="s">
-        <v>128</v>
+        <v>143</v>
       </c>
     </row>
     <row r="56">
       <c r="B56" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="C56" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D56" t="s">
         <v>50</v>
@@ -4019,46 +4019,46 @@
         <v>45</v>
       </c>
       <c r="F56" t="s">
-        <v>129</v>
+        <v>67</v>
       </c>
     </row>
     <row r="57">
       <c r="B57" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C57" t="s">
         <v>38</v>
       </c>
       <c r="D57" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E57" t="s">
         <v>45</v>
       </c>
       <c r="F57" t="s">
-        <v>179</v>
+        <v>75</v>
       </c>
     </row>
     <row r="58">
       <c r="B58" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="C58" t="s">
         <v>38</v>
       </c>
       <c r="D58" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E58" t="s">
         <v>45</v>
       </c>
       <c r="F58" t="s">
-        <v>143</v>
+        <v>102</v>
       </c>
     </row>
     <row r="59">
       <c r="B59" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="C59" t="s">
         <v>38</v>
@@ -4070,29 +4070,29 @@
         <v>45</v>
       </c>
       <c r="F59" t="s">
-        <v>67</v>
+        <v>137</v>
       </c>
     </row>
     <row r="60">
       <c r="B60" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C60" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D60" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E60" t="s">
         <v>45</v>
       </c>
       <c r="F60" t="s">
-        <v>75</v>
+        <v>151</v>
       </c>
     </row>
     <row r="61">
       <c r="B61" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="C61" t="s">
         <v>38</v>
@@ -4104,32 +4104,32 @@
         <v>45</v>
       </c>
       <c r="F61" t="s">
-        <v>102</v>
+        <v>153</v>
       </c>
     </row>
     <row r="62">
       <c r="B62" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C62" t="s">
         <v>38</v>
       </c>
       <c r="D62" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E62" t="s">
         <v>45</v>
       </c>
       <c r="F62" t="s">
-        <v>137</v>
+        <v>75</v>
       </c>
     </row>
     <row r="63">
       <c r="B63" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="C63" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D63" t="s">
         <v>50</v>
@@ -4138,29 +4138,29 @@
         <v>45</v>
       </c>
       <c r="F63" t="s">
-        <v>151</v>
+        <v>102</v>
       </c>
     </row>
     <row r="64">
       <c r="B64" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="C64" t="s">
         <v>38</v>
       </c>
       <c r="D64" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E64" t="s">
         <v>45</v>
       </c>
       <c r="F64" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
     </row>
     <row r="65">
       <c r="B65" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="C65" t="s">
         <v>38</v>
@@ -4172,29 +4172,29 @@
         <v>45</v>
       </c>
       <c r="F65" t="s">
-        <v>75</v>
+        <v>145</v>
       </c>
     </row>
     <row r="66">
       <c r="B66" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="C66" t="s">
         <v>38</v>
       </c>
       <c r="D66" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E66" t="s">
         <v>45</v>
       </c>
       <c r="F66" t="s">
-        <v>102</v>
+        <v>197</v>
       </c>
     </row>
     <row r="67">
       <c r="B67" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="C67" t="s">
         <v>38</v>
@@ -4211,7 +4211,7 @@
     </row>
     <row r="68">
       <c r="B68" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="C68" t="s">
         <v>38</v>
@@ -4228,7 +4228,7 @@
     </row>
     <row r="69">
       <c r="B69" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="C69" t="s">
         <v>38</v>
@@ -4245,58 +4245,58 @@
     </row>
     <row r="70">
       <c r="B70" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="C70" t="s">
-        <v>38</v>
+        <v>205</v>
       </c>
       <c r="D70" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E70" t="s">
         <v>45</v>
       </c>
       <c r="F70" t="s">
-        <v>135</v>
+        <v>328</v>
       </c>
     </row>
     <row r="71">
       <c r="B71" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="C71" t="s">
-        <v>38</v>
+        <v>205</v>
       </c>
       <c r="D71" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E71" t="s">
         <v>45</v>
       </c>
       <c r="F71" t="s">
-        <v>145</v>
+        <v>204</v>
       </c>
     </row>
     <row r="72">
       <c r="B72" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="C72" t="s">
-        <v>38</v>
+        <v>205</v>
       </c>
       <c r="D72" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E72" t="s">
         <v>45</v>
       </c>
       <c r="F72" t="s">
-        <v>197</v>
+        <v>328</v>
       </c>
     </row>
     <row r="73">
       <c r="B73" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="C73" t="s">
         <v>205</v>
@@ -4308,12 +4308,12 @@
         <v>45</v>
       </c>
       <c r="F73" t="s">
-        <v>328</v>
+        <v>204</v>
       </c>
     </row>
     <row r="74">
       <c r="B74" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="C74" t="s">
         <v>205</v>
@@ -4325,12 +4325,12 @@
         <v>45</v>
       </c>
       <c r="F74" t="s">
-        <v>204</v>
+        <v>328</v>
       </c>
     </row>
     <row r="75">
       <c r="B75" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="C75" t="s">
         <v>205</v>
@@ -4342,12 +4342,12 @@
         <v>45</v>
       </c>
       <c r="F75" t="s">
-        <v>328</v>
+        <v>204</v>
       </c>
     </row>
     <row r="76">
       <c r="B76" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="C76" t="s">
         <v>205</v>
@@ -4359,12 +4359,12 @@
         <v>45</v>
       </c>
       <c r="F76" t="s">
-        <v>204</v>
+        <v>328</v>
       </c>
     </row>
     <row r="77">
       <c r="B77" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="C77" t="s">
         <v>205</v>
@@ -4376,12 +4376,12 @@
         <v>45</v>
       </c>
       <c r="F77" t="s">
-        <v>328</v>
+        <v>204</v>
       </c>
     </row>
     <row r="78">
       <c r="B78" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="C78" t="s">
         <v>205</v>
@@ -4393,12 +4393,12 @@
         <v>45</v>
       </c>
       <c r="F78" t="s">
-        <v>204</v>
+        <v>328</v>
       </c>
     </row>
     <row r="79">
       <c r="B79" t="s">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="C79" t="s">
         <v>205</v>
@@ -4410,12 +4410,12 @@
         <v>45</v>
       </c>
       <c r="F79" t="s">
-        <v>328</v>
+        <v>204</v>
       </c>
     </row>
     <row r="80">
       <c r="B80" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="C80" t="s">
         <v>205</v>
@@ -4427,12 +4427,12 @@
         <v>45</v>
       </c>
       <c r="F80" t="s">
-        <v>204</v>
+        <v>328</v>
       </c>
     </row>
     <row r="81">
       <c r="B81" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="C81" t="s">
         <v>205</v>
@@ -4444,12 +4444,12 @@
         <v>45</v>
       </c>
       <c r="F81" t="s">
-        <v>328</v>
+        <v>204</v>
       </c>
     </row>
     <row r="82">
       <c r="B82" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C82" t="s">
         <v>205</v>
@@ -4461,12 +4461,12 @@
         <v>45</v>
       </c>
       <c r="F82" t="s">
-        <v>204</v>
+        <v>328</v>
       </c>
     </row>
     <row r="83">
       <c r="B83" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
       <c r="C83" t="s">
         <v>205</v>
@@ -4478,15 +4478,15 @@
         <v>45</v>
       </c>
       <c r="F83" t="s">
-        <v>328</v>
+        <v>204</v>
       </c>
     </row>
     <row r="84">
       <c r="B84" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="C84" t="s">
-        <v>205</v>
+        <v>224</v>
       </c>
       <c r="D84" t="s">
         <v>50</v>
@@ -4495,15 +4495,15 @@
         <v>45</v>
       </c>
       <c r="F84" t="s">
-        <v>204</v>
+        <v>273</v>
       </c>
     </row>
     <row r="85">
       <c r="B85" t="s">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="C85" t="s">
-        <v>205</v>
+        <v>225</v>
       </c>
       <c r="D85" t="s">
         <v>50</v>
@@ -4512,15 +4512,15 @@
         <v>45</v>
       </c>
       <c r="F85" t="s">
-        <v>328</v>
+        <v>230</v>
       </c>
     </row>
     <row r="86">
       <c r="B86" t="s">
-        <v>223</v>
+        <v>231</v>
       </c>
       <c r="C86" t="s">
-        <v>205</v>
+        <v>225</v>
       </c>
       <c r="D86" t="s">
         <v>50</v>
@@ -4529,12 +4529,12 @@
         <v>45</v>
       </c>
       <c r="F86" t="s">
-        <v>204</v>
+        <v>232</v>
       </c>
     </row>
     <row r="87">
       <c r="B87" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="C87" t="s">
         <v>224</v>
@@ -4551,27 +4551,27 @@
     </row>
     <row r="88">
       <c r="B88" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="C88" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D88" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E88" t="s">
         <v>45</v>
       </c>
       <c r="F88" t="s">
-        <v>230</v>
+        <v>75</v>
       </c>
     </row>
     <row r="89">
       <c r="B89" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="C89" t="s">
-        <v>225</v>
+        <v>205</v>
       </c>
       <c r="D89" t="s">
         <v>50</v>
@@ -4580,15 +4580,15 @@
         <v>45</v>
       </c>
       <c r="F89" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
     </row>
     <row r="90">
       <c r="B90" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="C90" t="s">
-        <v>224</v>
+        <v>205</v>
       </c>
       <c r="D90" t="s">
         <v>50</v>
@@ -4597,32 +4597,32 @@
         <v>45</v>
       </c>
       <c r="F90" t="s">
-        <v>273</v>
+        <v>238</v>
       </c>
     </row>
     <row r="91">
       <c r="B91" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="C91" t="s">
         <v>224</v>
       </c>
       <c r="D91" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E91" t="s">
         <v>45</v>
       </c>
       <c r="F91" t="s">
-        <v>75</v>
+        <v>273</v>
       </c>
     </row>
     <row r="92">
       <c r="B92" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="C92" t="s">
-        <v>205</v>
+        <v>224</v>
       </c>
       <c r="D92" t="s">
         <v>50</v>
@@ -4631,15 +4631,15 @@
         <v>45</v>
       </c>
       <c r="F92" t="s">
-        <v>236</v>
+        <v>273</v>
       </c>
     </row>
     <row r="93">
       <c r="B93" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="C93" t="s">
-        <v>205</v>
+        <v>224</v>
       </c>
       <c r="D93" t="s">
         <v>50</v>
@@ -4648,12 +4648,12 @@
         <v>45</v>
       </c>
       <c r="F93" t="s">
-        <v>238</v>
+        <v>273</v>
       </c>
     </row>
     <row r="94">
       <c r="B94" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="C94" t="s">
         <v>224</v>
@@ -4670,7 +4670,7 @@
     </row>
     <row r="95">
       <c r="B95" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="C95" t="s">
         <v>224</v>
@@ -4687,7 +4687,7 @@
     </row>
     <row r="96">
       <c r="B96" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="C96" t="s">
         <v>224</v>
@@ -4704,7 +4704,7 @@
     </row>
     <row r="97">
       <c r="B97" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="C97" t="s">
         <v>224</v>
@@ -4721,7 +4721,7 @@
     </row>
     <row r="98">
       <c r="B98" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="C98" t="s">
         <v>224</v>
@@ -4738,7 +4738,7 @@
     </row>
     <row r="99">
       <c r="B99" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="C99" t="s">
         <v>224</v>
@@ -4755,7 +4755,7 @@
     </row>
     <row r="100">
       <c r="B100" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C100" t="s">
         <v>224</v>
@@ -4772,7 +4772,7 @@
     </row>
     <row r="101">
       <c r="B101" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="C101" t="s">
         <v>224</v>
@@ -4789,7 +4789,7 @@
     </row>
     <row r="102">
       <c r="B102" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="C102" t="s">
         <v>224</v>
@@ -4806,58 +4806,58 @@
     </row>
     <row r="103">
       <c r="B103" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C103" t="s">
         <v>224</v>
       </c>
       <c r="D103" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E103" t="s">
         <v>45</v>
       </c>
       <c r="F103" t="s">
-        <v>273</v>
+        <v>75</v>
       </c>
     </row>
     <row r="104">
       <c r="B104" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="C104" t="s">
         <v>224</v>
       </c>
       <c r="D104" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E104" t="s">
         <v>45</v>
       </c>
       <c r="F104" t="s">
-        <v>273</v>
+        <v>75</v>
       </c>
     </row>
     <row r="105">
       <c r="B105" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="C105" t="s">
         <v>224</v>
       </c>
       <c r="D105" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E105" t="s">
         <v>45</v>
       </c>
       <c r="F105" t="s">
-        <v>273</v>
+        <v>75</v>
       </c>
     </row>
     <row r="106">
       <c r="B106" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C106" t="s">
         <v>224</v>
@@ -4874,7 +4874,7 @@
     </row>
     <row r="107">
       <c r="B107" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="C107" t="s">
         <v>224</v>
@@ -4891,7 +4891,7 @@
     </row>
     <row r="108">
       <c r="B108" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="C108" t="s">
         <v>224</v>
@@ -4908,13 +4908,13 @@
     </row>
     <row r="109">
       <c r="B109" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="C109" t="s">
-        <v>224</v>
+        <v>257</v>
       </c>
       <c r="D109" t="s">
-        <v>44</v>
+        <v>259</v>
       </c>
       <c r="E109" t="s">
         <v>45</v>
@@ -4925,13 +4925,13 @@
     </row>
     <row r="110">
       <c r="B110" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="C110" t="s">
-        <v>224</v>
+        <v>257</v>
       </c>
       <c r="D110" t="s">
-        <v>44</v>
+        <v>259</v>
       </c>
       <c r="E110" t="s">
         <v>45</v>
@@ -4942,13 +4942,13 @@
     </row>
     <row r="111">
       <c r="B111" t="s">
-        <v>256</v>
+        <v>261</v>
       </c>
       <c r="C111" t="s">
-        <v>224</v>
+        <v>257</v>
       </c>
       <c r="D111" t="s">
-        <v>44</v>
+        <v>259</v>
       </c>
       <c r="E111" t="s">
         <v>45</v>
@@ -4959,7 +4959,7 @@
     </row>
     <row r="112">
       <c r="B112" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="C112" t="s">
         <v>257</v>
@@ -4976,7 +4976,7 @@
     </row>
     <row r="113">
       <c r="B113" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="C113" t="s">
         <v>257</v>
@@ -4993,7 +4993,7 @@
     </row>
     <row r="114">
       <c r="B114" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="C114" t="s">
         <v>257</v>
@@ -5010,7 +5010,7 @@
     </row>
     <row r="115">
       <c r="B115" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="C115" t="s">
         <v>257</v>
@@ -5027,7 +5027,7 @@
     </row>
     <row r="116">
       <c r="B116" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="C116" t="s">
         <v>257</v>
@@ -5044,7 +5044,7 @@
     </row>
     <row r="117">
       <c r="B117" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="C117" t="s">
         <v>257</v>
@@ -5061,7 +5061,7 @@
     </row>
     <row r="118">
       <c r="B118" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="C118" t="s">
         <v>257</v>
@@ -5078,7 +5078,7 @@
     </row>
     <row r="119">
       <c r="B119" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="C119" t="s">
         <v>257</v>
@@ -5095,7 +5095,7 @@
     </row>
     <row r="120">
       <c r="B120" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="C120" t="s">
         <v>257</v>
@@ -5112,7 +5112,7 @@
     </row>
     <row r="121">
       <c r="B121" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="C121" t="s">
         <v>257</v>
@@ -5129,7 +5129,7 @@
     </row>
     <row r="122">
       <c r="B122" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="C122" t="s">
         <v>257</v>
@@ -5146,13 +5146,13 @@
     </row>
     <row r="123">
       <c r="B123" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="C123" t="s">
-        <v>257</v>
+        <v>224</v>
       </c>
       <c r="D123" t="s">
-        <v>259</v>
+        <v>44</v>
       </c>
       <c r="E123" t="s">
         <v>45</v>
@@ -5163,13 +5163,13 @@
     </row>
     <row r="124">
       <c r="B124" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="C124" t="s">
-        <v>257</v>
+        <v>224</v>
       </c>
       <c r="D124" t="s">
-        <v>259</v>
+        <v>44</v>
       </c>
       <c r="E124" t="s">
         <v>45</v>
@@ -5180,13 +5180,13 @@
     </row>
     <row r="125">
       <c r="B125" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="C125" t="s">
-        <v>257</v>
+        <v>224</v>
       </c>
       <c r="D125" t="s">
-        <v>259</v>
+        <v>44</v>
       </c>
       <c r="E125" t="s">
         <v>45</v>
@@ -5197,7 +5197,7 @@
     </row>
     <row r="126">
       <c r="B126" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="C126" t="s">
         <v>224</v>
@@ -5214,7 +5214,7 @@
     </row>
     <row r="127">
       <c r="B127" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="C127" t="s">
         <v>224</v>
@@ -5231,7 +5231,7 @@
     </row>
     <row r="128">
       <c r="B128" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="C128" t="s">
         <v>224</v>
@@ -5248,7 +5248,7 @@
     </row>
     <row r="129">
       <c r="B129" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="C129" t="s">
         <v>224</v>
@@ -5265,7 +5265,7 @@
     </row>
     <row r="130">
       <c r="B130" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="C130" t="s">
         <v>224</v>
@@ -5282,7 +5282,7 @@
     </row>
     <row r="131">
       <c r="B131" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="C131" t="s">
         <v>224</v>
@@ -5299,7 +5299,7 @@
     </row>
     <row r="132">
       <c r="B132" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="C132" t="s">
         <v>224</v>
@@ -5316,7 +5316,7 @@
     </row>
     <row r="133">
       <c r="B133" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="C133" t="s">
         <v>224</v>
@@ -5333,7 +5333,7 @@
     </row>
     <row r="134">
       <c r="B134" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="C134" t="s">
         <v>224</v>
@@ -5350,7 +5350,7 @@
     </row>
     <row r="135">
       <c r="B135" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="C135" t="s">
         <v>224</v>
@@ -5367,7 +5367,7 @@
     </row>
     <row r="136">
       <c r="B136" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="C136" t="s">
         <v>224</v>
@@ -5384,7 +5384,7 @@
     </row>
     <row r="137">
       <c r="B137" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="C137" t="s">
         <v>224</v>
@@ -5401,7 +5401,7 @@
     </row>
     <row r="138">
       <c r="B138" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="C138" t="s">
         <v>224</v>
@@ -5418,7 +5418,7 @@
     </row>
     <row r="139">
       <c r="B139" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="C139" t="s">
         <v>224</v>
@@ -5435,7 +5435,7 @@
     </row>
     <row r="140">
       <c r="B140" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="C140" t="s">
         <v>224</v>
@@ -5452,7 +5452,7 @@
     </row>
     <row r="141">
       <c r="B141" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="C141" t="s">
         <v>224</v>
@@ -5469,7 +5469,7 @@
     </row>
     <row r="142">
       <c r="B142" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="C142" t="s">
         <v>224</v>
@@ -5486,7 +5486,7 @@
     </row>
     <row r="143">
       <c r="B143" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="C143" t="s">
         <v>224</v>
@@ -5503,7 +5503,7 @@
     </row>
     <row r="144">
       <c r="B144" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="C144" t="s">
         <v>224</v>
@@ -5520,7 +5520,7 @@
     </row>
     <row r="145">
       <c r="B145" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="C145" t="s">
         <v>224</v>
@@ -5537,7 +5537,7 @@
     </row>
     <row r="146">
       <c r="B146" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="C146" t="s">
         <v>224</v>
@@ -5554,7 +5554,7 @@
     </row>
     <row r="147">
       <c r="B147" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="C147" t="s">
         <v>224</v>
@@ -5571,7 +5571,7 @@
     </row>
     <row r="148">
       <c r="B148" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="C148" t="s">
         <v>224</v>
@@ -5588,7 +5588,7 @@
     </row>
     <row r="149">
       <c r="B149" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="C149" t="s">
         <v>224</v>
@@ -5605,7 +5605,7 @@
     </row>
     <row r="150">
       <c r="B150" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="C150" t="s">
         <v>224</v>
@@ -5622,58 +5622,58 @@
     </row>
     <row r="151">
       <c r="B151" t="s">
-        <v>301</v>
+        <v>329</v>
       </c>
       <c r="C151" t="s">
-        <v>224</v>
+        <v>205</v>
       </c>
       <c r="D151" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E151" t="s">
         <v>45</v>
       </c>
       <c r="F151" t="s">
-        <v>75</v>
+        <v>330</v>
       </c>
     </row>
     <row r="152">
       <c r="B152" t="s">
-        <v>302</v>
+        <v>331</v>
       </c>
       <c r="C152" t="s">
-        <v>224</v>
+        <v>205</v>
       </c>
       <c r="D152" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E152" t="s">
         <v>45</v>
       </c>
       <c r="F152" t="s">
-        <v>75</v>
+        <v>332</v>
       </c>
     </row>
     <row r="153">
       <c r="B153" t="s">
-        <v>303</v>
+        <v>333</v>
       </c>
       <c r="C153" t="s">
-        <v>224</v>
+        <v>205</v>
       </c>
       <c r="D153" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E153" t="s">
         <v>45</v>
       </c>
       <c r="F153" t="s">
-        <v>75</v>
+        <v>334</v>
       </c>
     </row>
     <row r="154">
       <c r="B154" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="C154" t="s">
         <v>205</v>
@@ -5685,12 +5685,12 @@
         <v>45</v>
       </c>
       <c r="F154" t="s">
-        <v>330</v>
+        <v>336</v>
       </c>
     </row>
     <row r="155">
       <c r="B155" t="s">
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="C155" t="s">
         <v>205</v>
@@ -5702,12 +5702,12 @@
         <v>45</v>
       </c>
       <c r="F155" t="s">
-        <v>332</v>
+        <v>338</v>
       </c>
     </row>
     <row r="156">
       <c r="B156" t="s">
-        <v>333</v>
+        <v>339</v>
       </c>
       <c r="C156" t="s">
         <v>205</v>
@@ -5719,12 +5719,12 @@
         <v>45</v>
       </c>
       <c r="F156" t="s">
-        <v>334</v>
+        <v>340</v>
       </c>
     </row>
     <row r="157">
       <c r="B157" t="s">
-        <v>335</v>
+        <v>341</v>
       </c>
       <c r="C157" t="s">
         <v>205</v>
@@ -5736,12 +5736,12 @@
         <v>45</v>
       </c>
       <c r="F157" t="s">
-        <v>336</v>
+        <v>342</v>
       </c>
     </row>
     <row r="158">
       <c r="B158" t="s">
-        <v>337</v>
+        <v>343</v>
       </c>
       <c r="C158" t="s">
         <v>205</v>
@@ -5753,12 +5753,12 @@
         <v>45</v>
       </c>
       <c r="F158" t="s">
-        <v>338</v>
+        <v>344</v>
       </c>
     </row>
     <row r="159">
       <c r="B159" t="s">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="C159" t="s">
         <v>205</v>
@@ -5770,12 +5770,12 @@
         <v>45</v>
       </c>
       <c r="F159" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
     </row>
     <row r="160">
       <c r="B160" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="C160" t="s">
         <v>205</v>
@@ -5787,12 +5787,12 @@
         <v>45</v>
       </c>
       <c r="F160" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="161">
       <c r="B161" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="C161" t="s">
         <v>205</v>
@@ -5809,7 +5809,7 @@
     </row>
     <row r="162">
       <c r="B162" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="C162" t="s">
         <v>205</v>
@@ -5826,7 +5826,7 @@
     </row>
     <row r="163">
       <c r="B163" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="C163" t="s">
         <v>205</v>
@@ -5843,7 +5843,7 @@
     </row>
     <row r="164">
       <c r="B164" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="C164" t="s">
         <v>205</v>
@@ -5860,7 +5860,7 @@
     </row>
     <row r="165">
       <c r="B165" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="C165" t="s">
         <v>205</v>
@@ -5872,12 +5872,12 @@
         <v>45</v>
       </c>
       <c r="F165" t="s">
-        <v>344</v>
+        <v>352</v>
       </c>
     </row>
     <row r="166">
       <c r="B166" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="C166" t="s">
         <v>205</v>
@@ -5889,12 +5889,12 @@
         <v>45</v>
       </c>
       <c r="F166" t="s">
-        <v>344</v>
+        <v>354</v>
       </c>
     </row>
     <row r="167">
       <c r="B167" t="s">
-        <v>350</v>
+        <v>355</v>
       </c>
       <c r="C167" t="s">
         <v>205</v>
@@ -5906,12 +5906,12 @@
         <v>45</v>
       </c>
       <c r="F167" t="s">
-        <v>344</v>
+        <v>356</v>
       </c>
     </row>
     <row r="168">
       <c r="B168" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="C168" t="s">
         <v>205</v>
@@ -5923,12 +5923,12 @@
         <v>45</v>
       </c>
       <c r="F168" t="s">
-        <v>352</v>
+        <v>358</v>
       </c>
     </row>
     <row r="169">
       <c r="B169" t="s">
-        <v>353</v>
+        <v>359</v>
       </c>
       <c r="C169" t="s">
         <v>205</v>
@@ -5940,12 +5940,12 @@
         <v>45</v>
       </c>
       <c r="F169" t="s">
-        <v>354</v>
+        <v>360</v>
       </c>
     </row>
     <row r="170">
       <c r="B170" t="s">
-        <v>355</v>
+        <v>361</v>
       </c>
       <c r="C170" t="s">
         <v>205</v>
@@ -5957,12 +5957,12 @@
         <v>45</v>
       </c>
       <c r="F170" t="s">
-        <v>356</v>
+        <v>362</v>
       </c>
     </row>
     <row r="171">
       <c r="B171" t="s">
-        <v>357</v>
+        <v>363</v>
       </c>
       <c r="C171" t="s">
         <v>205</v>
@@ -5974,12 +5974,12 @@
         <v>45</v>
       </c>
       <c r="F171" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
     </row>
     <row r="172">
       <c r="B172" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="C172" t="s">
         <v>205</v>
@@ -5991,12 +5991,12 @@
         <v>45</v>
       </c>
       <c r="F172" t="s">
-        <v>360</v>
+        <v>344</v>
       </c>
     </row>
     <row r="173">
       <c r="B173" t="s">
-        <v>361</v>
+        <v>366</v>
       </c>
       <c r="C173" t="s">
         <v>205</v>
@@ -6008,15 +6008,15 @@
         <v>45</v>
       </c>
       <c r="F173" t="s">
-        <v>362</v>
+        <v>367</v>
       </c>
     </row>
     <row r="174">
       <c r="B174" t="s">
-        <v>363</v>
+        <v>368</v>
       </c>
       <c r="C174" t="s">
-        <v>205</v>
+        <v>225</v>
       </c>
       <c r="D174" t="s">
         <v>50</v>
@@ -6025,12 +6025,12 @@
         <v>45</v>
       </c>
       <c r="F174" t="s">
-        <v>364</v>
+        <v>232</v>
       </c>
     </row>
     <row r="175">
       <c r="B175" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="C175" t="s">
         <v>205</v>
@@ -6042,12 +6042,12 @@
         <v>45</v>
       </c>
       <c r="F175" t="s">
-        <v>344</v>
+        <v>236</v>
       </c>
     </row>
     <row r="176">
       <c r="B176" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="C176" t="s">
         <v>205</v>
@@ -6059,63 +6059,63 @@
         <v>45</v>
       </c>
       <c r="F176" t="s">
-        <v>367</v>
+        <v>238</v>
       </c>
     </row>
     <row r="177">
       <c r="B177" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="C177" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D177" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E177" t="s">
         <v>45</v>
       </c>
       <c r="F177" t="s">
-        <v>232</v>
+        <v>75</v>
       </c>
     </row>
     <row r="178">
       <c r="B178" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="C178" t="s">
-        <v>205</v>
+        <v>224</v>
       </c>
       <c r="D178" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E178" t="s">
         <v>45</v>
       </c>
       <c r="F178" t="s">
-        <v>236</v>
+        <v>75</v>
       </c>
     </row>
     <row r="179">
       <c r="B179" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="C179" t="s">
-        <v>205</v>
+        <v>224</v>
       </c>
       <c r="D179" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E179" t="s">
         <v>45</v>
       </c>
       <c r="F179" t="s">
-        <v>238</v>
+        <v>75</v>
       </c>
     </row>
     <row r="180">
       <c r="B180" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="C180" t="s">
         <v>224</v>
@@ -6132,7 +6132,7 @@
     </row>
     <row r="181">
       <c r="B181" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="C181" t="s">
         <v>224</v>
@@ -6149,7 +6149,7 @@
     </row>
     <row r="182">
       <c r="B182" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="C182" t="s">
         <v>224</v>
@@ -6166,7 +6166,7 @@
     </row>
     <row r="183">
       <c r="B183" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="C183" t="s">
         <v>224</v>
@@ -6183,7 +6183,7 @@
     </row>
     <row r="184">
       <c r="B184" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="C184" t="s">
         <v>224</v>
@@ -6200,13 +6200,13 @@
     </row>
     <row r="185">
       <c r="B185" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="C185" t="s">
-        <v>224</v>
+        <v>257</v>
       </c>
       <c r="D185" t="s">
-        <v>44</v>
+        <v>259</v>
       </c>
       <c r="E185" t="s">
         <v>45</v>
@@ -6217,13 +6217,13 @@
     </row>
     <row r="186">
       <c r="B186" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="C186" t="s">
-        <v>224</v>
+        <v>257</v>
       </c>
       <c r="D186" t="s">
-        <v>44</v>
+        <v>259</v>
       </c>
       <c r="E186" t="s">
         <v>45</v>
@@ -6234,13 +6234,13 @@
     </row>
     <row r="187">
       <c r="B187" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="C187" t="s">
-        <v>224</v>
+        <v>257</v>
       </c>
       <c r="D187" t="s">
-        <v>44</v>
+        <v>259</v>
       </c>
       <c r="E187" t="s">
         <v>45</v>
@@ -6251,7 +6251,7 @@
     </row>
     <row r="188">
       <c r="B188" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="C188" t="s">
         <v>257</v>
@@ -6268,7 +6268,7 @@
     </row>
     <row r="189">
       <c r="B189" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="C189" t="s">
         <v>257</v>
@@ -6285,7 +6285,7 @@
     </row>
     <row r="190">
       <c r="B190" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="C190" t="s">
         <v>257</v>
@@ -6302,7 +6302,7 @@
     </row>
     <row r="191">
       <c r="B191" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="C191" t="s">
         <v>257</v>
@@ -6319,7 +6319,7 @@
     </row>
     <row r="192">
       <c r="B192" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="C192" t="s">
         <v>257</v>
@@ -6336,7 +6336,7 @@
     </row>
     <row r="193">
       <c r="B193" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="C193" t="s">
         <v>257</v>
@@ -6353,7 +6353,7 @@
     </row>
     <row r="194">
       <c r="B194" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="C194" t="s">
         <v>257</v>
@@ -6370,7 +6370,7 @@
     </row>
     <row r="195">
       <c r="B195" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="C195" t="s">
         <v>257</v>
@@ -6387,7 +6387,7 @@
     </row>
     <row r="196">
       <c r="B196" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="C196" t="s">
         <v>257</v>
@@ -6404,7 +6404,7 @@
     </row>
     <row r="197">
       <c r="B197" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="C197" t="s">
         <v>257</v>
@@ -6421,7 +6421,7 @@
     </row>
     <row r="198">
       <c r="B198" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="C198" t="s">
         <v>257</v>
@@ -6438,7 +6438,7 @@
     </row>
     <row r="199">
       <c r="B199" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="C199" t="s">
         <v>257</v>
@@ -6455,7 +6455,7 @@
     </row>
     <row r="200">
       <c r="B200" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="C200" t="s">
         <v>257</v>
@@ -6472,13 +6472,13 @@
     </row>
     <row r="201">
       <c r="B201" t="s">
-        <v>392</v>
+        <v>402</v>
       </c>
       <c r="C201" t="s">
-        <v>257</v>
+        <v>224</v>
       </c>
       <c r="D201" t="s">
-        <v>259</v>
+        <v>44</v>
       </c>
       <c r="E201" t="s">
         <v>45</v>
@@ -6489,13 +6489,13 @@
     </row>
     <row r="202">
       <c r="B202" t="s">
-        <v>393</v>
+        <v>404</v>
       </c>
       <c r="C202" t="s">
-        <v>257</v>
+        <v>224</v>
       </c>
       <c r="D202" t="s">
-        <v>259</v>
+        <v>44</v>
       </c>
       <c r="E202" t="s">
         <v>45</v>
@@ -6506,13 +6506,13 @@
     </row>
     <row r="203">
       <c r="B203" t="s">
-        <v>394</v>
+        <v>405</v>
       </c>
       <c r="C203" t="s">
-        <v>257</v>
+        <v>224</v>
       </c>
       <c r="D203" t="s">
-        <v>259</v>
+        <v>44</v>
       </c>
       <c r="E203" t="s">
         <v>45</v>
@@ -6523,7 +6523,7 @@
     </row>
     <row r="204">
       <c r="B204" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="C204" t="s">
         <v>224</v>
@@ -6540,7 +6540,7 @@
     </row>
     <row r="205">
       <c r="B205" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="C205" t="s">
         <v>224</v>
@@ -6557,7 +6557,7 @@
     </row>
     <row r="206">
       <c r="B206" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="C206" t="s">
         <v>224</v>
@@ -6574,7 +6574,7 @@
     </row>
     <row r="207">
       <c r="B207" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="C207" t="s">
         <v>224</v>
@@ -6591,7 +6591,7 @@
     </row>
     <row r="208">
       <c r="B208" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="C208" t="s">
         <v>224</v>
@@ -6608,7 +6608,7 @@
     </row>
     <row r="209">
       <c r="B209" t="s">
-        <v>408</v>
+        <v>420</v>
       </c>
       <c r="C209" t="s">
         <v>224</v>
@@ -6625,7 +6625,7 @@
     </row>
     <row r="210">
       <c r="B210" t="s">
-        <v>409</v>
+        <v>422</v>
       </c>
       <c r="C210" t="s">
         <v>224</v>
@@ -6642,7 +6642,7 @@
     </row>
     <row r="211">
       <c r="B211" t="s">
-        <v>410</v>
+        <v>423</v>
       </c>
       <c r="C211" t="s">
         <v>224</v>
@@ -6659,7 +6659,7 @@
     </row>
     <row r="212">
       <c r="B212" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="C212" t="s">
         <v>224</v>
@@ -6676,7 +6676,7 @@
     </row>
     <row r="213">
       <c r="B213" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="C213" t="s">
         <v>224</v>
@@ -6693,7 +6693,7 @@
     </row>
     <row r="214">
       <c r="B214" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="C214" t="s">
         <v>224</v>
@@ -6710,7 +6710,7 @@
     </row>
     <row r="215">
       <c r="B215" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="C215" t="s">
         <v>224</v>
@@ -6727,7 +6727,7 @@
     </row>
     <row r="216">
       <c r="B216" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="C216" t="s">
         <v>224</v>
@@ -6744,10 +6744,10 @@
     </row>
     <row r="217">
       <c r="B217" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="C217" t="s">
-        <v>224</v>
+        <v>38</v>
       </c>
       <c r="D217" t="s">
         <v>44</v>
@@ -6756,15 +6756,15 @@
         <v>45</v>
       </c>
       <c r="F217" t="s">
-        <v>75</v>
+        <v>153</v>
       </c>
     </row>
     <row r="218">
       <c r="B218" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="C218" t="s">
-        <v>224</v>
+        <v>38</v>
       </c>
       <c r="D218" t="s">
         <v>44</v>
@@ -6773,114 +6773,114 @@
         <v>45</v>
       </c>
       <c r="F218" t="s">
-        <v>75</v>
+        <v>153</v>
       </c>
     </row>
     <row r="219">
       <c r="B219" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="C219" t="s">
-        <v>224</v>
+        <v>40</v>
       </c>
       <c r="D219" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E219" t="s">
         <v>45</v>
       </c>
       <c r="F219" t="s">
-        <v>75</v>
+        <v>452</v>
       </c>
     </row>
     <row r="220">
       <c r="B220" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="C220" t="s">
         <v>38</v>
       </c>
       <c r="D220" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E220" t="s">
         <v>45</v>
       </c>
       <c r="F220" t="s">
-        <v>153</v>
+        <v>453</v>
       </c>
     </row>
     <row r="221">
       <c r="B221" t="s">
-        <v>431</v>
+        <v>445</v>
       </c>
       <c r="C221" t="s">
-        <v>38</v>
+        <v>205</v>
       </c>
       <c r="D221" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E221" t="s">
         <v>45</v>
       </c>
       <c r="F221" t="s">
-        <v>153</v>
+        <v>463</v>
       </c>
     </row>
     <row r="222">
       <c r="B222" t="s">
-        <v>432</v>
+        <v>446</v>
       </c>
       <c r="C222" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D222" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E222" t="s">
         <v>45</v>
       </c>
       <c r="F222" t="s">
-        <v>452</v>
+        <v>464</v>
       </c>
     </row>
     <row r="223">
       <c r="B223" t="s">
-        <v>433</v>
+        <v>447</v>
       </c>
       <c r="C223" t="s">
         <v>38</v>
       </c>
       <c r="D223" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E223" t="s">
         <v>45</v>
       </c>
       <c r="F223" t="s">
-        <v>453</v>
+        <v>465</v>
       </c>
     </row>
     <row r="224">
       <c r="B224" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="C224" t="s">
-        <v>205</v>
+        <v>38</v>
       </c>
       <c r="D224" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E224" t="s">
         <v>45</v>
       </c>
       <c r="F224" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
     </row>
     <row r="225">
       <c r="B225" t="s">
-        <v>446</v>
+        <v>467</v>
       </c>
       <c r="C225" t="s">
         <v>38</v>
@@ -6892,12 +6892,12 @@
         <v>45</v>
       </c>
       <c r="F225" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
     </row>
     <row r="226">
       <c r="B226" t="s">
-        <v>447</v>
+        <v>469</v>
       </c>
       <c r="C226" t="s">
         <v>38</v>
@@ -6909,12 +6909,12 @@
         <v>45</v>
       </c>
       <c r="F226" t="s">
-        <v>465</v>
+        <v>470</v>
       </c>
     </row>
     <row r="227">
       <c r="B227" t="s">
-        <v>448</v>
+        <v>471</v>
       </c>
       <c r="C227" t="s">
         <v>38</v>
@@ -6926,12 +6926,12 @@
         <v>45</v>
       </c>
       <c r="F227" t="s">
-        <v>466</v>
+        <v>472</v>
       </c>
     </row>
     <row r="228">
       <c r="B228" t="s">
-        <v>467</v>
+        <v>473</v>
       </c>
       <c r="C228" t="s">
         <v>38</v>
@@ -6943,63 +6943,63 @@
         <v>45</v>
       </c>
       <c r="F228" t="s">
-        <v>468</v>
+        <v>474</v>
       </c>
     </row>
     <row r="229">
       <c r="B229" t="s">
-        <v>469</v>
+        <v>475</v>
       </c>
       <c r="C229" t="s">
-        <v>38</v>
+        <v>205</v>
       </c>
       <c r="D229" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E229" t="s">
         <v>45</v>
       </c>
       <c r="F229" t="s">
-        <v>470</v>
+        <v>479</v>
       </c>
     </row>
     <row r="230">
       <c r="B230" t="s">
-        <v>471</v>
+        <v>477</v>
       </c>
       <c r="C230" t="s">
-        <v>38</v>
+        <v>224</v>
       </c>
       <c r="D230" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E230" t="s">
         <v>45</v>
       </c>
       <c r="F230" t="s">
-        <v>472</v>
+        <v>455</v>
       </c>
     </row>
     <row r="231">
       <c r="B231" t="s">
-        <v>473</v>
+        <v>478</v>
       </c>
       <c r="C231" t="s">
-        <v>38</v>
+        <v>224</v>
       </c>
       <c r="D231" t="s">
-        <v>44</v>
+        <v>259</v>
       </c>
       <c r="E231" t="s">
         <v>45</v>
       </c>
       <c r="F231" t="s">
-        <v>474</v>
+        <v>455</v>
       </c>
     </row>
     <row r="232">
       <c r="B232" t="s">
-        <v>475</v>
+        <v>480</v>
       </c>
       <c r="C232" t="s">
         <v>205</v>
@@ -7011,63 +7011,63 @@
         <v>45</v>
       </c>
       <c r="F232" t="s">
-        <v>479</v>
+        <v>463</v>
       </c>
     </row>
     <row r="233">
       <c r="B233" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="C233" t="s">
-        <v>224</v>
+        <v>38</v>
       </c>
       <c r="D233" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E233" t="s">
         <v>45</v>
       </c>
       <c r="F233" t="s">
-        <v>455</v>
+        <v>482</v>
       </c>
     </row>
     <row r="234">
       <c r="B234" t="s">
-        <v>478</v>
+        <v>483</v>
       </c>
       <c r="C234" t="s">
-        <v>224</v>
+        <v>38</v>
       </c>
       <c r="D234" t="s">
-        <v>259</v>
+        <v>44</v>
       </c>
       <c r="E234" t="s">
         <v>45</v>
       </c>
       <c r="F234" t="s">
-        <v>455</v>
+        <v>484</v>
       </c>
     </row>
     <row r="235">
       <c r="B235" t="s">
-        <v>480</v>
+        <v>485</v>
       </c>
       <c r="C235" t="s">
-        <v>205</v>
+        <v>38</v>
       </c>
       <c r="D235" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E235" t="s">
         <v>45</v>
       </c>
       <c r="F235" t="s">
-        <v>463</v>
+        <v>486</v>
       </c>
     </row>
     <row r="236">
       <c r="B236" t="s">
-        <v>481</v>
+        <v>487</v>
       </c>
       <c r="C236" t="s">
         <v>38</v>
@@ -7079,12 +7079,12 @@
         <v>45</v>
       </c>
       <c r="F236" t="s">
-        <v>482</v>
+        <v>488</v>
       </c>
     </row>
     <row r="237">
       <c r="B237" t="s">
-        <v>483</v>
+        <v>489</v>
       </c>
       <c r="C237" t="s">
         <v>38</v>
@@ -7096,12 +7096,12 @@
         <v>45</v>
       </c>
       <c r="F237" t="s">
-        <v>484</v>
+        <v>490</v>
       </c>
     </row>
     <row r="238">
       <c r="B238" t="s">
-        <v>485</v>
+        <v>491</v>
       </c>
       <c r="C238" t="s">
         <v>38</v>
@@ -7113,12 +7113,12 @@
         <v>45</v>
       </c>
       <c r="F238" t="s">
-        <v>486</v>
+        <v>492</v>
       </c>
     </row>
     <row r="239">
       <c r="B239" t="s">
-        <v>487</v>
+        <v>493</v>
       </c>
       <c r="C239" t="s">
         <v>38</v>
@@ -7130,12 +7130,12 @@
         <v>45</v>
       </c>
       <c r="F239" t="s">
-        <v>488</v>
+        <v>494</v>
       </c>
     </row>
     <row r="240">
       <c r="B240" t="s">
-        <v>489</v>
+        <v>495</v>
       </c>
       <c r="C240" t="s">
         <v>38</v>
@@ -7147,111 +7147,63 @@
         <v>45</v>
       </c>
       <c r="F240" t="s">
-        <v>490</v>
+        <v>496</v>
       </c>
     </row>
     <row r="241">
       <c r="B241" t="s">
-        <v>491</v>
+        <v>497</v>
       </c>
       <c r="C241" t="s">
-        <v>38</v>
+        <v>205</v>
       </c>
       <c r="D241" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E241" t="s">
         <v>45</v>
       </c>
       <c r="F241" t="s">
-        <v>492</v>
+        <v>498</v>
       </c>
     </row>
     <row r="242">
       <c r="B242" t="s">
-        <v>493</v>
+        <v>499</v>
       </c>
       <c r="C242" t="s">
-        <v>38</v>
+        <v>224</v>
       </c>
       <c r="D242" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="E242" t="s">
         <v>45</v>
       </c>
       <c r="F242" t="s">
-        <v>494</v>
+        <v>455</v>
       </c>
     </row>
     <row r="243">
       <c r="B243" t="s">
-        <v>495</v>
+        <v>500</v>
       </c>
       <c r="C243" t="s">
-        <v>38</v>
+        <v>224</v>
       </c>
       <c r="D243" t="s">
-        <v>44</v>
+        <v>259</v>
       </c>
       <c r="E243" t="s">
         <v>45</v>
       </c>
       <c r="F243" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="244">
-      <c r="B244" t="s">
-        <v>497</v>
-      </c>
-      <c r="C244" t="s">
-        <v>205</v>
-      </c>
-      <c r="D244" t="s">
-        <v>50</v>
-      </c>
-      <c r="E244" t="s">
-        <v>45</v>
-      </c>
-      <c r="F244" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="245">
-      <c r="B245" t="s">
-        <v>499</v>
-      </c>
-      <c r="C245" t="s">
-        <v>224</v>
-      </c>
-      <c r="D245" t="s">
-        <v>50</v>
-      </c>
-      <c r="E245" t="s">
-        <v>45</v>
-      </c>
-      <c r="F245" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="246">
-      <c r="B246" t="s">
-        <v>500</v>
-      </c>
-      <c r="C246" t="s">
-        <v>224</v>
-      </c>
-      <c r="D246" t="s">
-        <v>259</v>
-      </c>
-      <c r="E246" t="s">
-        <v>45</v>
-      </c>
-      <c r="F246" t="s">
-        <v>455</v>
-      </c>
-    </row>
+    <row r="244"/>
+    <row r="245"/>
+    <row r="246"/>
     <row r="247"/>
     <row r="248"/>
     <row r="249"/>

</xml_diff>

<commit_message>
Added displaying value in calibration.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87850" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89370" uniqueCount="504">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1537,6 +1537,15 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId308</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId309</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId310</t>
   </si>
 </sst>
 </file>
@@ -7201,8 +7210,40 @@
         <v>455</v>
       </c>
     </row>
-    <row r="244"/>
-    <row r="245"/>
+    <row r="244">
+      <c r="B244" t="s">
+        <v>501</v>
+      </c>
+      <c r="C244" t="s">
+        <v>73</v>
+      </c>
+      <c r="D244" t="s">
+        <v>44</v>
+      </c>
+      <c r="E244" t="s">
+        <v>45</v>
+      </c>
+      <c r="F244" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="B245" t="s">
+        <v>503</v>
+      </c>
+      <c r="C245" t="s">
+        <v>73</v>
+      </c>
+      <c r="D245" t="s">
+        <v>50</v>
+      </c>
+      <c r="E245" t="s">
+        <v>45</v>
+      </c>
+      <c r="F245" t="s">
+        <v>102</v>
+      </c>
+    </row>
     <row r="246"/>
     <row r="247"/>
     <row r="248"/>

</xml_diff>

<commit_message>
Display unit in time graph.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89370" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97000" uniqueCount="509">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1546,6 +1546,21 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId310</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId311</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stamps number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId312</t>
   </si>
 </sst>
 </file>
@@ -7244,8 +7259,40 @@
         <v>102</v>
       </c>
     </row>
-    <row r="246"/>
-    <row r="247"/>
+    <row r="246">
+      <c r="B246" t="s">
+        <v>504</v>
+      </c>
+      <c r="C246" t="s">
+        <v>224</v>
+      </c>
+      <c r="D246" t="s">
+        <v>44</v>
+      </c>
+      <c r="E246" t="s">
+        <v>45</v>
+      </c>
+      <c r="F246" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="B247" t="s">
+        <v>508</v>
+      </c>
+      <c r="C247" t="s">
+        <v>224</v>
+      </c>
+      <c r="D247" t="s">
+        <v>44</v>
+      </c>
+      <c r="E247" t="s">
+        <v>45</v>
+      </c>
+      <c r="F247" t="s">
+        <v>75</v>
+      </c>
+    </row>
     <row r="248"/>
     <row r="249"/>
     <row r="250"/>

</xml_diff>

<commit_message>
Added label for frequency graph.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97000" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98544" uniqueCount="511">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1561,6 +1561,12 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId312</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId313</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId314</t>
   </si>
 </sst>
 </file>
@@ -7293,8 +7299,40 @@
         <v>75</v>
       </c>
     </row>
-    <row r="248"/>
-    <row r="249"/>
+    <row r="248">
+      <c r="B248" t="s">
+        <v>509</v>
+      </c>
+      <c r="C248" t="s">
+        <v>224</v>
+      </c>
+      <c r="D248" t="s">
+        <v>44</v>
+      </c>
+      <c r="E248" t="s">
+        <v>45</v>
+      </c>
+      <c r="F248" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="B249" t="s">
+        <v>510</v>
+      </c>
+      <c r="C249" t="s">
+        <v>224</v>
+      </c>
+      <c r="D249" t="s">
+        <v>44</v>
+      </c>
+      <c r="E249" t="s">
+        <v>45</v>
+      </c>
+      <c r="F249" t="s">
+        <v>75</v>
+      </c>
+    </row>
     <row r="250"/>
     <row r="251"/>
     <row r="252"/>

</xml_diff>

<commit_message>
Added info in about screen.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104822" uniqueCount="522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106414" uniqueCount="526">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1600,6 +1600,20 @@
   </si>
   <si>
     <t xml:space="preserve">ABOUT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId321</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Author:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId322</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kacper Janowski
+WEL18EC1S1
+Nr. albumu: 71980</t>
   </si>
 </sst>
 </file>
@@ -7468,8 +7482,40 @@
         <v>521</v>
       </c>
     </row>
-    <row r="256"/>
-    <row r="257"/>
+    <row r="256">
+      <c r="B256" t="s">
+        <v>522</v>
+      </c>
+      <c r="C256" t="s">
+        <v>205</v>
+      </c>
+      <c r="D256" t="s">
+        <v>50</v>
+      </c>
+      <c r="E256" t="s">
+        <v>45</v>
+      </c>
+      <c r="F256" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="B257" t="s">
+        <v>524</v>
+      </c>
+      <c r="C257" t="s">
+        <v>38</v>
+      </c>
+      <c r="D257" t="s">
+        <v>50</v>
+      </c>
+      <c r="E257" t="s">
+        <v>45</v>
+      </c>
+      <c r="F257" t="s">
+        <v>525</v>
+      </c>
+    </row>
     <row r="258"/>
     <row r="259"/>
     <row r="260"/>

</xml_diff>

<commit_message>
Fixed displaying number of graphs.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112852" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114469" uniqueCount="534">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -3183,13 +3183,13 @@
         <v>17</v>
       </c>
       <c r="G13" t="s">
-        <v>42</v>
+        <v>288</v>
       </c>
       <c r="H13" t="s">
         <v>42</v>
       </c>
       <c r="I13" t="s">
-        <v>42</v>
+        <v>122</v>
       </c>
       <c r="J13" t="s">
         <v>42</v>

</xml_diff>

<commit_message>
Fixed scroll wheel in freq panel configure.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114469" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116086" uniqueCount="535">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1641,6 +1641,9 @@
   <si>
     <t xml:space="preserve">TIME INTERVAL/MODE: 
 INDEPENDENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freq </t>
   </si>
 </sst>
 </file>
@@ -6005,7 +6008,7 @@
         <v>45</v>
       </c>
       <c r="F165" t="s">
-        <v>352</v>
+        <v>534</v>
       </c>
     </row>
     <row r="166">
@@ -6022,7 +6025,7 @@
         <v>45</v>
       </c>
       <c r="F166" t="s">
-        <v>354</v>
+        <v>534</v>
       </c>
     </row>
     <row r="167">
@@ -6039,7 +6042,7 @@
         <v>45</v>
       </c>
       <c r="F167" t="s">
-        <v>356</v>
+        <v>534</v>
       </c>
     </row>
     <row r="168">
@@ -6056,7 +6059,7 @@
         <v>45</v>
       </c>
       <c r="F168" t="s">
-        <v>358</v>
+        <v>534</v>
       </c>
     </row>
     <row r="169">
@@ -6073,7 +6076,7 @@
         <v>45</v>
       </c>
       <c r="F169" t="s">
-        <v>360</v>
+        <v>534</v>
       </c>
     </row>
     <row r="170">
@@ -6090,7 +6093,7 @@
         <v>45</v>
       </c>
       <c r="F170" t="s">
-        <v>362</v>
+        <v>534</v>
       </c>
     </row>
     <row r="171">
@@ -6107,7 +6110,7 @@
         <v>45</v>
       </c>
       <c r="F171" t="s">
-        <v>364</v>
+        <v>534</v>
       </c>
     </row>
     <row r="172">
@@ -6141,7 +6144,7 @@
         <v>45</v>
       </c>
       <c r="F173" t="s">
-        <v>367</v>
+        <v>534</v>
       </c>
     </row>
     <row r="174">

</xml_diff>

<commit_message>
Added new structure for all data.
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116086" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117703" uniqueCount="536">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1644,6 +1644,11 @@
   </si>
   <si>
     <t xml:space="preserve">Freq </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kacper Janowski
+WEL18EC1S1
+Student ID number: 71980</t>
   </si>
 </sst>
 </file>
@@ -7572,7 +7577,7 @@
         <v>45</v>
       </c>
       <c r="F257" t="s">
-        <v>527</v>
+        <v>535</v>
       </c>
     </row>
     <row r="258">

</xml_diff>